<commit_message>
Se agregaron algunos de los requisitos
</commit_message>
<xml_diff>
--- a/Excel-Burndown-Chart-Template.xlsx
+++ b/Excel-Burndown-Chart-Template.xlsx
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="172">
   <si>
     <t>Start Date</t>
   </si>
@@ -225,9 +225,6 @@
     <t>Agregar un proveedor</t>
   </si>
   <si>
-    <t>agregar un proveedor a la base de datos</t>
-  </si>
-  <si>
     <t>Agregar productos</t>
   </si>
   <si>
@@ -411,12 +408,6 @@
     <t>No iniciado</t>
   </si>
   <si>
-    <t>Aceptado</t>
-  </si>
-  <si>
-    <t>Falta verdificar por el usuario</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -552,10 +543,49 @@
     <t>Cajero</t>
   </si>
   <si>
-    <t>Agregar datos del cliente</t>
-  </si>
-  <si>
     <t>agregar datos generales del cliente</t>
+  </si>
+  <si>
+    <t>Propietario</t>
+  </si>
+  <si>
+    <t>Registrar datos del cliente</t>
+  </si>
+  <si>
+    <t>Registrar datos del cajero</t>
+  </si>
+  <si>
+    <t>agregar datos generales del cajero</t>
+  </si>
+  <si>
+    <t>Modificar datos del cliente</t>
+  </si>
+  <si>
+    <t>Control de caja</t>
+  </si>
+  <si>
+    <t>registrar las ventas realizadas y realizar el arqueo de caja</t>
+  </si>
+  <si>
+    <t>Modificar datos del cajero</t>
+  </si>
+  <si>
+    <t>Eliminar datos del cajero</t>
+  </si>
+  <si>
+    <t>actualizar datos del cajero</t>
+  </si>
+  <si>
+    <t>eliminar datos del cajero</t>
+  </si>
+  <si>
+    <t>actualizar datos del cliente</t>
+  </si>
+  <si>
+    <t>Impresión de facturas</t>
+  </si>
+  <si>
+    <t>Imprimir la información correspondiente a la venta</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1045,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1056,7 +1086,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1110,13 +1139,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1728,7 +1757,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2181,11 +2209,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="232676928"/>
-        <c:axId val="232677320"/>
+        <c:axId val="234865192"/>
+        <c:axId val="234865584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="232676928"/>
+        <c:axId val="234865192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2228,7 +2256,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="232677320"/>
+        <c:crossAx val="234865584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2236,7 +2264,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="232677320"/>
+        <c:axId val="234865584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2287,7 +2315,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="232676928"/>
+        <c:crossAx val="234865192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2301,7 +2329,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3261,7 +3288,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3272,342 +3299,341 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="38" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="C2" s="35" t="s">
+      <c r="A2" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="34" t="s">
         <v>159</v>
-      </c>
-      <c r="D2" s="35" t="s">
-        <v>160</v>
       </c>
       <c r="E2" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="F2" s="24" t="e">
-        <f>-C3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G2" s="36" t="s">
+      <c r="F2" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3" s="25" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="G3" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="G3" s="27" t="s">
+      <c r="B6" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H6" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="F7" s="25" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="G4" s="27" t="s">
+      <c r="G7" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H7" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="F8" s="25" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" s="27" t="s">
+      <c r="G8" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="H8" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="B6" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
-        <v>152</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>146</v>
+      <c r="B9" s="33" t="s">
+        <v>143</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="F9" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="G9" s="27" t="s">
+      <c r="E10" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>113</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>112</v>
+      <c r="H10" s="30" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>146</v>
+      <c r="A11" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>143</v>
       </c>
       <c r="C11" s="23" t="s">
         <v>45</v>
       </c>
       <c r="D11" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="F11" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>114</v>
-      </c>
-      <c r="G11" s="27" t="s">
+      <c r="E12" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G12" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="31" t="s">
+      <c r="H12" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="25" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="G12" s="28" t="s">
+      <c r="G13" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="G13" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="32" t="s">
-        <v>112</v>
+      <c r="H13" s="31" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -3637,16 +3663,16 @@
         <v>38</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>10</v>
@@ -3679,71 +3705,71 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="42" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="42" t="s">
+      <c r="H3" s="42"/>
+      <c r="I3" s="43" t="s">
         <v>77</v>
-      </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="44" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="45" t="s">
-        <v>118</v>
+      <c r="B4" s="44" t="s">
+        <v>115</v>
       </c>
       <c r="C4" s="62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D4" s="63"/>
       <c r="E4" s="63"/>
       <c r="F4" s="63"/>
-      <c r="G4" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="47">
+      <c r="G4" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="45"/>
+      <c r="I4" s="46">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
-      <c r="B5" s="48" t="s">
-        <v>145</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="H5" s="49"/>
-      <c r="I5" s="50">
+      <c r="B5" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="48"/>
+      <c r="I5" s="49">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
       <c r="G6" s="18"/>
-      <c r="H6" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="I6" s="59">
+      <c r="H6" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" s="58">
         <f>SUM(I4:I5)</f>
         <v>10</v>
       </c>
@@ -3760,16 +3786,16 @@
         <v>38</v>
       </c>
       <c r="E7" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>10</v>
@@ -3784,13 +3810,13 @@
         <v>44</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>50</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20" t="s">
@@ -3804,88 +3830,88 @@
       <c r="A9" s="19"/>
       <c r="B9" s="18"/>
       <c r="C9" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
-      <c r="B10" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" s="65" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="H10" s="43"/>
-      <c r="I10" s="51">
+      <c r="B10" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="H10" s="42"/>
+      <c r="I10" s="50">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
-      <c r="B11" s="45" t="s">
-        <v>120</v>
+      <c r="B11" s="44" t="s">
+        <v>117</v>
       </c>
       <c r="C11" s="62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="63"/>
       <c r="E11" s="63"/>
       <c r="F11" s="63"/>
-      <c r="G11" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="H11" s="46"/>
-      <c r="I11" s="47">
+      <c r="G11" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" s="45"/>
+      <c r="I11" s="46">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
-      <c r="B12" s="48" t="s">
-        <v>143</v>
-      </c>
-      <c r="C12" s="60" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="H12" s="49"/>
-      <c r="I12" s="52">
+      <c r="B12" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="64" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="H12" s="48"/>
+      <c r="I12" s="51">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
       <c r="G13" s="18"/>
-      <c r="H13" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="I13" s="59">
+      <c r="H13" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="I13" s="58">
         <f>SUM(I10:I12)</f>
         <v>20</v>
       </c>
@@ -3902,16 +3928,16 @@
         <v>38</v>
       </c>
       <c r="E14" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>10</v>
@@ -3929,10 +3955,10 @@
         <v>45</v>
       </c>
       <c r="E15" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>52</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>53</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="20" t="s">
@@ -3946,73 +3972,73 @@
       <c r="A16" s="19"/>
       <c r="B16" s="18"/>
       <c r="C16" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
-      <c r="B17" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="C17" s="65" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="66"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="H17" s="43"/>
-      <c r="I17" s="51">
+      <c r="B17" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="H17" s="42"/>
+      <c r="I17" s="50">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
-      <c r="B18" s="45" t="s">
-        <v>123</v>
+      <c r="B18" s="44" t="s">
+        <v>120</v>
       </c>
       <c r="C18" s="62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="63"/>
       <c r="E18" s="63"/>
       <c r="F18" s="63"/>
-      <c r="G18" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="H18" s="46"/>
-      <c r="I18" s="47">
+      <c r="G18" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" s="45"/>
+      <c r="I18" s="46">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
-      <c r="B19" s="48" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="60" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="H19" s="49"/>
-      <c r="I19" s="50">
+      <c r="B19" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="64" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="H19" s="48"/>
+      <c r="I19" s="49">
         <v>2</v>
       </c>
     </row>
@@ -4024,10 +4050,10 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
-      <c r="H20" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="I20" s="59">
+      <c r="H20" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="I20" s="58">
         <f>SUM(I17:I19)</f>
         <v>10</v>
       </c>
@@ -4044,16 +4070,16 @@
         <v>38</v>
       </c>
       <c r="E21" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I21" s="17" t="s">
         <v>10</v>
@@ -4071,10 +4097,10 @@
         <v>45</v>
       </c>
       <c r="E22" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="20" t="s">
         <v>54</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>55</v>
       </c>
       <c r="G22" s="21"/>
       <c r="H22" s="20" t="s">
@@ -4088,69 +4114,69 @@
       <c r="A23" s="19"/>
       <c r="B23" s="18"/>
       <c r="C23" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
-      <c r="B24" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="C24" s="65" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="H24" s="43"/>
-      <c r="I24" s="51">
+      <c r="B24" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="42"/>
+      <c r="I24" s="50">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
-      <c r="B25" s="48" t="s">
-        <v>125</v>
-      </c>
-      <c r="C25" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="H25" s="49"/>
-      <c r="I25" s="50">
+      <c r="B25" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="64" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="H25" s="48"/>
+      <c r="I25" s="49">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
       <c r="G26" s="18"/>
-      <c r="H26" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="I26" s="59">
+      <c r="H26" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="I26" s="58">
         <f>SUM(I24:I25)</f>
         <v>10</v>
       </c>
@@ -4167,16 +4193,16 @@
         <v>38</v>
       </c>
       <c r="E27" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I27" s="17" t="s">
         <v>10</v>
@@ -4194,10 +4220,10 @@
         <v>45</v>
       </c>
       <c r="E28" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="20" t="s">
         <v>56</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>57</v>
       </c>
       <c r="G28" s="21"/>
       <c r="H28" s="20" t="s">
@@ -4222,54 +4248,54 @@
       <c r="A30" s="19"/>
       <c r="B30" s="18"/>
       <c r="C30" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H30" s="18"/>
       <c r="I30" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
-      <c r="B31" s="41" t="s">
-        <v>126</v>
-      </c>
-      <c r="C31" s="65" t="s">
-        <v>90</v>
-      </c>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="H31" s="43"/>
-      <c r="I31" s="51">
+      <c r="B31" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="H31" s="42"/>
+      <c r="I31" s="50">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
-      <c r="B32" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="C32" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="H32" s="49"/>
-      <c r="I32" s="50">
+      <c r="B32" s="47" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="48"/>
+      <c r="I32" s="49">
         <v>5</v>
       </c>
     </row>
@@ -4281,10 +4307,10 @@
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
       <c r="G33" s="18"/>
-      <c r="H33" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="I33" s="59">
+      <c r="H33" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="I33" s="58">
         <f>SUM(I31:I32)</f>
         <v>10</v>
       </c>
@@ -4301,16 +4327,16 @@
         <v>38</v>
       </c>
       <c r="E34" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I34" s="17" t="s">
         <v>10</v>
@@ -4328,10 +4354,10 @@
         <v>45</v>
       </c>
       <c r="E35" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="20" t="s">
         <v>58</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>59</v>
       </c>
       <c r="G35" s="21"/>
       <c r="H35" s="20" t="s">
@@ -4345,69 +4371,69 @@
       <c r="A36" s="19"/>
       <c r="B36" s="18"/>
       <c r="C36" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H36" s="18"/>
       <c r="I36" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
-      <c r="B37" s="41" t="s">
-        <v>128</v>
-      </c>
-      <c r="C37" s="65" t="s">
-        <v>90</v>
-      </c>
-      <c r="D37" s="66"/>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
-      <c r="G37" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="H37" s="43"/>
-      <c r="I37" s="51">
+      <c r="B37" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="61"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="H37" s="42"/>
+      <c r="I37" s="50">
         <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19"/>
-      <c r="B38" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="C38" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="D38" s="61"/>
-      <c r="E38" s="61"/>
-      <c r="F38" s="61"/>
-      <c r="G38" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="H38" s="49"/>
-      <c r="I38" s="50">
+      <c r="B38" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="H38" s="48"/>
+      <c r="I38" s="49">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
       <c r="B39" s="18"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="64"/>
-      <c r="E39" s="64"/>
-      <c r="F39" s="64"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="59"/>
+      <c r="F39" s="59"/>
       <c r="G39" s="18"/>
-      <c r="H39" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="I39" s="59">
+      <c r="H39" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="I39" s="58">
         <f>SUM(I37:I38)</f>
         <v>10</v>
       </c>
@@ -4424,16 +4450,16 @@
         <v>38</v>
       </c>
       <c r="E40" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="G40" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I40" s="17" t="s">
         <v>10</v>
@@ -4448,13 +4474,13 @@
         <v>44</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E41" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F41" s="20" t="s">
         <v>60</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>61</v>
       </c>
       <c r="G41" s="21"/>
       <c r="H41" s="20" t="s">
@@ -4468,73 +4494,73 @@
       <c r="A42" s="19"/>
       <c r="B42" s="18"/>
       <c r="C42" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H42" s="18"/>
       <c r="I42" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
-      <c r="B43" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="C43" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="D43" s="66"/>
-      <c r="E43" s="66"/>
-      <c r="F43" s="66"/>
-      <c r="G43" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="H43" s="43"/>
-      <c r="I43" s="51">
+      <c r="B43" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="61"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="61"/>
+      <c r="G43" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="H43" s="42"/>
+      <c r="I43" s="50">
         <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
-      <c r="B44" s="45" t="s">
-        <v>131</v>
+      <c r="B44" s="44" t="s">
+        <v>128</v>
       </c>
       <c r="C44" s="62" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D44" s="63"/>
       <c r="E44" s="63"/>
       <c r="F44" s="63"/>
-      <c r="G44" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="H44" s="46"/>
-      <c r="I44" s="47">
+      <c r="G44" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="H44" s="45"/>
+      <c r="I44" s="46">
         <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
-      <c r="B45" s="48" t="s">
-        <v>132</v>
-      </c>
-      <c r="C45" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="D45" s="61"/>
-      <c r="E45" s="61"/>
-      <c r="F45" s="61"/>
-      <c r="G45" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="H45" s="49"/>
-      <c r="I45" s="50">
+      <c r="B45" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="C45" s="64" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" s="65"/>
+      <c r="E45" s="65"/>
+      <c r="F45" s="65"/>
+      <c r="G45" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="H45" s="48"/>
+      <c r="I45" s="49">
         <v>4</v>
       </c>
     </row>
@@ -4546,10 +4572,10 @@
       <c r="E46" s="17"/>
       <c r="F46" s="17"/>
       <c r="G46" s="17"/>
-      <c r="H46" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="I46" s="59">
+      <c r="H46" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="I46" s="58">
         <f>SUM(I43:I45)</f>
         <v>10</v>
       </c>
@@ -4566,16 +4592,16 @@
         <v>38</v>
       </c>
       <c r="E47" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F47" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="G47" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I47" s="17" t="s">
         <v>10</v>
@@ -4593,10 +4619,10 @@
         <v>45</v>
       </c>
       <c r="E48" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F48" s="20" t="s">
         <v>62</v>
-      </c>
-      <c r="F48" s="20" t="s">
-        <v>63</v>
       </c>
       <c r="G48" s="21"/>
       <c r="H48" s="20" t="s">
@@ -4610,81 +4636,81 @@
       <c r="A49" s="19"/>
       <c r="B49" s="18"/>
       <c r="C49" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
       <c r="G49" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H49" s="18"/>
       <c r="I49" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="19"/>
-      <c r="B50" s="41" t="s">
-        <v>133</v>
-      </c>
-      <c r="C50" s="65" t="s">
-        <v>96</v>
-      </c>
-      <c r="D50" s="66"/>
-      <c r="E50" s="66"/>
-      <c r="F50" s="66"/>
-      <c r="G50" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="H50" s="43"/>
-      <c r="I50" s="51">
+      <c r="B50" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="C50" s="60" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" s="61"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="H50" s="42"/>
+      <c r="I50" s="50">
         <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="19"/>
-      <c r="B51" s="45" t="s">
-        <v>134</v>
+      <c r="B51" s="44" t="s">
+        <v>131</v>
       </c>
       <c r="C51" s="62" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D51" s="63"/>
       <c r="E51" s="63"/>
       <c r="F51" s="63"/>
-      <c r="G51" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="H51" s="46"/>
-      <c r="I51" s="47">
+      <c r="G51" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="H51" s="45"/>
+      <c r="I51" s="46">
         <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="19"/>
-      <c r="B52" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="C52" s="60" t="s">
-        <v>98</v>
-      </c>
-      <c r="D52" s="61"/>
-      <c r="E52" s="61"/>
-      <c r="F52" s="61"/>
-      <c r="G52" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="H52" s="49"/>
-      <c r="I52" s="50">
+      <c r="B52" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="D52" s="65"/>
+      <c r="E52" s="65"/>
+      <c r="F52" s="65"/>
+      <c r="G52" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="H52" s="48"/>
+      <c r="I52" s="49">
         <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H53" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="I53" s="59">
+      <c r="H53" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="I53" s="58">
         <f>SUM(I50:I52)</f>
         <v>20</v>
       </c>
@@ -4700,16 +4726,16 @@
         <v>38</v>
       </c>
       <c r="E54" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F54" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="F54" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="G54" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H54" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I54" s="17" t="s">
         <v>10</v>
@@ -4723,13 +4749,13 @@
         <v>44</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E55" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F55" s="20" t="s">
         <v>64</v>
-      </c>
-      <c r="F55" s="20" t="s">
-        <v>65</v>
       </c>
       <c r="G55" s="21"/>
       <c r="H55" s="20" t="s">
@@ -4752,66 +4778,66 @@
     <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="18"/>
       <c r="C57" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
       <c r="F57" s="18"/>
       <c r="G57" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H57" s="18"/>
       <c r="I57" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="41" t="s">
-        <v>136</v>
-      </c>
-      <c r="C58" s="65" t="s">
+      <c r="B58" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="C58" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58" s="61"/>
+      <c r="E58" s="61"/>
+      <c r="F58" s="61"/>
+      <c r="G58" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="H58" s="42"/>
+      <c r="I58" s="50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="D58" s="66"/>
-      <c r="E58" s="66"/>
-      <c r="F58" s="66"/>
-      <c r="G58" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="H58" s="43"/>
-      <c r="I58" s="51">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="48" t="s">
-        <v>144</v>
-      </c>
-      <c r="C59" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="D59" s="49"/>
-      <c r="E59" s="49"/>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="H59" s="49"/>
-      <c r="I59" s="50">
+      <c r="D59" s="48"/>
+      <c r="E59" s="48"/>
+      <c r="F59" s="48"/>
+      <c r="G59" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="H59" s="48"/>
+      <c r="I59" s="49">
         <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="18"/>
-      <c r="C60" s="64"/>
-      <c r="D60" s="64"/>
-      <c r="E60" s="64"/>
-      <c r="F60" s="64"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="59"/>
+      <c r="F60" s="59"/>
       <c r="G60" s="18"/>
-      <c r="H60" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="I60" s="59">
+      <c r="H60" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="I60" s="58">
         <f>SUM(I58:I59)</f>
         <v>20</v>
       </c>
@@ -4827,16 +4853,16 @@
         <v>38</v>
       </c>
       <c r="E61" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F61" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="F61" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="G61" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H61" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I61" s="17" t="s">
         <v>10</v>
@@ -4853,10 +4879,10 @@
         <v>45</v>
       </c>
       <c r="E62" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F62" s="20" t="s">
         <v>66</v>
-      </c>
-      <c r="F62" s="20" t="s">
-        <v>67</v>
       </c>
       <c r="G62" s="21"/>
       <c r="H62" s="20" t="s">
@@ -4869,90 +4895,75 @@
     <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="18"/>
       <c r="C63" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D63" s="18"/>
       <c r="E63" s="18"/>
       <c r="F63" s="18"/>
       <c r="G63" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H63" s="18"/>
       <c r="I63" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="C64" s="65" t="s">
+      <c r="B64" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="C64" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="D64" s="61"/>
+      <c r="E64" s="61"/>
+      <c r="F64" s="61"/>
+      <c r="G64" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="H64" s="42"/>
+      <c r="I64" s="50">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="D64" s="66"/>
-      <c r="E64" s="66"/>
-      <c r="F64" s="66"/>
-      <c r="G64" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="H64" s="43"/>
-      <c r="I64" s="51">
+      <c r="D65" s="48"/>
+      <c r="E65" s="48"/>
+      <c r="F65" s="48"/>
+      <c r="G65" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="H65" s="48"/>
+      <c r="I65" s="49">
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="C65" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="D65" s="49"/>
-      <c r="E65" s="49"/>
-      <c r="F65" s="49"/>
-      <c r="G65" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="H65" s="49"/>
-      <c r="I65" s="50">
-        <v>20</v>
-      </c>
-    </row>
     <row r="66" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H66" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="I66" s="59">
+      <c r="H66" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="I66" s="58">
         <f>SUM(I64:I65)</f>
         <v>40</v>
       </c>
     </row>
     <row r="67" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="H67" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="I67" s="54">
+      <c r="H67" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="I67" s="53">
         <f>I6+I13+I20+I26+I33+I39+I46+I53+I60+I66</f>
         <v>160</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="C64:F64"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="C52:F52"/>
-    <mergeCell ref="C58:F58"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="C45:F45"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C5:F5"/>
@@ -4965,6 +4976,21 @@
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C60:F60"/>
+    <mergeCell ref="C64:F64"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="C52:F52"/>
+    <mergeCell ref="C58:F58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5002,16 +5028,16 @@
         <v>38</v>
       </c>
       <c r="E2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="G2" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I2" s="17" t="s">
         <v>10</v>
@@ -5019,7 +5045,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>44</v>
@@ -5028,10 +5054,10 @@
         <v>45</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G3" s="21"/>
       <c r="H3" s="20" t="s">
@@ -5044,66 +5070,66 @@
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="18"/>
       <c r="C4" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
       <c r="G4" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H4" s="18"/>
       <c r="I4" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" s="65" t="s">
+      <c r="B5" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="42"/>
+      <c r="I5" s="50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="48" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="51">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="48" t="s">
-        <v>140</v>
-      </c>
-      <c r="C6" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="H6" s="49"/>
-      <c r="I6" s="50">
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="48"/>
+      <c r="I6" s="49">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="18"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
       <c r="G7" s="18"/>
-      <c r="H7" s="57" t="s">
-        <v>117</v>
-      </c>
-      <c r="I7" s="58">
+      <c r="H7" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="I7" s="57">
         <f>SUM(I5:I6)</f>
         <v>20</v>
       </c>
@@ -5129,16 +5155,16 @@
         <v>38</v>
       </c>
       <c r="E9" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>73</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>74</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I9" s="17" t="s">
         <v>10</v>
@@ -5146,7 +5172,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>44</v>
@@ -5155,10 +5181,10 @@
         <v>45</v>
       </c>
       <c r="E10" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="20" t="s">
         <v>70</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>71</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="20" t="s">
@@ -5171,69 +5197,69 @@
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="18"/>
       <c r="C11" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="41" t="s">
-        <v>141</v>
-      </c>
-      <c r="C12" s="65" t="s">
+      <c r="B12" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" s="42"/>
+      <c r="I12" s="50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="51">
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="48" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="48"/>
+      <c r="I13" s="49">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="48" t="s">
-        <v>142</v>
-      </c>
-      <c r="C13" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" s="49"/>
-      <c r="I13" s="50">
-        <v>10</v>
-      </c>
-    </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H14" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="I14" s="56">
+      <c r="H14" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="I14" s="55">
         <f>SUM(I12:I13)</f>
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="53" t="s">
-        <v>116</v>
-      </c>
-      <c r="I15" s="53">
+      <c r="H15" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15" s="52">
         <f>I7+I14</f>
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Editado la tabla de sprint1 y sprint2
</commit_message>
<xml_diff>
--- a/Excel-Burndown-Chart-Template.xlsx
+++ b/Excel-Burndown-Chart-Template.xlsx
@@ -1,47 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos de Micha\Tercer Semestre\Proyecto Metodologia\proyectometodologia7342\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Desktop\New folder (2)\ProyectoMetodologia\proyectometodologia7342\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604DB024-E6B2-40F6-9A00-2C6C0A304B69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="4" r:id="rId1"/>
     <sheet name="Sprint1" sheetId="5" r:id="rId2"/>
     <sheet name="Sprint2" sheetId="6" r:id="rId3"/>
     <sheet name="Sprint1Info" sheetId="2" r:id="rId4"/>
-    <sheet name="Backlog1Table" sheetId="1" r:id="rId5"/>
-    <sheet name="BurnDown1Table" sheetId="3" r:id="rId6"/>
+    <sheet name="Sprint2Info" sheetId="7" r:id="rId5"/>
+    <sheet name="Backlog1Table" sheetId="1" r:id="rId6"/>
+    <sheet name="BurnDown1Table" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
+    <definedName name="DevRate" localSheetId="4">Sprint2Info!$B$10</definedName>
     <definedName name="DevRate">Sprint1Info!$B$10</definedName>
+    <definedName name="RemainingHours" localSheetId="4">SprintBacklog[[#Totals],[Remaining Hours]]</definedName>
     <definedName name="RemainingHours">SprintBacklog[[#Totals],[Remaining Hours]]</definedName>
+    <definedName name="StartDate" localSheetId="4">Sprint2Info!$B$2</definedName>
     <definedName name="StartDate">Sprint1Info!$B$2</definedName>
+    <definedName name="TotalHours" localSheetId="4">SprintBacklog[[#Totals],[Estimated Hours]]</definedName>
     <definedName name="TotalHours">SprintBacklog[[#Totals],[Estimated Hours]]</definedName>
+    <definedName name="WorkingDays" localSheetId="4">Sprint2Info!$B$6</definedName>
     <definedName name="WorkingDays">Sprint1Info!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>PowerUps for Excel</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -70,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="180">
   <si>
     <t>Start Date</t>
   </si>
@@ -267,18 +283,9 @@
     <t>visualizar el registro de compras realizadas</t>
   </si>
   <si>
-    <t>Visualizar proveedor</t>
-  </si>
-  <si>
-    <t>visualizar los datos del proveedor asociado a la compra</t>
-  </si>
-  <si>
     <t>Visualizar productos</t>
   </si>
   <si>
-    <t>visualizar los productos que se adquiereron en una compra</t>
-  </si>
-  <si>
     <t>Buscar compra</t>
   </si>
   <si>
@@ -306,99 +313,15 @@
     <t>Estimado</t>
   </si>
   <si>
-    <t>Crear un formulario para el ingreso de los datos de una compra</t>
-  </si>
-  <si>
-    <t>Validación de datos</t>
-  </si>
-  <si>
     <t>Gerente</t>
   </si>
   <si>
     <t>Agregar un proveedor a la base de datos</t>
   </si>
   <si>
-    <t>Crear un formulario para el ingreso de los datos del proveedor</t>
-  </si>
-  <si>
-    <t>Habilitar la Base de Datos para guardar a proveedores</t>
-  </si>
-  <si>
-    <t>Crear un formulario para el ingreso de los datos de la compra</t>
-  </si>
-  <si>
-    <t>Habilitar la Base de Datos para guardar los datos de la compra</t>
-  </si>
-  <si>
-    <t>Crear un formulario para eliminar las compras</t>
-  </si>
-  <si>
-    <t>Crear una sección que permita buscar la compra que se eliminará</t>
-  </si>
-  <si>
-    <t>Diego</t>
-  </si>
-  <si>
-    <t>Crear un formulario para eliminar el proveedor</t>
-  </si>
-  <si>
-    <t>Crear una sección que permita buscar el proveedor que se eliminará</t>
-  </si>
-  <si>
-    <t>Crear una sección que permita buscar los productos a eliminar</t>
-  </si>
-  <si>
-    <t>Crear un formulario para realizar las modificaciones de una compra</t>
-  </si>
-  <si>
-    <t>Crear una sección que permita ingresar el de codigo de la compra y buscarla</t>
-  </si>
-  <si>
-    <t>Actualización de bases de datos</t>
-  </si>
-  <si>
-    <t>Crear un formulario para realizar la modificación de un proveedor</t>
-  </si>
-  <si>
-    <t>Crear una sección que permita ingresar los datos del proveedor</t>
-  </si>
-  <si>
-    <t>Actualización de base de datos</t>
-  </si>
-  <si>
-    <t>Crear un formulario para poder visualizar la compra</t>
-  </si>
-  <si>
-    <t>Habilitar la Base de Datos para buscar la información de la compra</t>
-  </si>
-  <si>
-    <t>Crear un formulario para poder visualizar los datos del proveedor</t>
-  </si>
-  <si>
-    <t>Habilitar la Base de Datos para buscar la información del proveedor</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Pedro</t>
-  </si>
-  <si>
     <t>visualizar los productos que se adquirieron en una compra</t>
   </si>
   <si>
-    <t>Crear un formulario para poder visualizar los datos de los productos</t>
-  </si>
-  <si>
-    <t>Habilitar la Base de Datos para buscar la información de los productos</t>
-  </si>
-  <si>
-    <t>Crear un formulario para poder realizar la busqueda de la compra</t>
-  </si>
-  <si>
-    <t>Crear una sección que permita ingresar el codigo de la compra</t>
-  </si>
-  <si>
     <t>HU11</t>
   </si>
   <si>
@@ -471,15 +394,6 @@
     <t>HU8-3</t>
   </si>
   <si>
-    <t>HU9-1</t>
-  </si>
-  <si>
-    <t>HU10-1</t>
-  </si>
-  <si>
-    <t>HU10-2</t>
-  </si>
-  <si>
     <t>HU11-1</t>
   </si>
   <si>
@@ -495,9 +409,6 @@
     <t>HU2-3</t>
   </si>
   <si>
-    <t>HU9-2</t>
-  </si>
-  <si>
     <t>HU1-2</t>
   </si>
   <si>
@@ -546,9 +457,6 @@
     <t>agregar datos generales del cliente</t>
   </si>
   <si>
-    <t>Propietario</t>
-  </si>
-  <si>
     <t>Registrar datos del cliente</t>
   </si>
   <si>
@@ -586,12 +494,144 @@
   </si>
   <si>
     <t>Imprimir la información correspondiente a la venta</t>
+  </si>
+  <si>
+    <t>VP13</t>
+  </si>
+  <si>
+    <t>a ap</t>
+  </si>
+  <si>
+    <t>visualizar los productos que se desean comprar</t>
+  </si>
+  <si>
+    <t>ver el precio de los productos con su precio</t>
+  </si>
+  <si>
+    <t>Ver los productos a vender</t>
+  </si>
+  <si>
+    <t>Visualizar reportes de ventas</t>
+  </si>
+  <si>
+    <t>Visualizar reportes de ventas realizadas en un periodo de tiempo</t>
+  </si>
+  <si>
+    <t>Calcular el precio total de venta</t>
+  </si>
+  <si>
+    <t>Cobrar al cliente el valor exacto de sus productos, con el valor del iva incluido</t>
+  </si>
+  <si>
+    <t>realizar la busqueda de una determinada compra mediante su código de venta</t>
+  </si>
+  <si>
+    <t>Crear una base de datos</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Crear proyecto en C# y configurarlo</t>
+  </si>
+  <si>
+    <t>Emilio</t>
+  </si>
+  <si>
+    <t>Conectar base de datos con proyecto</t>
+  </si>
+  <si>
+    <t>Crear procedimientos de almacenamiento en base de datos</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Crear tablas y campos de base de datos</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Configurar el programa para almacenar datos</t>
+  </si>
+  <si>
+    <t>Robinson</t>
+  </si>
+  <si>
+    <t>Crear formulario de categorías de productos</t>
+  </si>
+  <si>
+    <t>Configurar opciones de CRUD en formulario de categorias</t>
+  </si>
+  <si>
+    <t>Crear formulario de artículos/productos</t>
+  </si>
+  <si>
+    <t>Crear listado de artículos</t>
+  </si>
+  <si>
+    <t>Crear tablas y configuración del programa de clientes</t>
+  </si>
+  <si>
+    <t>Crear tablas y configuración de trabajadores</t>
+  </si>
+  <si>
+    <t>Crear sistema de acceso</t>
+  </si>
+  <si>
+    <t>Sebastian/Emilio</t>
+  </si>
+  <si>
+    <t>Crear gestión de accesos</t>
+  </si>
+  <si>
+    <t>Formulario principal</t>
+  </si>
+  <si>
+    <t>Formularios de ingresos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formulario y registro de ventas </t>
+  </si>
+  <si>
+    <t>Tablas de ventas (base de datos)</t>
+  </si>
+  <si>
+    <t>Generación e impresión de facturas</t>
+  </si>
+  <si>
+    <t>Crear reportes de ventas</t>
+  </si>
+  <si>
+    <t>Crear formulario de reportes de ventas</t>
+  </si>
+  <si>
+    <t>Generar listado de artículos</t>
+  </si>
+  <si>
+    <t>Crear instalador</t>
+  </si>
+  <si>
+    <t>Generar reportes de ingresos</t>
+  </si>
+  <si>
+    <t>Realizar pruebas de software</t>
+  </si>
+  <si>
+    <t>Grupo</t>
+  </si>
+  <si>
+    <t>Configurar el formulario de artículos para crear, eliminar, editar artículos</t>
+  </si>
+  <si>
+    <t>Media</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1045,7 +1085,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1090,8 +1130,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1139,20 +1177,108 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="35">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1635,7 +1761,7 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -1713,9 +1839,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1782,7 +1908,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1882,40 +2008,40 @@
                   <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>144</c:v>
+                  <c:v>153.04347826086956</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>128</c:v>
+                  <c:v>146.08695652173913</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>112</c:v>
+                  <c:v>139.13043478260869</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96</c:v>
+                  <c:v>132.17391304347825</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80</c:v>
+                  <c:v>125.21739130434783</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>64</c:v>
+                  <c:v>118.26086956521739</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>48</c:v>
+                  <c:v>111.30434782608697</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32</c:v>
+                  <c:v>104.34782608695653</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16</c:v>
+                  <c:v>97.391304347826093</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>90.434782608695656</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -2050,7 +2176,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -2193,7 +2319,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -2253,7 +2379,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="234865584"/>
@@ -2312,7 +2438,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="234865192"/>
@@ -2354,7 +2480,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2384,7 +2510,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2955,7 +3081,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2976,47 +3108,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <tableColumns count="2">
-    <tableColumn id="1" name="Column1" headerRowDxfId="26" dataDxfId="25"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="24" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" headerRowDxfId="32" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" headerRowDxfId="30" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SprintBacklog" displayName="SprintBacklog" ref="A2:G13" totalsRowCount="1" headerRowDxfId="22" dataDxfId="21" totalsRowDxfId="20">
-  <autoFilter ref="A2:G12"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Sprint" totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="2" name="Item ID" dataDxfId="17" totalsRowDxfId="16">
-      <calculatedColumnFormula>IFERROR(B2+1,1)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="4" name="Task Name" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="5" name="Assigned To" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="6" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8">
-      <calculatedColumnFormula>SprintBacklog[[#This Row],[Estimated Hours]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" name="Status" dataDxfId="7" totalsRowDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9690B42F-0F66-42FC-96B5-C92407E5E0AA}" name="Table25" displayName="Table25" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{2C1DE8EA-74A8-4808-A174-BDA31F8B91A8}" name="Column1" headerRowDxfId="3" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{CDAA31F4-B050-43BF-9BE8-A878D23B1774}" name="Column2" headerRowDxfId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:D13" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A2:D13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="SprintBacklog" displayName="SprintBacklog" ref="A2:G13" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
+  <autoFilter ref="A2:G12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Sprint" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Item ID" dataDxfId="23" totalsRowDxfId="22">
+      <calculatedColumnFormula>IFERROR(B2+1,1)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Task Name" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Assigned To" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14">
+      <calculatedColumnFormula>SprintBacklog[[#This Row],[Estimated Hours]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Status" dataDxfId="13" totalsRowDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A2:D13" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A2:D13" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Work Day" dataDxfId="3"/>
-    <tableColumn id="2" name="Target Burn Down" dataDxfId="2">
-      <calculatedColumnFormula>IFERROR(TotalHours-(Table3[Work Day]*(TotalHours/WorkingDays)),0)</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Work Day" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Target Burn Down" dataDxfId="8">
+      <calculatedColumnFormula>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="1">
-      <calculatedColumnFormula>TotalHours-(Table3[Work Day]*DevRate)</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Forecast Burn Down" dataDxfId="7">
+      <calculatedColumnFormula>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Actual Burn Down" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Actual Burn Down" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3284,356 +3426,382 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="51.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="63.85546875" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="37" t="s">
+      <c r="A1" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="36" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>159</v>
+      <c r="A2" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>123</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>161</v>
+        <v>122</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G2" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>111</v>
+        <v>81</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>157</v>
+      <c r="A3" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>125</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="G3" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="30" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>143</v>
+      <c r="B4" s="31" t="s">
+        <v>108</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="F4" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>179</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="G4" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="30" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>164</v>
+      <c r="B5" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>128</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="G5" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="30" t="s">
-        <v>111</v>
+      <c r="H5" s="28" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>167</v>
+      <c r="A6" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>131</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="G6" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="30" t="s">
-        <v>111</v>
+      <c r="H6" s="28" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>168</v>
+      <c r="A7" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>132</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="30" t="s">
-        <v>111</v>
+      <c r="H7" s="28" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>143</v>
+      <c r="A8" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>108</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>170</v>
+        <v>134</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>171</v>
+        <v>135</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="30" t="s">
-        <v>111</v>
+        <v>179</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
-        <v>151</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>143</v>
+      <c r="A9" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>108</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>111</v>
+        <v>179</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="32" t="s">
-        <v>152</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>143</v>
+      <c r="A10" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>108</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>63</v>
+        <v>140</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>64</v>
+        <v>139</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="G10" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="30" t="s">
-        <v>111</v>
+      <c r="H10" s="28" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="B11" s="33" t="s">
+      <c r="A11" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>65</v>
-      </c>
       <c r="E11" s="23" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="G11" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="30" t="s">
-        <v>111</v>
+      <c r="H11" s="28" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>143</v>
+      <c r="A12" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>108</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>45</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>68</v>
+        <v>142</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="G12" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="F13" s="69" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="30" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" s="31" t="s">
-        <v>111</v>
+      <c r="H13" s="28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="70" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="70" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14" s="69" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="71" t="s">
+        <v>179</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3642,14 +3810,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="32.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="19"/>
@@ -3663,16 +3834,16 @@
         <v>38</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>10</v>
@@ -3705,73 +3876,73 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="43" t="s">
-        <v>77</v>
+      <c r="B3" s="38"/>
+      <c r="C3" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="40"/>
+      <c r="I3" s="41" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="62" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" s="45"/>
-      <c r="I4" s="46">
-        <v>5</v>
+      <c r="B4" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="63" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
-      <c r="B5" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="C5" s="64" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="48" t="s">
-        <v>102</v>
-      </c>
-      <c r="H5" s="48"/>
-      <c r="I5" s="49">
-        <v>5</v>
+      <c r="B5" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="H5" s="46"/>
+      <c r="I5" s="47">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
       <c r="G6" s="18"/>
-      <c r="H6" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="I6" s="58">
+      <c r="H6" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" s="56">
         <f>SUM(I4:I5)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3786,16 +3957,16 @@
         <v>38</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>10</v>
@@ -3810,13 +3981,13 @@
         <v>44</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>50</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20" t="s">
@@ -3830,90 +4001,90 @@
       <c r="A9" s="19"/>
       <c r="B9" s="18"/>
       <c r="C9" s="22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
-      <c r="B10" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="C10" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="H10" s="42"/>
-      <c r="I10" s="50">
-        <v>7</v>
+      <c r="B10" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="H10" s="40"/>
+      <c r="I10" s="48">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
-      <c r="B11" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="C11" s="62" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="H11" s="45"/>
-      <c r="I11" s="46">
-        <v>7</v>
+      <c r="B11" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="H11" s="43"/>
+      <c r="I11" s="44">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
-      <c r="B12" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="C12" s="64" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="48" t="s">
-        <v>103</v>
-      </c>
-      <c r="H12" s="48"/>
-      <c r="I12" s="51">
-        <v>6</v>
+      <c r="B12" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="61" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="H12" s="46"/>
+      <c r="I12" s="49">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="59"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
       <c r="G13" s="18"/>
-      <c r="H13" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="I13" s="58">
+      <c r="H13" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="I13" s="56">
         <f>SUM(I10:I12)</f>
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3928,16 +4099,16 @@
         <v>38</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>10</v>
@@ -3972,74 +4143,74 @@
       <c r="A16" s="19"/>
       <c r="B16" s="18"/>
       <c r="C16" s="22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
-      <c r="B17" s="40" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" s="60" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="H17" s="42"/>
-      <c r="I17" s="50">
-        <v>4</v>
+      <c r="B17" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="66" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="H17" s="40"/>
+      <c r="I17" s="48">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
-      <c r="B18" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" s="62" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="H18" s="45"/>
-      <c r="I18" s="46">
-        <v>4</v>
+      <c r="B18" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="63" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="H18" s="43"/>
+      <c r="I18" s="44">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
-      <c r="B19" s="47" t="s">
-        <v>118</v>
-      </c>
-      <c r="C19" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="48" t="s">
-        <v>102</v>
-      </c>
-      <c r="H19" s="48"/>
-      <c r="I19" s="49">
-        <v>2</v>
+      <c r="B19" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="61" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="H19" s="46"/>
+      <c r="I19" s="47">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4050,12 +4221,12 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
-      <c r="H20" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="I20" s="58">
+      <c r="H20" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" s="56">
         <f>SUM(I17:I19)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -4070,16 +4241,16 @@
         <v>38</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I21" s="17" t="s">
         <v>10</v>
@@ -4114,69 +4285,69 @@
       <c r="A23" s="19"/>
       <c r="B23" s="18"/>
       <c r="C23" s="22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
-      <c r="B24" s="40" t="s">
-        <v>121</v>
-      </c>
-      <c r="C24" s="60" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="H24" s="42"/>
-      <c r="I24" s="50">
-        <v>5</v>
+      <c r="B24" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="66" t="s">
+        <v>159</v>
+      </c>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="H24" s="40"/>
+      <c r="I24" s="48">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
-      <c r="B25" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="C25" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="48" t="s">
-        <v>103</v>
-      </c>
-      <c r="H25" s="48"/>
-      <c r="I25" s="49">
-        <v>5</v>
+      <c r="B25" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="72" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="H25" s="46"/>
+      <c r="I25" s="47">
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
       <c r="G26" s="18"/>
-      <c r="H26" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="I26" s="58">
+      <c r="H26" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="I26" s="56">
         <f>SUM(I24:I25)</f>
         <v>10</v>
       </c>
@@ -4193,16 +4364,16 @@
         <v>38</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I27" s="17" t="s">
         <v>10</v>
@@ -4248,55 +4419,55 @@
       <c r="A30" s="19"/>
       <c r="B30" s="18"/>
       <c r="C30" s="22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H30" s="18"/>
       <c r="I30" s="22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
-      <c r="B31" s="40" t="s">
-        <v>123</v>
-      </c>
-      <c r="C31" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="H31" s="42"/>
-      <c r="I31" s="50">
-        <v>5</v>
+      <c r="B31" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="66" t="s">
+        <v>160</v>
+      </c>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="H31" s="40"/>
+      <c r="I31" s="48">
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
-      <c r="B32" s="47" t="s">
-        <v>124</v>
-      </c>
-      <c r="C32" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="48" t="s">
-        <v>103</v>
-      </c>
-      <c r="H32" s="48"/>
-      <c r="I32" s="49">
-        <v>5</v>
+      <c r="B32" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="61" t="s">
+        <v>162</v>
+      </c>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="H32" s="46"/>
+      <c r="I32" s="47">
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4307,10 +4478,10 @@
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
       <c r="G33" s="18"/>
-      <c r="H33" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="I33" s="58">
+      <c r="H33" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="I33" s="56">
         <f>SUM(I31:I32)</f>
         <v>10</v>
       </c>
@@ -4327,16 +4498,16 @@
         <v>38</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>41</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I34" s="17" t="s">
         <v>10</v>
@@ -4371,599 +4542,167 @@
       <c r="A36" s="19"/>
       <c r="B36" s="18"/>
       <c r="C36" s="22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H36" s="18"/>
       <c r="I36" s="22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
-      <c r="B37" s="40" t="s">
-        <v>125</v>
-      </c>
-      <c r="C37" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D37" s="61"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="61"/>
-      <c r="G37" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="H37" s="42"/>
-      <c r="I37" s="50">
+      <c r="B37" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="66" t="s">
+        <v>161</v>
+      </c>
+      <c r="D37" s="67"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="67"/>
+      <c r="G37" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="H37" s="40"/>
+      <c r="I37" s="48">
         <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19"/>
-      <c r="B38" s="47" t="s">
-        <v>126</v>
-      </c>
-      <c r="C38" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="D38" s="65"/>
-      <c r="E38" s="65"/>
-      <c r="F38" s="65"/>
-      <c r="G38" s="48" t="s">
-        <v>103</v>
-      </c>
-      <c r="H38" s="48"/>
-      <c r="I38" s="49">
-        <v>5</v>
+      <c r="B38" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="H38" s="46"/>
+      <c r="I38" s="47">
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
       <c r="B39" s="18"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="59"/>
-      <c r="E39" s="59"/>
-      <c r="F39" s="59"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="65"/>
       <c r="G39" s="18"/>
-      <c r="H39" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="I39" s="58">
+      <c r="H39" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="I39" s="56">
         <f>SUM(I37:I38)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
-      <c r="B40" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F40" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H40" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="I40" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A41" s="19"/>
-      <c r="B41" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E41" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="G41" s="21"/>
-      <c r="H41" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I41" s="20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H41" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="I41" s="51">
+        <f>I6+I13+I20+I26+I33+I39</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="19"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="H42" s="18"/>
-      <c r="I42" s="22" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
-      <c r="B43" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="C43" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43" s="61"/>
-      <c r="E43" s="61"/>
-      <c r="F43" s="61"/>
-      <c r="G43" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="H43" s="42"/>
-      <c r="I43" s="50">
-        <v>3</v>
-      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
-      <c r="B44" s="44" t="s">
-        <v>128</v>
-      </c>
-      <c r="C44" s="62" t="s">
-        <v>93</v>
-      </c>
-      <c r="D44" s="63"/>
-      <c r="E44" s="63"/>
-      <c r="F44" s="63"/>
-      <c r="G44" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="H44" s="45"/>
-      <c r="I44" s="46">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="19"/>
-      <c r="B45" s="47" t="s">
-        <v>129</v>
-      </c>
-      <c r="C45" s="64" t="s">
-        <v>94</v>
-      </c>
-      <c r="D45" s="65"/>
-      <c r="E45" s="65"/>
-      <c r="F45" s="65"/>
-      <c r="G45" s="48" t="s">
-        <v>102</v>
-      </c>
-      <c r="H45" s="48"/>
-      <c r="I45" s="49">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="19"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="I46" s="58">
-        <f>SUM(I43:I45)</f>
-        <v>10</v>
-      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
-      <c r="B47" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E47" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F47" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="G47" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H47" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="I47" s="17" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
-      <c r="B48" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="F48" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="G48" s="21"/>
-      <c r="H48" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I48" s="20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="19"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="H49" s="18"/>
-      <c r="I49" s="22" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="19"/>
-      <c r="B50" s="40" t="s">
-        <v>130</v>
-      </c>
-      <c r="C50" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="D50" s="61"/>
-      <c r="E50" s="61"/>
-      <c r="F50" s="61"/>
-      <c r="G50" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="H50" s="42"/>
-      <c r="I50" s="50">
-        <v>7</v>
-      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="19"/>
-      <c r="B51" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="C51" s="62" t="s">
-        <v>96</v>
-      </c>
-      <c r="D51" s="63"/>
-      <c r="E51" s="63"/>
-      <c r="F51" s="63"/>
-      <c r="G51" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="H51" s="45"/>
-      <c r="I51" s="46">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="19"/>
-      <c r="B52" s="47" t="s">
-        <v>132</v>
-      </c>
-      <c r="C52" s="64" t="s">
-        <v>97</v>
-      </c>
-      <c r="D52" s="65"/>
-      <c r="E52" s="65"/>
-      <c r="F52" s="65"/>
-      <c r="G52" s="48" t="s">
-        <v>103</v>
-      </c>
-      <c r="H52" s="48"/>
-      <c r="I52" s="49">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H53" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="I53" s="58">
-        <f>SUM(I50:I52)</f>
-        <v>20</v>
-      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C54" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D54" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E54" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F54" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="G54" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H54" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="I54" s="17" t="s">
-        <v>10</v>
-      </c>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C55" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D55" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E55" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F55" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="G55" s="21"/>
-      <c r="H55" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I55" s="20" t="s">
-        <v>49</v>
-      </c>
+      <c r="B55" s="18"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="22"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-    </row>
-    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="17"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B57" s="18"/>
-      <c r="C57" s="22" t="s">
-        <v>75</v>
-      </c>
+      <c r="C57" s="22"/>
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
       <c r="F57" s="18"/>
-      <c r="G57" s="22" t="s">
-        <v>76</v>
-      </c>
+      <c r="G57" s="22"/>
       <c r="H57" s="18"/>
-      <c r="I57" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="40" t="s">
-        <v>133</v>
-      </c>
-      <c r="C58" s="60" t="s">
-        <v>98</v>
-      </c>
-      <c r="D58" s="61"/>
-      <c r="E58" s="61"/>
-      <c r="F58" s="61"/>
-      <c r="G58" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="H58" s="42"/>
-      <c r="I58" s="50">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="C59" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="D59" s="48"/>
-      <c r="E59" s="48"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="48" t="s">
-        <v>103</v>
-      </c>
-      <c r="H59" s="48"/>
-      <c r="I59" s="49">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="18"/>
-      <c r="C60" s="59"/>
-      <c r="D60" s="59"/>
-      <c r="E60" s="59"/>
-      <c r="F60" s="59"/>
-      <c r="G60" s="18"/>
-      <c r="H60" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="I60" s="58">
-        <f>SUM(I58:I59)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B61" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D61" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E61" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F61" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="G61" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H61" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="I61" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C62" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D62" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E62" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="F62" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="G62" s="21"/>
-      <c r="H62" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I62" s="20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="18"/>
-      <c r="C63" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="H63" s="18"/>
-      <c r="I63" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B64" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="C64" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="D64" s="61"/>
-      <c r="E64" s="61"/>
-      <c r="F64" s="61"/>
-      <c r="G64" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="H64" s="42"/>
-      <c r="I64" s="50">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="65" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="47" t="s">
-        <v>135</v>
-      </c>
-      <c r="C65" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="D65" s="48"/>
-      <c r="E65" s="48"/>
-      <c r="F65" s="48"/>
-      <c r="G65" s="48" t="s">
-        <v>102</v>
-      </c>
-      <c r="H65" s="48"/>
-      <c r="I65" s="49">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H66" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="I66" s="58">
-        <f>SUM(I64:I65)</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="67" spans="2:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="H67" s="53" t="s">
-        <v>113</v>
-      </c>
-      <c r="I67" s="53">
-        <f>I6+I13+I20+I26+I33+I39+I46+I53+I60+I66</f>
-        <v>160</v>
-      </c>
+      <c r="I57" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="18">
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C5:F5"/>
@@ -4976,314 +4715,607 @@
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="C64:F64"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="C52:F52"/>
-    <mergeCell ref="C58:F58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="B1" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="21"/>
+      <c r="H2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="18"/>
+      <c r="C3" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="H4" s="40"/>
+      <c r="I4" s="48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="63" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="H5" s="43"/>
+      <c r="I5" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="61" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" s="46"/>
+      <c r="I6" s="47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="56">
+        <f>SUM(I4:I6)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C8" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D8" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E8" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="18"/>
+      <c r="C10" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="H10" s="18"/>
+      <c r="I10" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>168</v>
+      </c>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="H11" s="40"/>
+      <c r="I11" s="48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="H12" s="43"/>
+      <c r="I12" s="44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="61" t="s">
+        <v>170</v>
+      </c>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="46" t="s">
+        <v>152</v>
+      </c>
+      <c r="H13" s="46"/>
+      <c r="I13" s="47">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="56">
+        <f>SUM(I11:I13)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H16" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="21"/>
+      <c r="H17" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="60"/>
+      <c r="C18" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="60"/>
+      <c r="I18" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="17" t="s">
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="66" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="57" t="s">
+        <v>156</v>
+      </c>
+      <c r="H19" s="57"/>
+      <c r="I19" s="48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59" t="s">
+        <v>154</v>
+      </c>
+      <c r="H20" s="59"/>
+      <c r="I20" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="60"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="I21" s="55">
+        <f>SUM(I19:I20)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" s="17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="20" t="s">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D24" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E24" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="G24" s="21"/>
+      <c r="H24" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="60"/>
+      <c r="C25" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" s="60"/>
+      <c r="I25" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="18"/>
-      <c r="C4" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="40" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" s="60" t="s">
+      <c r="C26" s="66" t="s">
+        <v>173</v>
+      </c>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="57" t="s">
+        <v>164</v>
+      </c>
+      <c r="H26" s="57"/>
+      <c r="I26" s="48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="H5" s="42"/>
-      <c r="I5" s="50">
+      <c r="C27" s="66" t="s">
+        <v>175</v>
+      </c>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="58" t="s">
+        <v>152</v>
+      </c>
+      <c r="H27" s="58"/>
+      <c r="I27" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="61" t="s">
+        <v>174</v>
+      </c>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="59" t="s">
+        <v>149</v>
+      </c>
+      <c r="H28" s="59"/>
+      <c r="I28" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="59" t="s">
+        <v>177</v>
+      </c>
+      <c r="H29" s="59"/>
+      <c r="I29" s="47">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="47" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="48" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="H6" s="48"/>
-      <c r="I6" s="49">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="18"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="56" t="s">
-        <v>114</v>
-      </c>
-      <c r="I7" s="57">
-        <f>SUM(I5:I6)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I10" s="20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="18"/>
-      <c r="C11" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="40" t="s">
-        <v>138</v>
-      </c>
-      <c r="C12" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="H12" s="42"/>
-      <c r="I12" s="50">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="C13" s="64" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="48" t="s">
-        <v>102</v>
-      </c>
-      <c r="H13" s="48"/>
-      <c r="I13" s="49">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H14" s="54" t="s">
-        <v>114</v>
-      </c>
-      <c r="I14" s="55">
-        <f>SUM(I12:I13)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H15" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="I15" s="52">
-        <f>I7+I14</f>
-        <v>40</v>
+    <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H30" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="I30" s="53">
+        <f>SUM(I26:I29)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H31" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="I31" s="50">
+        <f>I14+I7+I21+I30</f>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
+  <mergeCells count="12">
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" customWidth="1"/>
@@ -5298,7 +5330,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5">
-        <v>43271</v>
+        <v>44552</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>19</v>
@@ -5306,7 +5338,7 @@
     </row>
     <row r="3" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6">
-        <v>43284</v>
+        <v>44583</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -5318,7 +5350,7 @@
       </c>
       <c r="B4" s="3">
         <f>NETWORKDAYS(B2,B3)</f>
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -5339,7 +5371,7 @@
       </c>
       <c r="B6" s="3">
         <f>B4-B5</f>
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -5348,7 +5380,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -5357,7 +5389,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="8">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -5369,7 +5401,7 @@
       </c>
       <c r="B9" s="3">
         <f>(B4-B5)*B8*B7*8</f>
-        <v>160</v>
+        <v>368</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -5414,14 +5446,152 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79BF2F1-DFA9-47D0-A6C6-5EF1E2B2F467}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11" style="3" customWidth="1"/>
+    <col min="3" max="3" width="43.42578125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <v>44584</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="6">
+        <v>44614</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3">
+        <f>NETWORKDAYS(B2,B3)</f>
+        <v>22</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3">
+        <f>B4-B5</f>
+        <v>22</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3">
+        <f>(B4-B5)*B8*B7*8</f>
+        <v>352</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3">
+        <f>IFERROR(B9/B4,0)</f>
+        <v>16</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:G13"/>
   <sheetViews>
-    <sheetView topLeftCell="E8" zoomScale="268" zoomScaleNormal="268" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="9.5703125" style="3" customWidth="1"/>
@@ -5701,7 +5871,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G12" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"In Progress, Completed, Blocked"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5712,15 +5882,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:E13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="7.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="3" customWidth="1"/>
     <col min="2" max="4" width="10.28515625" style="15" customWidth="1"/>
@@ -5747,11 +5917,11 @@
         <v>0</v>
       </c>
       <c r="B3" s="15">
-        <f>IFERROR(TotalHours-(Table3[Work Day]*(TotalHours/WorkingDays)),0)</f>
+        <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
         <v>160</v>
       </c>
       <c r="C3" s="15">
-        <f>TotalHours-(Table3[Work Day]*DevRate)</f>
+        <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
         <v>160</v>
       </c>
       <c r="D3" s="15">
@@ -5765,11 +5935,11 @@
         <v>1</v>
       </c>
       <c r="B4" s="15">
-        <f>IFERROR(TotalHours-(Table3[Work Day]*(TotalHours/WorkingDays)),0)</f>
-        <v>144</v>
+        <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
+        <v>153.04347826086956</v>
       </c>
       <c r="C4" s="15">
-        <f>TotalHours-(Table3[Work Day]*DevRate)</f>
+        <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
         <v>144</v>
       </c>
       <c r="D4" s="16">
@@ -5782,11 +5952,11 @@
         <v>2</v>
       </c>
       <c r="B5" s="15">
-        <f>IFERROR(TotalHours-(Table3[Work Day]*(TotalHours/WorkingDays)),0)</f>
-        <v>128</v>
+        <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
+        <v>146.08695652173913</v>
       </c>
       <c r="C5" s="15">
-        <f>TotalHours-(Table3[Work Day]*DevRate)</f>
+        <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
         <v>128</v>
       </c>
       <c r="D5" s="16">
@@ -5799,11 +5969,11 @@
         <v>3</v>
       </c>
       <c r="B6" s="15">
-        <f>IFERROR(TotalHours-(Table3[Work Day]*(TotalHours/WorkingDays)),0)</f>
-        <v>112</v>
+        <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
+        <v>139.13043478260869</v>
       </c>
       <c r="C6" s="15">
-        <f>TotalHours-(Table3[Work Day]*DevRate)</f>
+        <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
         <v>112</v>
       </c>
       <c r="D6" s="16">
@@ -5816,11 +5986,11 @@
         <v>4</v>
       </c>
       <c r="B7" s="15">
-        <f>IFERROR(TotalHours-(Table3[Work Day]*(TotalHours/WorkingDays)),0)</f>
-        <v>96</v>
+        <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
+        <v>132.17391304347825</v>
       </c>
       <c r="C7" s="15">
-        <f>TotalHours-(Table3[Work Day]*DevRate)</f>
+        <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
         <v>96</v>
       </c>
       <c r="D7" s="16">
@@ -5833,11 +6003,11 @@
         <v>5</v>
       </c>
       <c r="B8" s="15">
-        <f>IFERROR(TotalHours-(Table3[Work Day]*(TotalHours/WorkingDays)),0)</f>
-        <v>80</v>
+        <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
+        <v>125.21739130434783</v>
       </c>
       <c r="C8" s="15">
-        <f>TotalHours-(Table3[Work Day]*DevRate)</f>
+        <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
         <v>80</v>
       </c>
       <c r="D8" s="16">
@@ -5850,11 +6020,11 @@
         <v>6</v>
       </c>
       <c r="B9" s="15">
-        <f>IFERROR(TotalHours-(Table3[Work Day]*(TotalHours/WorkingDays)),0)</f>
-        <v>64</v>
+        <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
+        <v>118.26086956521739</v>
       </c>
       <c r="C9" s="15">
-        <f>TotalHours-(Table3[Work Day]*DevRate)</f>
+        <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
         <v>64</v>
       </c>
       <c r="D9" s="16">
@@ -5867,11 +6037,11 @@
         <v>7</v>
       </c>
       <c r="B10" s="15">
-        <f>IFERROR(TotalHours-(Table3[Work Day]*(TotalHours/WorkingDays)),0)</f>
-        <v>48</v>
+        <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
+        <v>111.30434782608697</v>
       </c>
       <c r="C10" s="15">
-        <f>TotalHours-(Table3[Work Day]*DevRate)</f>
+        <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
         <v>48</v>
       </c>
       <c r="D10" s="16">
@@ -5884,11 +6054,11 @@
         <v>8</v>
       </c>
       <c r="B11" s="15">
-        <f>IFERROR(TotalHours-(Table3[Work Day]*(TotalHours/WorkingDays)),0)</f>
-        <v>32</v>
+        <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
+        <v>104.34782608695653</v>
       </c>
       <c r="C11" s="15">
-        <f>TotalHours-(Table3[Work Day]*DevRate)</f>
+        <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
         <v>32</v>
       </c>
       <c r="D11" s="16">
@@ -5901,11 +6071,11 @@
         <v>9</v>
       </c>
       <c r="B12" s="15">
-        <f>IFERROR(TotalHours-(Table3[Work Day]*(TotalHours/WorkingDays)),0)</f>
-        <v>16</v>
+        <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
+        <v>97.391304347826093</v>
       </c>
       <c r="C12" s="15">
-        <f>TotalHours-(Table3[Work Day]*DevRate)</f>
+        <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
         <v>16</v>
       </c>
       <c r="D12" s="16">
@@ -5918,11 +6088,11 @@
         <v>10</v>
       </c>
       <c r="B13" s="15">
-        <f>IFERROR(TotalHours-(Table3[Work Day]*(TotalHours/WorkingDays)),0)</f>
-        <v>0</v>
+        <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
+        <v>90.434782608695656</v>
       </c>
       <c r="C13" s="15">
-        <f>TotalHours-(Table3[Work Day]*DevRate)</f>
+        <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
         <v>0</v>
       </c>
       <c r="D13" s="16">

</xml_diff>

<commit_message>
Se designaron y corrigieron los nombres y tiempos estimados en el burndonw1table
</commit_message>
<xml_diff>
--- a/Excel-Burndown-Chart-Template.xlsx
+++ b/Excel-Burndown-Chart-Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="4" r:id="rId1"/>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="179">
   <si>
     <t>Start Date</t>
   </si>
@@ -350,9 +350,6 @@
     <t>visualizar los productos que se adquirieron en una compra</t>
   </si>
   <si>
-    <t>HU11</t>
-  </si>
-  <si>
     <t>No iniciado</t>
   </si>
   <si>
@@ -419,12 +416,6 @@
     <t>HU8-3</t>
   </si>
   <si>
-    <t>HU11-1</t>
-  </si>
-  <si>
-    <t>HU11-2</t>
-  </si>
-  <si>
     <t>HU2-3</t>
   </si>
   <si>
@@ -653,10 +644,19 @@
     <t>HU10-2</t>
   </si>
   <si>
-    <t>HU11-3</t>
-  </si>
-  <si>
-    <t>HU11-4</t>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>HU9-1</t>
+  </si>
+  <si>
+    <t>HU9-2</t>
+  </si>
+  <si>
+    <t>HU10-3</t>
+  </si>
+  <si>
+    <t>HU10-4</t>
   </si>
 </sst>
 </file>
@@ -1247,16 +1247,16 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1264,125 +1264,6 @@
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="41">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1548,6 +1429,23 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1578,6 +1476,23 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1617,6 +1532,23 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1647,6 +1579,23 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1686,6 +1635,23 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1719,6 +1685,23 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1734,6 +1717,23 @@
           <color indexed="64"/>
         </right>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -2103,10 +2103,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BurnDown1Table!$A$3:$A$26</c:f>
+              <c:f>BurnDown1Table!$A$3:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2169,95 +2169,77 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BurnDown1Table!$B$3:$B$26</c:f>
+              <c:f>BurnDown1Table!$B$3:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>124</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>118.60869565217391</c:v>
+                  <c:v>54.15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>113.21739130434783</c:v>
+                  <c:v>51.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>107.82608695652173</c:v>
+                  <c:v>48.45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>102.43478260869566</c:v>
+                  <c:v>45.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>97.043478260869563</c:v>
+                  <c:v>42.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>91.65217391304347</c:v>
+                  <c:v>39.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>86.260869565217391</c:v>
+                  <c:v>37.049999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80.869565217391312</c:v>
+                  <c:v>34.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>75.478260869565219</c:v>
+                  <c:v>31.349999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>70.086956521739125</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64.695652173913047</c:v>
+                  <c:v>25.65</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>59.304347826086953</c:v>
+                  <c:v>22.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>53.913043478260875</c:v>
+                  <c:v>19.949999999999996</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>48.521739130434781</c:v>
+                  <c:v>17.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43.130434782608702</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>37.739130434782609</c:v>
+                  <c:v>11.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>32.347826086956516</c:v>
+                  <c:v>8.5499999999999972</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26.956521739130437</c:v>
+                  <c:v>5.6999999999999957</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>21.565217391304344</c:v>
+                  <c:v>2.8500000000000014</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>16.173913043478265</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>10.782608695652172</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5.3913043478260931</c:v>
-                </c:pt>
-                <c:pt idx="23">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2316,10 +2298,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BurnDown1Table!$A$3:$A$26</c:f>
+              <c:f>BurnDown1Table!$A$3:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2382,96 +2364,78 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BurnDown1Table!$C$3:$C$26</c:f>
+              <c:f>BurnDown1Table!$C$3:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>124</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108</c:v>
+                  <c:v>50.043478260869563</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92</c:v>
+                  <c:v>43.086956521739133</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76</c:v>
+                  <c:v>36.130434782608695</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60</c:v>
+                  <c:v>29.173913043478262</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44</c:v>
+                  <c:v>22.217391304347828</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28</c:v>
+                  <c:v>15.260869565217391</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12</c:v>
+                  <c:v>8.3043478260869605</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4</c:v>
+                  <c:v>1.3478260869565233</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-20</c:v>
+                  <c:v>-5.608695652173914</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-36</c:v>
+                  <c:v>-12.565217391304344</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-52</c:v>
+                  <c:v>-19.521739130434781</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-68</c:v>
+                  <c:v>-26.478260869565219</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-84</c:v>
+                  <c:v>-33.434782608695656</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-100</c:v>
+                  <c:v>-40.391304347826079</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-116</c:v>
+                  <c:v>-47.347826086956516</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-132</c:v>
+                  <c:v>-54.304347826086953</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-148</c:v>
+                  <c:v>-61.260869565217391</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-164</c:v>
+                  <c:v>-68.217391304347828</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-180</c:v>
+                  <c:v>-75.173913043478251</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-196</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-212</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-228</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-244</c:v>
+                  <c:v>-82.130434782608688</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2537,10 +2501,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BurnDown1Table!$A$3:$A$26</c:f>
+              <c:f>BurnDown1Table!$A$3:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2603,96 +2567,78 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BurnDown1Table!$D$3:$D$26</c:f>
+              <c:f>BurnDown1Table!$D$3:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>124</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>170</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>120</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2714,11 +2660,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="243407336"/>
-        <c:axId val="243407728"/>
+        <c:axId val="236348624"/>
+        <c:axId val="236349016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="243407336"/>
+        <c:axId val="236348624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2761,7 +2707,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243407728"/>
+        <c:crossAx val="236349016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2769,7 +2715,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243407728"/>
+        <c:axId val="236349016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2820,7 +2766,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243407336"/>
+        <c:crossAx val="236348624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2946,7 +2892,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3022,10 +2967,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BurnDown1Table!$A$3:$A$26</c:f>
+              <c:f>BurnDown1Table!$A$3:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3088,95 +3033,77 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BurnDown1Table!$B$3:$B$26</c:f>
+              <c:f>BurnDown1Table!$B$3:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>124</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>118.60869565217391</c:v>
+                  <c:v>54.15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>113.21739130434783</c:v>
+                  <c:v>51.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>107.82608695652173</c:v>
+                  <c:v>48.45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>102.43478260869566</c:v>
+                  <c:v>45.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>97.043478260869563</c:v>
+                  <c:v>42.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>91.65217391304347</c:v>
+                  <c:v>39.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>86.260869565217391</c:v>
+                  <c:v>37.049999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80.869565217391312</c:v>
+                  <c:v>34.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>75.478260869565219</c:v>
+                  <c:v>31.349999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>70.086956521739125</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>64.695652173913047</c:v>
+                  <c:v>25.65</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>59.304347826086953</c:v>
+                  <c:v>22.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>53.913043478260875</c:v>
+                  <c:v>19.949999999999996</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>48.521739130434781</c:v>
+                  <c:v>17.100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>43.130434782608702</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>37.739130434782609</c:v>
+                  <c:v>11.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>32.347826086956516</c:v>
+                  <c:v>8.5499999999999972</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>26.956521739130437</c:v>
+                  <c:v>5.6999999999999957</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>21.565217391304344</c:v>
+                  <c:v>2.8500000000000014</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>16.173913043478265</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>10.782608695652172</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5.3913043478260931</c:v>
-                </c:pt>
-                <c:pt idx="23">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3235,10 +3162,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BurnDown1Table!$A$3:$A$26</c:f>
+              <c:f>BurnDown1Table!$A$3:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3301,96 +3228,78 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BurnDown1Table!$C$3:$C$26</c:f>
+              <c:f>BurnDown1Table!$C$3:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>124</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108</c:v>
+                  <c:v>50.043478260869563</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92</c:v>
+                  <c:v>43.086956521739133</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76</c:v>
+                  <c:v>36.130434782608695</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60</c:v>
+                  <c:v>29.173913043478262</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44</c:v>
+                  <c:v>22.217391304347828</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28</c:v>
+                  <c:v>15.260869565217391</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12</c:v>
+                  <c:v>8.3043478260869605</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4</c:v>
+                  <c:v>1.3478260869565233</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-20</c:v>
+                  <c:v>-5.608695652173914</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-36</c:v>
+                  <c:v>-12.565217391304344</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-52</c:v>
+                  <c:v>-19.521739130434781</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-68</c:v>
+                  <c:v>-26.478260869565219</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-84</c:v>
+                  <c:v>-33.434782608695656</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-100</c:v>
+                  <c:v>-40.391304347826079</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-116</c:v>
+                  <c:v>-47.347826086956516</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-132</c:v>
+                  <c:v>-54.304347826086953</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-148</c:v>
+                  <c:v>-61.260869565217391</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-164</c:v>
+                  <c:v>-68.217391304347828</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-180</c:v>
+                  <c:v>-75.173913043478251</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-196</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-212</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-228</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-244</c:v>
+                  <c:v>-82.130434782608688</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3456,10 +3365,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BurnDown1Table!$A$3:$A$26</c:f>
+              <c:f>BurnDown1Table!$A$3:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3522,96 +3431,78 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BurnDown1Table!$D$3:$D$26</c:f>
+              <c:f>BurnDown1Table!$D$3:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>124</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>170</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>120</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3633,11 +3524,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="243408512"/>
-        <c:axId val="244669568"/>
+        <c:axId val="236349800"/>
+        <c:axId val="236350192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="243408512"/>
+        <c:axId val="236349800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3680,7 +3571,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244669568"/>
+        <c:crossAx val="236350192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3688,7 +3579,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244669568"/>
+        <c:axId val="236350192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3739,7 +3630,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243408512"/>
+        <c:crossAx val="236349800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3753,7 +3644,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5013,54 +4903,54 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SprintBacklog" displayName="SprintBacklog" ref="A2:G14" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
-  <autoFilter ref="A2:G13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SprintBacklog" displayName="SprintBacklog" ref="A2:G17" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
+  <autoFilter ref="A2:G16"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Sprint" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="6"/>
-    <tableColumn id="2" name="Item ID" dataDxfId="24" totalsRowDxfId="5">
+    <tableColumn id="1" name="Sprint" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="Item ID" dataDxfId="23" totalsRowDxfId="22">
       <calculatedColumnFormula>IFERROR(B2+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="4"/>
-    <tableColumn id="4" name="Task Name" dataDxfId="22" totalsRowDxfId="3"/>
-    <tableColumn id="5" name="Assigned To" dataDxfId="21" totalsRowDxfId="2"/>
-    <tableColumn id="6" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="1">
+    <tableColumn id="3" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="Task Name" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="Assigned To" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula>SprintBacklog[[#This Row],[Estimated Hours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Status" dataDxfId="19" totalsRowDxfId="0"/>
+    <tableColumn id="7" name="Status" dataDxfId="13" totalsRowDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:D26" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A2:D26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:D23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A2:D23"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Work Day" dataDxfId="16"/>
-    <tableColumn id="2" name="Target Burn Down" dataDxfId="15">
+    <tableColumn id="1" name="Work Day" dataDxfId="9"/>
+    <tableColumn id="2" name="Target Burn Down" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="14">
+    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="7">
       <calculatedColumnFormula>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Actual Burn Down" dataDxfId="13"/>
+    <tableColumn id="4" name="Actual Burn Down" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table38" displayName="Table38" ref="A2:D13" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A2:D13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table38" displayName="Table38" ref="A2:D25" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A2:D25"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Work Day" dataDxfId="10"/>
-    <tableColumn id="2" name="Target Burn Down" dataDxfId="9">
-      <calculatedColumnFormula>IFERROR(TotalHours-(Table38[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</calculatedColumnFormula>
+    <tableColumn id="1" name="Work Day" dataDxfId="3"/>
+    <tableColumn id="2" name="Target Burn Down" dataDxfId="2">
+      <calculatedColumnFormula>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="8">
-      <calculatedColumnFormula>TotalHours-(Table38[[#This Row],[Work Day]]*DevRate)</calculatedColumnFormula>
+    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="1">
+      <calculatedColumnFormula>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Actual Burn Down" dataDxfId="7"/>
+    <tableColumn id="4" name="Actual Burn Down" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5331,7 +5221,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -5344,7 +5234,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>35</v>
@@ -5370,195 +5260,195 @@
     </row>
     <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G3" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G5" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G6" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>61</v>
@@ -5567,143 +5457,143 @@
         <v>62</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>116</v>
-      </c>
       <c r="D11" s="23" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="30" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>63</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F13" s="61" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G13" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="30" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C14" s="62" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D14" s="62" t="s">
         <v>64</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F14" s="61" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G14" s="63" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -5715,8 +5605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView topLeftCell="A29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5796,16 +5686,16 @@
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
       <c r="B4" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="71" t="s">
-        <v>141</v>
-      </c>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
+        <v>80</v>
+      </c>
+      <c r="C4" s="75" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
       <c r="G4" s="43" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H4" s="43"/>
       <c r="I4" s="44">
@@ -5815,16 +5705,16 @@
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
       <c r="B5" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="73" t="s">
-        <v>148</v>
-      </c>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
+        <v>99</v>
+      </c>
+      <c r="C5" s="71" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
       <c r="G5" s="46" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H5" s="46"/>
       <c r="I5" s="47">
@@ -5834,13 +5724,13 @@
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
       <c r="G6" s="18"/>
       <c r="H6" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I6" s="56">
         <f>SUM(I4:I5)</f>
@@ -5919,16 +5809,16 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="75" t="s">
-        <v>143</v>
-      </c>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
+        <v>81</v>
+      </c>
+      <c r="C10" s="69" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
       <c r="G10" s="40" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H10" s="40"/>
       <c r="I10" s="48">
@@ -5938,16 +5828,16 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="B11" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="71" t="s">
-        <v>145</v>
-      </c>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
+        <v>82</v>
+      </c>
+      <c r="C11" s="75" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
       <c r="G11" s="43" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H11" s="43"/>
       <c r="I11" s="44">
@@ -5957,16 +5847,16 @@
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
       <c r="B12" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="73" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
+        <v>98</v>
+      </c>
+      <c r="C12" s="71" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
       <c r="G12" s="46" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H12" s="46"/>
       <c r="I12" s="49">
@@ -5976,13 +5866,13 @@
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
       <c r="G13" s="18"/>
       <c r="H13" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I13" s="56">
         <f>SUM(I10:I12)</f>
@@ -6061,16 +5951,16 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="75" t="s">
-        <v>150</v>
-      </c>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
+        <v>84</v>
+      </c>
+      <c r="C17" s="69" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
       <c r="G17" s="40" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H17" s="40"/>
       <c r="I17" s="48">
@@ -6080,16 +5970,16 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="71" t="s">
-        <v>152</v>
-      </c>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
+        <v>85</v>
+      </c>
+      <c r="C18" s="75" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
       <c r="G18" s="43" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H18" s="43"/>
       <c r="I18" s="44">
@@ -6099,16 +5989,16 @@
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
       <c r="B19" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" s="73" t="s">
-        <v>153</v>
-      </c>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
+        <v>83</v>
+      </c>
+      <c r="C19" s="71" t="s">
+        <v>150</v>
+      </c>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
       <c r="G19" s="46" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H19" s="46"/>
       <c r="I19" s="47">
@@ -6124,7 +6014,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I20" s="56">
         <f>SUM(I17:I19)</f>
@@ -6203,16 +6093,16 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="75" t="s">
-        <v>154</v>
-      </c>
-      <c r="D24" s="76"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="76"/>
+        <v>86</v>
+      </c>
+      <c r="C24" s="69" t="s">
+        <v>151</v>
+      </c>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
       <c r="G24" s="40" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H24" s="40"/>
       <c r="I24" s="48">
@@ -6222,16 +6112,16 @@
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="70" t="s">
-        <v>173</v>
-      </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
-      <c r="F25" s="70"/>
+        <v>87</v>
+      </c>
+      <c r="C25" s="74" t="s">
+        <v>170</v>
+      </c>
+      <c r="D25" s="74"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
       <c r="G25" s="46" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H25" s="46"/>
       <c r="I25" s="47">
@@ -6242,12 +6132,12 @@
       <c r="A26" s="19"/>
       <c r="B26" s="18"/>
       <c r="C26" s="77"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
       <c r="G26" s="18"/>
       <c r="H26" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I26" s="56">
         <f>SUM(I24:I25)</f>
@@ -6337,16 +6227,16 @@
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="75" t="s">
-        <v>155</v>
-      </c>
-      <c r="D31" s="76"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="76"/>
+        <v>88</v>
+      </c>
+      <c r="C31" s="69" t="s">
+        <v>152</v>
+      </c>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
       <c r="G31" s="40" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H31" s="40"/>
       <c r="I31" s="48">
@@ -6356,16 +6246,16 @@
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
       <c r="B32" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" s="73" t="s">
-        <v>157</v>
-      </c>
-      <c r="D32" s="74"/>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
+        <v>89</v>
+      </c>
+      <c r="C32" s="71" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" s="72"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="72"/>
       <c r="G32" s="46" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H32" s="46"/>
       <c r="I32" s="47">
@@ -6381,7 +6271,7 @@
       <c r="F33" s="19"/>
       <c r="G33" s="18"/>
       <c r="H33" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I33" s="56">
         <f>SUM(I31:I32)</f>
@@ -6460,16 +6350,16 @@
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
       <c r="B37" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="75" t="s">
-        <v>156</v>
-      </c>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="76"/>
+        <v>90</v>
+      </c>
+      <c r="C37" s="69" t="s">
+        <v>153</v>
+      </c>
+      <c r="D37" s="70"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
       <c r="G37" s="40" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H37" s="40"/>
       <c r="I37" s="48">
@@ -6479,16 +6369,16 @@
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19"/>
       <c r="B38" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" s="73" t="s">
-        <v>161</v>
-      </c>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="74"/>
+        <v>91</v>
+      </c>
+      <c r="C38" s="71" t="s">
+        <v>158</v>
+      </c>
+      <c r="D38" s="72"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="72"/>
       <c r="G38" s="46" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H38" s="46"/>
       <c r="I38" s="47">
@@ -6498,13 +6388,13 @@
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
       <c r="B39" s="18"/>
-      <c r="C39" s="69"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="69"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="73"/>
       <c r="G39" s="18"/>
       <c r="H39" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I39" s="56">
         <f>SUM(I37:I38)</f>
@@ -6517,7 +6407,7 @@
     <row r="41" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A41" s="19"/>
       <c r="H41" s="51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I41" s="51">
         <f>I6+I13+I20+I26+I33+I39</f>
@@ -6599,9 +6489,7 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="C26:F26"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C5:F5"/>
@@ -6614,9 +6502,11 @@
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C26:F26"/>
     <mergeCell ref="C31:F31"/>
     <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6628,7 +6518,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6701,16 +6591,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="75" t="s">
-        <v>158</v>
-      </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
+        <v>92</v>
+      </c>
+      <c r="C4" s="69" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
       <c r="G4" s="40" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H4" s="40"/>
       <c r="I4" s="48">
@@ -6719,16 +6609,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="71" t="s">
-        <v>160</v>
-      </c>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
+        <v>93</v>
+      </c>
+      <c r="C5" s="75" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
       <c r="G5" s="43" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H5" s="43"/>
       <c r="I5" s="44">
@@ -6737,16 +6627,16 @@
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>162</v>
-      </c>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
+        <v>94</v>
+      </c>
+      <c r="C6" s="71" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
       <c r="G6" s="46" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H6" s="46"/>
       <c r="I6" s="47">
@@ -6761,7 +6651,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I7" s="56">
         <f>SUM(I4:I6)</f>
@@ -6836,16 +6726,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="75" t="s">
-        <v>163</v>
-      </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
+        <v>95</v>
+      </c>
+      <c r="C11" s="69" t="s">
+        <v>160</v>
+      </c>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
       <c r="G11" s="40" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H11" s="40"/>
       <c r="I11" s="48">
@@ -6854,16 +6744,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" s="71" t="s">
-        <v>164</v>
-      </c>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
+        <v>96</v>
+      </c>
+      <c r="C12" s="75" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
       <c r="G12" s="43" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H12" s="43"/>
       <c r="I12" s="44">
@@ -6872,16 +6762,16 @@
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="C13" s="73" t="s">
-        <v>165</v>
-      </c>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
+        <v>97</v>
+      </c>
+      <c r="C13" s="71" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
       <c r="G13" s="46" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H13" s="46"/>
       <c r="I13" s="47">
@@ -6890,7 +6780,7 @@
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H14" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I14" s="56">
         <f>SUM(I11:I13)</f>
@@ -6935,7 +6825,7 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>42</v>
@@ -6977,14 +6867,14 @@
       <c r="B19" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="C19" s="75" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
+      <c r="C19" s="69" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
       <c r="G19" s="57" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H19" s="57"/>
       <c r="I19" s="48">
@@ -6996,13 +6886,13 @@
         <v>176</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D20" s="59"/>
       <c r="E20" s="59"/>
       <c r="F20" s="59"/>
       <c r="G20" s="59" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H20" s="59"/>
       <c r="I20" s="47">
@@ -7011,13 +6901,13 @@
     </row>
     <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="60"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
       <c r="G21" s="60"/>
       <c r="H21" s="54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I21" s="55">
         <f>SUM(I19:I20)</f>
@@ -7062,7 +6952,7 @@
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="20" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>42</v>
@@ -7102,16 +6992,16 @@
     </row>
     <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="75" t="s">
-        <v>168</v>
-      </c>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
+        <v>172</v>
+      </c>
+      <c r="C26" s="69" t="s">
+        <v>165</v>
+      </c>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
       <c r="G26" s="57" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H26" s="57"/>
       <c r="I26" s="48">
@@ -7120,16 +7010,16 @@
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="C27" s="75" t="s">
-        <v>170</v>
-      </c>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
+        <v>173</v>
+      </c>
+      <c r="C27" s="69" t="s">
+        <v>167</v>
+      </c>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
       <c r="G27" s="58" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H27" s="58"/>
       <c r="I27" s="44">
@@ -7140,14 +7030,14 @@
       <c r="B28" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="C28" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
+      <c r="C28" s="71" t="s">
+        <v>166</v>
+      </c>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
       <c r="G28" s="59" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H28" s="59"/>
       <c r="I28" s="47">
@@ -7158,14 +7048,14 @@
       <c r="B29" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="73" t="s">
-        <v>171</v>
-      </c>
-      <c r="D29" s="73"/>
-      <c r="E29" s="73"/>
-      <c r="F29" s="73"/>
+      <c r="C29" s="71" t="s">
+        <v>168</v>
+      </c>
+      <c r="D29" s="71"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="71"/>
       <c r="G29" s="59" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H29" s="59"/>
       <c r="I29" s="47">
@@ -7174,7 +7064,7 @@
     </row>
     <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H30" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I30" s="53">
         <f>SUM(I26:I29)</f>
@@ -7183,7 +7073,7 @@
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H31" s="50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I31" s="50">
         <f>I14+I7+I21+I30</f>
@@ -7214,7 +7104,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7261,7 +7151,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -7273,7 +7163,7 @@
       </c>
       <c r="B6" s="3">
         <f>B4-B5</f>
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -7291,7 +7181,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="8">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -7303,7 +7193,7 @@
       </c>
       <c r="B9" s="3">
         <f>(B4-B5)*B8*B7*8</f>
-        <v>368</v>
+        <v>160</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -7313,7 +7203,7 @@
       </c>
       <c r="B10" s="3">
         <f>IFERROR(B9/B4,0)</f>
-        <v>16</v>
+        <v>6.9565217391304346</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -7351,8 +7241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7370,7 +7260,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5">
-        <v>44584</v>
+        <v>44585</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>19</v>
@@ -7429,7 +7319,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="8">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -7441,7 +7331,7 @@
       </c>
       <c r="B9" s="3">
         <f>(B4-B5)*B8*B7*8</f>
-        <v>352</v>
+        <v>70.400000000000006</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -7451,7 +7341,7 @@
       </c>
       <c r="B10" s="3">
         <f>IFERROR(B9/B4,0)</f>
-        <v>16</v>
+        <v>3.2</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -7487,10 +7377,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G14"/>
+  <dimension ref="A2:G17"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7537,16 +7427,20 @@
         <v>1</v>
       </c>
       <c r="C3" s="11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="11"/>
+        <v>80</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>146</v>
+      </c>
       <c r="F3" s="11">
-        <v>6</v>
-      </c>
-      <c r="G3" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
@@ -7557,16 +7451,20 @@
         <v>2</v>
       </c>
       <c r="C4" s="11">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="11"/>
+        <v>99</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>139</v>
+      </c>
       <c r="F4" s="11">
-        <v>8</v>
-      </c>
-      <c r="G4" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
@@ -7577,16 +7475,20 @@
         <v>3</v>
       </c>
       <c r="C5" s="11">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="11"/>
+        <v>81</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>141</v>
+      </c>
       <c r="F5" s="11">
-        <v>11</v>
-      </c>
-      <c r="G5" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
@@ -7597,17 +7499,20 @@
         <v>4</v>
       </c>
       <c r="C6" s="11">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="11"/>
+        <v>82</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>139</v>
+      </c>
       <c r="F6" s="11">
-        <f>SprintBacklog[[#This Row],[Estimated Hours]]</f>
-        <v>10</v>
-      </c>
-      <c r="G6" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
@@ -7618,17 +7523,20 @@
         <v>5</v>
       </c>
       <c r="C7" s="11">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="11"/>
+        <v>98</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="F7" s="11">
-        <f>SprintBacklog[[#This Row],[Estimated Hours]]</f>
-        <v>10</v>
-      </c>
-      <c r="G7" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
@@ -7639,81 +7547,96 @@
         <v>6</v>
       </c>
       <c r="C8" s="11">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="11"/>
+        <v>84</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>148</v>
+      </c>
       <c r="F8" s="11">
-        <v>12</v>
-      </c>
-      <c r="G8" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C9" s="11">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="11"/>
+        <v>85</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>141</v>
+      </c>
       <c r="F9" s="11">
-        <v>14</v>
-      </c>
-      <c r="G9" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C10" s="11">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="11"/>
+        <v>83</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>139</v>
+      </c>
       <c r="F10" s="11">
-        <v>15</v>
-      </c>
-      <c r="G10" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C11" s="11">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="11"/>
+        <v>86</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="F11" s="11">
-        <f>SprintBacklog[[#This Row],[Estimated Hours]]</f>
-        <v>20</v>
-      </c>
-      <c r="G11" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="3">
         <f t="shared" si="0"/>
@@ -7723,55 +7646,136 @@
         <v>8</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="11"/>
+        <v>87</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>146</v>
+      </c>
       <c r="F12" s="11">
         <v>8</v>
       </c>
-      <c r="G12" s="11"/>
+      <c r="G12" s="11" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="65">
         <f>IFERROR(B12+1,1)</f>
         <v>11</v>
       </c>
       <c r="C13" s="66">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="67"/>
+        <v>88</v>
+      </c>
+      <c r="E13" s="67" t="s">
+        <v>139</v>
+      </c>
       <c r="F13" s="64">
+        <v>4</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="64">
+        <v>1</v>
+      </c>
+      <c r="B14" s="65">
+        <f t="shared" ref="B14:B15" si="1">IFERROR(B13+1,1)</f>
+        <v>12</v>
+      </c>
+      <c r="C14" s="66">
+        <v>6</v>
+      </c>
+      <c r="D14" s="64" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" s="67" t="s">
+        <v>144</v>
+      </c>
+      <c r="F14" s="64">
+        <v>6</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="64">
+        <v>1</v>
+      </c>
+      <c r="B15" s="65">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C15" s="66">
+        <v>5</v>
+      </c>
+      <c r="D15" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="67" t="s">
+        <v>141</v>
+      </c>
+      <c r="F15" s="64">
         <f>SprintBacklog[[#This Row],[Estimated Hours]]</f>
-        <v>10</v>
-      </c>
-      <c r="G13" s="67"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="64">
+        <v>1</v>
+      </c>
+      <c r="B16" s="65">
+        <f t="shared" ref="B16" si="2">IFERROR(B15+1,1)</f>
+        <v>14</v>
+      </c>
+      <c r="C16" s="66">
+        <v>7</v>
+      </c>
+      <c r="D16" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="67" t="s">
+        <v>148</v>
+      </c>
+      <c r="F16" s="64">
+        <f>SprintBacklog[[#This Row],[Estimated Hours]]</f>
+        <v>7</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68">
+      <c r="B17" s="68"/>
+      <c r="C17" s="68">
         <f>SUBTOTAL(109,SprintBacklog[Estimated Hours])</f>
-        <v>124</v>
-      </c>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68">
+        <v>57</v>
+      </c>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68">
         <f>SUBTOTAL(109,SprintBacklog[Remaining Hours])</f>
-        <v>124</v>
-      </c>
-      <c r="G14" s="68"/>
+        <v>57</v>
+      </c>
+      <c r="G17" s="68"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G16">
       <formula1>"In Progress, Completed, Blocked"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7784,10 +7788,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E26"/>
+  <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7818,15 +7822,15 @@
       </c>
       <c r="B3" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="C3" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="D3" s="15">
         <f>Table3[[#This Row],[Target Burn Down]]</f>
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="E3" s="15"/>
     </row>
@@ -7836,14 +7840,14 @@
       </c>
       <c r="B4" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>118.60869565217391</v>
+        <v>54.15</v>
       </c>
       <c r="C4" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>108</v>
+        <v>50.043478260869563</v>
       </c>
       <c r="D4" s="16">
-        <v>170</v>
+        <v>57</v>
       </c>
       <c r="E4" s="15"/>
     </row>
@@ -7853,14 +7857,14 @@
       </c>
       <c r="B5" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>113.21739130434783</v>
+        <v>51.3</v>
       </c>
       <c r="C5" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>92</v>
+        <v>43.086956521739133</v>
       </c>
       <c r="D5" s="16">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="E5" s="15"/>
     </row>
@@ -7870,14 +7874,14 @@
       </c>
       <c r="B6" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>107.82608695652173</v>
+        <v>48.45</v>
       </c>
       <c r="C6" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>76</v>
+        <v>36.130434782608695</v>
       </c>
       <c r="D6" s="16">
-        <v>110</v>
+        <v>57</v>
       </c>
       <c r="E6" s="15"/>
     </row>
@@ -7887,14 +7891,14 @@
       </c>
       <c r="B7" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>102.43478260869566</v>
+        <v>45.6</v>
       </c>
       <c r="C7" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>60</v>
+        <v>29.173913043478262</v>
       </c>
       <c r="D7" s="16">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="E7" s="15"/>
     </row>
@@ -7904,14 +7908,14 @@
       </c>
       <c r="B8" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>97.043478260869563</v>
+        <v>42.75</v>
       </c>
       <c r="C8" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>44</v>
+        <v>22.217391304347828</v>
       </c>
       <c r="D8" s="16">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="E8" s="15"/>
     </row>
@@ -7921,14 +7925,14 @@
       </c>
       <c r="B9" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>91.65217391304347</v>
+        <v>39.9</v>
       </c>
       <c r="C9" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>28</v>
+        <v>15.260869565217391</v>
       </c>
       <c r="D9" s="16">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E9" s="15"/>
     </row>
@@ -7938,14 +7942,14 @@
       </c>
       <c r="B10" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>86.260869565217391</v>
+        <v>37.049999999999997</v>
       </c>
       <c r="C10" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>12</v>
+        <v>8.3043478260869605</v>
       </c>
       <c r="D10" s="16">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="E10" s="15"/>
     </row>
@@ -7955,14 +7959,14 @@
       </c>
       <c r="B11" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>80.869565217391312</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="C11" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-4</v>
+        <v>1.3478260869565233</v>
       </c>
       <c r="D11" s="16">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E11" s="15"/>
     </row>
@@ -7972,14 +7976,14 @@
       </c>
       <c r="B12" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>75.478260869565219</v>
+        <v>31.349999999999998</v>
       </c>
       <c r="C12" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-20</v>
+        <v>-5.608695652173914</v>
       </c>
       <c r="D12" s="16">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="E12" s="15"/>
     </row>
@@ -7989,14 +7993,14 @@
       </c>
       <c r="B13" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>70.086956521739125</v>
+        <v>28.5</v>
       </c>
       <c r="C13" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-36</v>
+        <v>-12.565217391304344</v>
       </c>
       <c r="D13" s="16">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="E13" s="15"/>
     </row>
@@ -8006,14 +8010,14 @@
       </c>
       <c r="B14" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>64.695652173913047</v>
+        <v>25.65</v>
       </c>
       <c r="C14" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-52</v>
+        <v>-19.521739130434781</v>
       </c>
       <c r="D14" s="16">
-        <v>11</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -8022,14 +8026,14 @@
       </c>
       <c r="B15" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>59.304347826086953</v>
+        <v>22.799999999999997</v>
       </c>
       <c r="C15" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-68</v>
+        <v>-26.478260869565219</v>
       </c>
       <c r="D15" s="16">
-        <v>12</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -8038,14 +8042,14 @@
       </c>
       <c r="B16" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>53.913043478260875</v>
+        <v>19.949999999999996</v>
       </c>
       <c r="C16" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-84</v>
+        <v>-33.434782608695656</v>
       </c>
       <c r="D16" s="16">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -8054,14 +8058,14 @@
       </c>
       <c r="B17" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>48.521739130434781</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="C17" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-100</v>
+        <v>-40.391304347826079</v>
       </c>
       <c r="D17" s="16">
-        <v>14</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -8070,14 +8074,14 @@
       </c>
       <c r="B18" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>43.130434782608702</v>
+        <v>14.25</v>
       </c>
       <c r="C18" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-116</v>
+        <v>-47.347826086956516</v>
       </c>
       <c r="D18" s="16">
-        <v>15</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -8086,14 +8090,14 @@
       </c>
       <c r="B19" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>37.739130434782609</v>
+        <v>11.399999999999999</v>
       </c>
       <c r="C19" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-132</v>
+        <v>-54.304347826086953</v>
       </c>
       <c r="D19" s="16">
-        <v>16</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -8102,14 +8106,14 @@
       </c>
       <c r="B20" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>32.347826086956516</v>
+        <v>8.5499999999999972</v>
       </c>
       <c r="C20" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-148</v>
+        <v>-61.260869565217391</v>
       </c>
       <c r="D20" s="16">
-        <v>17</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -8118,14 +8122,14 @@
       </c>
       <c r="B21" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>26.956521739130437</v>
+        <v>5.6999999999999957</v>
       </c>
       <c r="C21" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-164</v>
+        <v>-68.217391304347828</v>
       </c>
       <c r="D21" s="16">
-        <v>18</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -8134,14 +8138,14 @@
       </c>
       <c r="B22" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>21.565217391304344</v>
+        <v>2.8500000000000014</v>
       </c>
       <c r="C22" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-180</v>
+        <v>-75.173913043478251</v>
       </c>
       <c r="D22" s="16">
-        <v>19</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -8150,62 +8154,14 @@
       </c>
       <c r="B23" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>16.173913043478265</v>
+        <v>0</v>
       </c>
       <c r="C23" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-196</v>
+        <v>-82.130434782608688</v>
       </c>
       <c r="D23" s="16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
-        <v>21</v>
-      </c>
-      <c r="B24" s="15">
-        <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>10.782608695652172</v>
-      </c>
-      <c r="C24" s="15">
-        <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-212</v>
-      </c>
-      <c r="D24" s="16">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="3">
-        <v>22</v>
-      </c>
-      <c r="B25" s="15">
-        <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>5.3913043478260931</v>
-      </c>
-      <c r="C25" s="15">
-        <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-228</v>
-      </c>
-      <c r="D25" s="16">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
-        <v>23</v>
-      </c>
-      <c r="B26" s="15">
-        <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C26" s="15">
-        <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-244</v>
-      </c>
-      <c r="D26" s="16">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -8221,9 +8177,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -8278,16 +8234,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="15">
-        <f>IFERROR(TotalHours-(Table38[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>124</v>
-      </c>
-      <c r="C3" s="15">
-        <f>TotalHours-(Table38[[#This Row],[Work Day]]*DevRate)</f>
-        <v>124</v>
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
       </c>
       <c r="D3" s="15">
         <f>Table38[[#This Row],[Target Burn Down]]</f>
-        <v>124</v>
+        <v>0</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="3"/>
@@ -8307,15 +8263,15 @@
         <v>1</v>
       </c>
       <c r="B4" s="15">
-        <f>IFERROR(TotalHours-(Table38[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>118.60869565217391</v>
-      </c>
-      <c r="C4" s="15">
-        <f>TotalHours-(Table38[[#This Row],[Work Day]]*DevRate)</f>
-        <v>108</v>
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
       </c>
       <c r="D4" s="16">
-        <v>150</v>
+        <v>59</v>
       </c>
       <c r="E4" s="15"/>
       <c r="F4" s="3"/>
@@ -8335,15 +8291,15 @@
         <v>2</v>
       </c>
       <c r="B5" s="15">
-        <f>IFERROR(TotalHours-(Table38[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>113.21739130434783</v>
-      </c>
-      <c r="C5" s="15">
-        <f>TotalHours-(Table38[[#This Row],[Work Day]]*DevRate)</f>
-        <v>92</v>
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
       </c>
       <c r="D5" s="16">
-        <v>120</v>
+        <v>59</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="3"/>
@@ -8363,15 +8319,15 @@
         <v>3</v>
       </c>
       <c r="B6" s="15">
-        <f>IFERROR(TotalHours-(Table38[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>107.82608695652173</v>
-      </c>
-      <c r="C6" s="15">
-        <f>TotalHours-(Table38[[#This Row],[Work Day]]*DevRate)</f>
-        <v>76</v>
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
       </c>
       <c r="D6" s="16">
-        <v>110</v>
+        <v>59</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="3"/>
@@ -8391,15 +8347,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="15">
-        <f>IFERROR(TotalHours-(Table38[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>102.43478260869566</v>
-      </c>
-      <c r="C7" s="15">
-        <f>TotalHours-(Table38[[#This Row],[Work Day]]*DevRate)</f>
-        <v>60</v>
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
       </c>
       <c r="D7" s="16">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="3"/>
@@ -8419,15 +8375,15 @@
         <v>5</v>
       </c>
       <c r="B8" s="15">
-        <f>IFERROR(TotalHours-(Table38[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>97.043478260869563</v>
-      </c>
-      <c r="C8" s="15">
-        <f>TotalHours-(Table38[[#This Row],[Work Day]]*DevRate)</f>
-        <v>44</v>
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
       </c>
       <c r="D8" s="16">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="3"/>
@@ -8447,15 +8403,15 @@
         <v>6</v>
       </c>
       <c r="B9" s="15">
-        <f>IFERROR(TotalHours-(Table38[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>91.65217391304347</v>
-      </c>
-      <c r="C9" s="15">
-        <f>TotalHours-(Table38[[#This Row],[Work Day]]*DevRate)</f>
-        <v>28</v>
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
       </c>
       <c r="D9" s="16">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="3"/>
@@ -8475,15 +8431,15 @@
         <v>7</v>
       </c>
       <c r="B10" s="15">
-        <f>IFERROR(TotalHours-(Table38[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>86.260869565217391</v>
-      </c>
-      <c r="C10" s="15">
-        <f>TotalHours-(Table38[[#This Row],[Work Day]]*DevRate)</f>
-        <v>12</v>
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
       </c>
       <c r="D10" s="16">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="3"/>
@@ -8503,15 +8459,15 @@
         <v>8</v>
       </c>
       <c r="B11" s="15">
-        <f>IFERROR(TotalHours-(Table38[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>80.869565217391312</v>
-      </c>
-      <c r="C11" s="15">
-        <f>TotalHours-(Table38[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-4</v>
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
       </c>
       <c r="D11" s="16">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="3"/>
@@ -8531,15 +8487,15 @@
         <v>9</v>
       </c>
       <c r="B12" s="15">
-        <f>IFERROR(TotalHours-(Table38[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>75.478260869565219</v>
-      </c>
-      <c r="C12" s="15">
-        <f>TotalHours-(Table38[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-20</v>
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
       </c>
       <c r="D12" s="16">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="3"/>
@@ -8559,15 +8515,15 @@
         <v>10</v>
       </c>
       <c r="B13" s="15">
-        <f>IFERROR(TotalHours-(Table38[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>70.086956521739125</v>
-      </c>
-      <c r="C13" s="15">
-        <f>TotalHours-(Table38[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-36</v>
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
       </c>
       <c r="D13" s="16">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="3"/>
@@ -8583,10 +8539,20 @@
       <c r="P13" s="3"/>
     </row>
     <row r="14" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
+      <c r="A14" s="3">
+        <v>11</v>
+      </c>
+      <c r="B14" s="15">
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D14" s="16">
+        <v>59</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -8601,10 +8567,20 @@
       <c r="P14" s="3"/>
     </row>
     <row r="15" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
+      <c r="A15" s="3">
+        <v>12</v>
+      </c>
+      <c r="B15" s="15">
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D15" s="16">
+        <v>59</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -8618,6 +8594,166 @@
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
     </row>
+    <row r="16" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>13</v>
+      </c>
+      <c r="B16" s="15">
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D16" s="16">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>14</v>
+      </c>
+      <c r="B17" s="15">
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D17" s="16">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>15</v>
+      </c>
+      <c r="B18" s="15">
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D18" s="16">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>16</v>
+      </c>
+      <c r="B19" s="15">
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D19" s="16">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>17</v>
+      </c>
+      <c r="B20" s="15">
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D20" s="16">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>18</v>
+      </c>
+      <c r="B21" s="15">
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D21" s="16">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>19</v>
+      </c>
+      <c r="B22" s="15">
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D22" s="16">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>20</v>
+      </c>
+      <c r="B23" s="15">
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C23" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D23" s="16">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>21</v>
+      </c>
+      <c r="B24" s="15">
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D24" s="16">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>22</v>
+      </c>
+      <c r="B25" s="15">
+        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="15" t="e">
+        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D25" s="16">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Se agrego la Backlog2Table, con su respectiva las horas estimadas y los correspondientes nombres
</commit_message>
<xml_diff>
--- a/Excel-Burndown-Chart-Template.xlsx
+++ b/Excel-Burndown-Chart-Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="4" r:id="rId1"/>
@@ -18,16 +18,19 @@
     <sheet name="Sprint1Info" sheetId="2" r:id="rId4"/>
     <sheet name="Sprint2Info" sheetId="7" r:id="rId5"/>
     <sheet name="Backlog1Table" sheetId="1" r:id="rId6"/>
-    <sheet name="BurnDown1Table" sheetId="3" r:id="rId7"/>
-    <sheet name="BurnDown2Table" sheetId="8" r:id="rId8"/>
+    <sheet name="Backlog2Table" sheetId="9" r:id="rId7"/>
+    <sheet name="BurnDown1Table" sheetId="3" r:id="rId8"/>
+    <sheet name="BurnDown2Table" sheetId="8" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="DevRate" localSheetId="4">Sprint2Info!$B$10</definedName>
     <definedName name="DevRate">Sprint1Info!$B$10</definedName>
+    <definedName name="RemainingHours" localSheetId="6">SprintBacklog6[[#Totals],[Remaining Hours]]</definedName>
     <definedName name="RemainingHours" localSheetId="4">SprintBacklog[[#Totals],[Remaining Hours]]</definedName>
     <definedName name="RemainingHours">SprintBacklog[[#Totals],[Remaining Hours]]</definedName>
     <definedName name="StartDate" localSheetId="4">Sprint2Info!$B$2</definedName>
     <definedName name="StartDate">Sprint1Info!$B$2</definedName>
+    <definedName name="TotalHours" localSheetId="6">SprintBacklog6[[#Totals],[Estimated Hours]]</definedName>
     <definedName name="TotalHours" localSheetId="4">SprintBacklog[[#Totals],[Estimated Hours]]</definedName>
     <definedName name="TotalHours">SprintBacklog[[#Totals],[Estimated Hours]]</definedName>
     <definedName name="WorkingDays" localSheetId="4">Sprint2Info!$B$6</definedName>
@@ -120,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="179">
   <si>
     <t>Start Date</t>
   </si>
@@ -1247,23 +1250,410 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="58">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2660,11 +3050,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="236348624"/>
-        <c:axId val="236349016"/>
+        <c:axId val="236507032"/>
+        <c:axId val="236507424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="236348624"/>
+        <c:axId val="236507032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2707,7 +3097,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236349016"/>
+        <c:crossAx val="236507424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2715,7 +3105,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236349016"/>
+        <c:axId val="236507424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2766,7 +3156,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236348624"/>
+        <c:crossAx val="236507032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2892,6 +3282,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3524,11 +3915,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="236349800"/>
-        <c:axId val="236350192"/>
+        <c:axId val="236508208"/>
+        <c:axId val="236508600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="236349800"/>
+        <c:axId val="236508208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3571,7 +3962,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236350192"/>
+        <c:crossAx val="236508600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3579,7 +3970,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236350192"/>
+        <c:axId val="236508600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3630,7 +4021,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236349800"/>
+        <c:crossAx val="236508208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3644,6 +4035,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4816,7 +5208,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4859,7 +5251,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4883,74 +5275,94 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
   <tableColumns count="2">
-    <tableColumn id="1" name="Column1" headerRowDxfId="38" dataDxfId="37"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="36" dataDxfId="35"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="55" dataDxfId="54"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="53" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <tableColumns count="2">
-    <tableColumn id="1" name="Column1" headerRowDxfId="32" dataDxfId="31"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="30" dataDxfId="29"/>
+    <tableColumn id="1" name="Column1" headerRowDxfId="49" dataDxfId="48"/>
+    <tableColumn id="2" name="Column2" headerRowDxfId="47" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SprintBacklog" displayName="SprintBacklog" ref="A2:G17" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SprintBacklog" displayName="SprintBacklog" ref="A2:G17" totalsRowCount="1" headerRowDxfId="45" dataDxfId="44" totalsRowDxfId="43">
   <autoFilter ref="A2:G16"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Sprint" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="2" name="Item ID" dataDxfId="23" totalsRowDxfId="22">
+    <tableColumn id="1" name="Sprint" totalsRowLabel="Total" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="2" name="Item ID" dataDxfId="40" totalsRowDxfId="39">
       <calculatedColumnFormula>IFERROR(B2+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="4" name="Task Name" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="5" name="Assigned To" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="6" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14">
+    <tableColumn id="3" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="4" name="Task Name" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="5" name="Assigned To" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="6" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31">
       <calculatedColumnFormula>SprintBacklog[[#This Row],[Estimated Hours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Status" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="7" name="Status" dataDxfId="30" totalsRowDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:D23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A2:D23"/>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Work Day" dataDxfId="9"/>
-    <tableColumn id="2" name="Target Burn Down" dataDxfId="8">
-      <calculatedColumnFormula>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="SprintBacklog6" displayName="SprintBacklog6" ref="A2:G15" totalsRowCount="1" headerRowDxfId="16" dataDxfId="15" totalsRowDxfId="14">
+  <autoFilter ref="A2:G14"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Sprint" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="6"/>
+    <tableColumn id="2" name="Item ID" dataDxfId="12" totalsRowDxfId="5">
+      <calculatedColumnFormula>IFERROR(B2+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="7">
-      <calculatedColumnFormula>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</calculatedColumnFormula>
+    <tableColumn id="3" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="4"/>
+    <tableColumn id="4" name="Task Name" dataDxfId="10" totalsRowDxfId="3"/>
+    <tableColumn id="5" name="Assigned To" dataDxfId="9" totalsRowDxfId="2"/>
+    <tableColumn id="6" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="1">
+      <calculatedColumnFormula>SprintBacklog6[[#This Row],[Estimated Hours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Actual Burn Down" dataDxfId="6"/>
+    <tableColumn id="7" name="Status" dataDxfId="7" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table38" displayName="Table38" ref="A2:D25" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:D23" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+  <autoFilter ref="A2:D23"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Work Day" dataDxfId="26"/>
+    <tableColumn id="2" name="Target Burn Down" dataDxfId="25">
+      <calculatedColumnFormula>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="24">
+      <calculatedColumnFormula>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Actual Burn Down" dataDxfId="23"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table38" displayName="Table38" ref="A2:D25" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A2:D25"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Work Day" dataDxfId="3"/>
-    <tableColumn id="2" name="Target Burn Down" dataDxfId="2">
+    <tableColumn id="1" name="Work Day" dataDxfId="20"/>
+    <tableColumn id="2" name="Target Burn Down" dataDxfId="19">
       <calculatedColumnFormula>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="1">
+    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="18">
       <calculatedColumnFormula>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Actual Burn Down" dataDxfId="0"/>
+    <tableColumn id="4" name="Actual Burn Down" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5688,12 +6100,12 @@
       <c r="B4" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="72" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
       <c r="G4" s="43" t="s">
         <v>146</v>
       </c>
@@ -5707,12 +6119,12 @@
       <c r="B5" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="71" t="s">
+      <c r="C5" s="74" t="s">
         <v>145</v>
       </c>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
       <c r="G5" s="46" t="s">
         <v>139</v>
       </c>
@@ -5724,10 +6136,10 @@
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
       <c r="G6" s="18"/>
       <c r="H6" s="52" t="s">
         <v>79</v>
@@ -5811,12 +6223,12 @@
       <c r="B10" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="69" t="s">
+      <c r="C10" s="76" t="s">
         <v>140</v>
       </c>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
       <c r="G10" s="40" t="s">
         <v>141</v>
       </c>
@@ -5830,12 +6242,12 @@
       <c r="B11" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
       <c r="G11" s="43" t="s">
         <v>139</v>
       </c>
@@ -5849,12 +6261,12 @@
       <c r="B12" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="C12" s="71" t="s">
+      <c r="C12" s="74" t="s">
         <v>143</v>
       </c>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
       <c r="G12" s="46" t="s">
         <v>144</v>
       </c>
@@ -5866,10 +6278,10 @@
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
       <c r="G13" s="18"/>
       <c r="H13" s="52" t="s">
         <v>79</v>
@@ -5953,12 +6365,12 @@
       <c r="B17" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="69" t="s">
+      <c r="C17" s="76" t="s">
         <v>147</v>
       </c>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
       <c r="G17" s="40" t="s">
         <v>148</v>
       </c>
@@ -5972,12 +6384,12 @@
       <c r="B18" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="75" t="s">
+      <c r="C18" s="72" t="s">
         <v>149</v>
       </c>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
       <c r="G18" s="43" t="s">
         <v>141</v>
       </c>
@@ -5991,12 +6403,12 @@
       <c r="B19" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="71" t="s">
+      <c r="C19" s="74" t="s">
         <v>150</v>
       </c>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
+      <c r="D19" s="75"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="75"/>
       <c r="G19" s="46" t="s">
         <v>139</v>
       </c>
@@ -6095,12 +6507,12 @@
       <c r="B24" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="69" t="s">
+      <c r="C24" s="76" t="s">
         <v>151</v>
       </c>
-      <c r="D24" s="70"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="70"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
       <c r="G24" s="40" t="s">
         <v>144</v>
       </c>
@@ -6114,12 +6526,12 @@
       <c r="B25" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="74" t="s">
+      <c r="C25" s="71" t="s">
         <v>170</v>
       </c>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
       <c r="G25" s="46" t="s">
         <v>146</v>
       </c>
@@ -6131,10 +6543,10 @@
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
       <c r="G26" s="18"/>
       <c r="H26" s="52" t="s">
         <v>79</v>
@@ -6229,12 +6641,12 @@
       <c r="B31" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="69" t="s">
+      <c r="C31" s="76" t="s">
         <v>152</v>
       </c>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
       <c r="G31" s="40" t="s">
         <v>139</v>
       </c>
@@ -6248,12 +6660,12 @@
       <c r="B32" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="71" t="s">
+      <c r="C32" s="74" t="s">
         <v>154</v>
       </c>
-      <c r="D32" s="72"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="72"/>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
       <c r="G32" s="46" t="s">
         <v>144</v>
       </c>
@@ -6352,12 +6764,12 @@
       <c r="B37" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="69" t="s">
+      <c r="C37" s="76" t="s">
         <v>153</v>
       </c>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="77"/>
       <c r="G37" s="40" t="s">
         <v>141</v>
       </c>
@@ -6371,12 +6783,12 @@
       <c r="B38" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="71" t="s">
+      <c r="C38" s="74" t="s">
         <v>158</v>
       </c>
-      <c r="D38" s="72"/>
-      <c r="E38" s="72"/>
-      <c r="F38" s="72"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="75"/>
+      <c r="F38" s="75"/>
       <c r="G38" s="46" t="s">
         <v>148</v>
       </c>
@@ -6388,10 +6800,10 @@
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
       <c r="B39" s="18"/>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="73"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="70"/>
       <c r="G39" s="18"/>
       <c r="H39" s="52" t="s">
         <v>79</v>
@@ -6489,6 +6901,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="C4:F4"/>
@@ -6502,11 +6919,6 @@
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6593,12 +7005,12 @@
       <c r="B4" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="76" t="s">
         <v>155</v>
       </c>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
       <c r="G4" s="40" t="s">
         <v>156</v>
       </c>
@@ -6611,12 +7023,12 @@
       <c r="B5" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="72" t="s">
         <v>157</v>
       </c>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
       <c r="G5" s="43" t="s">
         <v>146</v>
       </c>
@@ -6629,12 +7041,12 @@
       <c r="B6" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="71" t="s">
+      <c r="C6" s="74" t="s">
         <v>159</v>
       </c>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="46" t="s">
         <v>144</v>
       </c>
@@ -6728,12 +7140,12 @@
       <c r="B11" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="76" t="s">
         <v>160</v>
       </c>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
       <c r="G11" s="40" t="s">
         <v>141</v>
       </c>
@@ -6746,12 +7158,12 @@
       <c r="B12" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="75" t="s">
+      <c r="C12" s="72" t="s">
         <v>161</v>
       </c>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
       <c r="G12" s="43" t="s">
         <v>139</v>
       </c>
@@ -6764,12 +7176,12 @@
       <c r="B13" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="71" t="s">
+      <c r="C13" s="74" t="s">
         <v>162</v>
       </c>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
       <c r="G13" s="46" t="s">
         <v>144</v>
       </c>
@@ -6867,12 +7279,12 @@
       <c r="B19" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="C19" s="69" t="s">
+      <c r="C19" s="76" t="s">
         <v>163</v>
       </c>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="69"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
       <c r="G19" s="57" t="s">
         <v>148</v>
       </c>
@@ -6901,10 +7313,10 @@
     </row>
     <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="60"/>
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
       <c r="G21" s="60"/>
       <c r="H21" s="54" t="s">
         <v>79</v>
@@ -6994,12 +7406,12 @@
       <c r="B26" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="C26" s="69" t="s">
+      <c r="C26" s="76" t="s">
         <v>165</v>
       </c>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="76"/>
       <c r="G26" s="57" t="s">
         <v>156</v>
       </c>
@@ -7012,12 +7424,12 @@
       <c r="B27" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="C27" s="69" t="s">
+      <c r="C27" s="76" t="s">
         <v>167</v>
       </c>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="76"/>
       <c r="G27" s="58" t="s">
         <v>144</v>
       </c>
@@ -7030,12 +7442,12 @@
       <c r="B28" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="C28" s="71" t="s">
+      <c r="C28" s="74" t="s">
         <v>166</v>
       </c>
-      <c r="D28" s="71"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
       <c r="G28" s="59" t="s">
         <v>141</v>
       </c>
@@ -7048,12 +7460,12 @@
       <c r="B29" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="71" t="s">
+      <c r="C29" s="74" t="s">
         <v>168</v>
       </c>
-      <c r="D29" s="71"/>
-      <c r="E29" s="71"/>
-      <c r="F29" s="71"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
       <c r="G29" s="59" t="s">
         <v>169</v>
       </c>
@@ -7082,18 +7494,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C26:F26"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C26:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7787,10 +8199,371 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="9.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" ht="33" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <f>IFERROR(B2+1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="11">
+        <v>7</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="11">
+        <v>7</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <f t="shared" ref="B4:B12" si="0">IFERROR(B3+1,1)</f>
+        <v>2</v>
+      </c>
+      <c r="C4" s="11">
+        <v>3</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F4" s="11">
+        <v>3</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C5" s="11">
+        <v>4</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="F5" s="11">
+        <v>4</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C6" s="11">
+        <v>7</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F6" s="11">
+        <v>7</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C7" s="11">
+        <v>2</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" s="11">
+        <v>2</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C8" s="11">
+        <v>6</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="F8" s="11">
+        <v>6</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C9" s="11">
+        <v>5</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="F9" s="11">
+        <v>5</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="11">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="11">
+        <v>3</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F10" s="11">
+        <v>3</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C11" s="11">
+        <v>8</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11" s="11">
+        <v>8</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="11">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C12" s="11">
+        <v>3</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="F12" s="11">
+        <v>3</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>2</v>
+      </c>
+      <c r="B13" s="65">
+        <f>IFERROR(B12+1,1)</f>
+        <v>11</v>
+      </c>
+      <c r="C13" s="66">
+        <v>1</v>
+      </c>
+      <c r="D13" s="64" t="s">
+        <v>177</v>
+      </c>
+      <c r="E13" s="67" t="s">
+        <v>141</v>
+      </c>
+      <c r="F13" s="64">
+        <v>1</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="11">
+        <v>2</v>
+      </c>
+      <c r="B14" s="65">
+        <f t="shared" ref="B14" si="1">IFERROR(B13+1,1)</f>
+        <v>12</v>
+      </c>
+      <c r="C14" s="66">
+        <v>10</v>
+      </c>
+      <c r="D14" s="64" t="s">
+        <v>178</v>
+      </c>
+      <c r="E14" s="67" t="s">
+        <v>169</v>
+      </c>
+      <c r="F14" s="64">
+        <v>10</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="68" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="68"/>
+      <c r="C15" s="68">
+        <f>SUBTOTAL(109,SprintBacklog6[Estimated Hours])</f>
+        <v>59</v>
+      </c>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68">
+        <f>SUBTOTAL(109,SprintBacklog6[Remaining Hours])</f>
+        <v>59</v>
+      </c>
+      <c r="G15" s="68"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G14">
+      <formula1>"In Progress, Completed, Blocked"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -8175,7 +8948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>

</xml_diff>

<commit_message>
Se arreglaron los problemas con la graficas y se asignaron los valores correspondientes a las mismas
</commit_message>
<xml_diff>
--- a/Excel-Burndown-Chart-Template.xlsx
+++ b/Excel-Burndown-Chart-Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="4" r:id="rId1"/>
@@ -1250,410 +1250,23 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="58">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-      <border outline="0">
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1815,6 +1428,393 @@
         <name val="Segoe UI Light"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2411,7 +2411,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Burn Down</a:t>
+              <a:t> 1 Burn Down</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -3050,11 +3050,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="236507032"/>
-        <c:axId val="236507424"/>
+        <c:axId val="237257144"/>
+        <c:axId val="237257536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="236507032"/>
+        <c:axId val="237257144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3097,7 +3097,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236507424"/>
+        <c:crossAx val="237257536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3105,7 +3105,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236507424"/>
+        <c:axId val="237257536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3156,7 +3156,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236507032"/>
+        <c:crossAx val="237257144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3271,14 +3271,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Sprint</a:t>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Sprint 2 Burn Down</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Burn Down</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3323,7 +3323,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BurnDown1Table!$B$2</c:f>
+              <c:f>BurnDown2Table!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3358,10 +3358,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BurnDown1Table!$A$3:$A$23</c:f>
+              <c:f>BurnDown2Table!$A$3:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3424,95 +3424,102 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BurnDown1Table!$B$3:$B$23</c:f>
+              <c:f>BurnDown2Table!$B$3:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54.15</c:v>
+                  <c:v>56.31818181818182</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51.3</c:v>
+                  <c:v>53.63636363636364</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48.45</c:v>
+                  <c:v>50.954545454545453</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.6</c:v>
+                  <c:v>48.272727272727273</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42.75</c:v>
+                  <c:v>45.590909090909093</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39.9</c:v>
+                  <c:v>42.909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37.049999999999997</c:v>
+                  <c:v>40.227272727272727</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34.200000000000003</c:v>
+                  <c:v>37.545454545454547</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.349999999999998</c:v>
+                  <c:v>34.863636363636367</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>28.5</c:v>
+                  <c:v>32.181818181818187</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25.65</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>22.799999999999997</c:v>
+                  <c:v>26.81818181818182</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19.949999999999996</c:v>
+                  <c:v>24.13636363636364</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17.100000000000001</c:v>
+                  <c:v>21.454545454545453</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14.25</c:v>
+                  <c:v>18.772727272727273</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.399999999999999</c:v>
+                  <c:v>16.090909090909093</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.5499999999999972</c:v>
+                  <c:v>13.409090909090914</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.6999999999999957</c:v>
+                  <c:v>10.727272727272734</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.8500000000000014</c:v>
+                  <c:v>8.0454545454545467</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>5.3636363636363669</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.681818181818187</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-57AD-4103-AA38-D12E8EA744C5}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>BurnDown1Table!$C$2</c:f>
+              <c:f>BurnDown2Table!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3524,9 +3531,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -3537,15 +3542,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -3553,10 +3554,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BurnDown1Table!$A$3:$A$23</c:f>
+              <c:f>BurnDown2Table!$A$3:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3619,95 +3620,102 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BurnDown1Table!$C$3:$C$23</c:f>
+              <c:f>BurnDown2Table!$C$3:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.043478260869563</c:v>
+                  <c:v>55.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.086956521739133</c:v>
+                  <c:v>52.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.130434782608695</c:v>
+                  <c:v>49.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.173913043478262</c:v>
+                  <c:v>46.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.217391304347828</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.260869565217391</c:v>
+                  <c:v>39.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.3043478260869605</c:v>
+                  <c:v>36.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3478260869565233</c:v>
+                  <c:v>33.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-5.608695652173914</c:v>
+                  <c:v>30.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-12.565217391304344</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-19.521739130434781</c:v>
+                  <c:v>23.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-26.478260869565219</c:v>
+                  <c:v>20.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-33.434782608695656</c:v>
+                  <c:v>17.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-40.391304347826079</c:v>
+                  <c:v>14.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-47.347826086956516</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-54.304347826086953</c:v>
+                  <c:v>7.7999999999999972</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-61.260869565217391</c:v>
+                  <c:v>4.5999999999999943</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-68.217391304347828</c:v>
+                  <c:v>1.3999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-75.173913043478251</c:v>
+                  <c:v>-1.8000000000000043</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-82.130434782608688</c:v>
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-8.2000000000000028</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-11.400000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-57AD-4103-AA38-D12E8EA744C5}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>BurnDown1Table!$D$2</c:f>
+              <c:f>BurnDown2Table!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3719,47 +3727,33 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                <a:prstClr val="black">
-                  <a:alpha val="40000"/>
-                </a:prstClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFC000"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
+              <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>BurnDown1Table!$A$3:$A$23</c:f>
+              <c:f>BurnDown2Table!$A$3:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3822,88 +3816,95 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BurnDown1Table!$D$3:$D$23</c:f>
+              <c:f>BurnDown2Table!$D$3:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-57AD-4103-AA38-D12E8EA744C5}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3915,11 +3916,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="236508208"/>
-        <c:axId val="236508600"/>
+        <c:axId val="390160960"/>
+        <c:axId val="390160568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="236508208"/>
+        <c:axId val="390160960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3962,7 +3963,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236508600"/>
+        <c:crossAx val="390160568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3970,7 +3971,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236508600"/>
+        <c:axId val="390160568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4021,7 +4022,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236508208"/>
+        <c:crossAx val="390160960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4034,7 +4035,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -5208,7 +5209,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5236,28 +5237,20 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>200024</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -5315,54 +5308,54 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="SprintBacklog6" displayName="SprintBacklog6" ref="A2:G15" totalsRowCount="1" headerRowDxfId="16" dataDxfId="15" totalsRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="SprintBacklog6" displayName="SprintBacklog6" ref="A2:G15" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
   <autoFilter ref="A2:G14"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Sprint" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="6"/>
-    <tableColumn id="2" name="Item ID" dataDxfId="12" totalsRowDxfId="5">
+    <tableColumn id="1" name="Sprint" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" name="Item ID" dataDxfId="23" totalsRowDxfId="22">
       <calculatedColumnFormula>IFERROR(B2+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="4"/>
-    <tableColumn id="4" name="Task Name" dataDxfId="10" totalsRowDxfId="3"/>
-    <tableColumn id="5" name="Assigned To" dataDxfId="9" totalsRowDxfId="2"/>
-    <tableColumn id="6" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="1">
+    <tableColumn id="3" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="Task Name" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" name="Assigned To" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula>SprintBacklog6[[#This Row],[Estimated Hours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Status" dataDxfId="7" totalsRowDxfId="0"/>
+    <tableColumn id="7" name="Status" dataDxfId="13" totalsRowDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:D23" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:D23" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A2:D23"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Work Day" dataDxfId="26"/>
-    <tableColumn id="2" name="Target Burn Down" dataDxfId="25">
+    <tableColumn id="1" name="Work Day" dataDxfId="9"/>
+    <tableColumn id="2" name="Target Burn Down" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="24">
+    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="7">
       <calculatedColumnFormula>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Actual Burn Down" dataDxfId="23"/>
+    <tableColumn id="4" name="Actual Burn Down" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table38" displayName="Table38" ref="A2:D25" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table38" displayName="Table38" ref="A2:D25" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A2:D25"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Work Day" dataDxfId="20"/>
-    <tableColumn id="2" name="Target Burn Down" dataDxfId="19">
-      <calculatedColumnFormula>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</calculatedColumnFormula>
+    <tableColumn id="1" name="Work Day" dataDxfId="3"/>
+    <tableColumn id="2" name="Target Burn Down" dataDxfId="2">
+      <calculatedColumnFormula>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="18">
-      <calculatedColumnFormula>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</calculatedColumnFormula>
+    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="1">
+      <calculatedColumnFormula>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Actual Burn Down" dataDxfId="17"/>
+    <tableColumn id="4" name="Actual Burn Down" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5633,7 +5626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -6100,12 +6093,12 @@
       <c r="B4" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="76" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
       <c r="G4" s="43" t="s">
         <v>146</v>
       </c>
@@ -6119,12 +6112,12 @@
       <c r="B5" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="74" t="s">
+      <c r="C5" s="71" t="s">
         <v>145</v>
       </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
       <c r="G5" s="46" t="s">
         <v>139</v>
       </c>
@@ -6136,10 +6129,10 @@
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
       <c r="G6" s="18"/>
       <c r="H6" s="52" t="s">
         <v>79</v>
@@ -6223,12 +6216,12 @@
       <c r="B10" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="76" t="s">
+      <c r="C10" s="69" t="s">
         <v>140</v>
       </c>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
       <c r="G10" s="40" t="s">
         <v>141</v>
       </c>
@@ -6242,12 +6235,12 @@
       <c r="B11" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="72" t="s">
+      <c r="C11" s="76" t="s">
         <v>142</v>
       </c>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="73"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
       <c r="G11" s="43" t="s">
         <v>139</v>
       </c>
@@ -6261,12 +6254,12 @@
       <c r="B12" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="C12" s="74" t="s">
+      <c r="C12" s="71" t="s">
         <v>143</v>
       </c>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="72"/>
       <c r="G12" s="46" t="s">
         <v>144</v>
       </c>
@@ -6278,10 +6271,10 @@
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="70"/>
-      <c r="D13" s="70"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="70"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
       <c r="G13" s="18"/>
       <c r="H13" s="52" t="s">
         <v>79</v>
@@ -6365,12 +6358,12 @@
       <c r="B17" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="76" t="s">
+      <c r="C17" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
       <c r="G17" s="40" t="s">
         <v>148</v>
       </c>
@@ -6384,12 +6377,12 @@
       <c r="B18" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="72" t="s">
+      <c r="C18" s="76" t="s">
         <v>149</v>
       </c>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="73"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="77"/>
       <c r="G18" s="43" t="s">
         <v>141</v>
       </c>
@@ -6403,12 +6396,12 @@
       <c r="B19" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="74" t="s">
+      <c r="C19" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
       <c r="G19" s="46" t="s">
         <v>139</v>
       </c>
@@ -6507,12 +6500,12 @@
       <c r="B24" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="C24" s="76" t="s">
+      <c r="C24" s="69" t="s">
         <v>151</v>
       </c>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
       <c r="G24" s="40" t="s">
         <v>144</v>
       </c>
@@ -6526,12 +6519,12 @@
       <c r="B25" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="71" t="s">
+      <c r="C25" s="75" t="s">
         <v>170</v>
       </c>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
+      <c r="D25" s="75"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
       <c r="G25" s="46" t="s">
         <v>146</v>
       </c>
@@ -6543,10 +6536,10 @@
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
       <c r="G26" s="18"/>
       <c r="H26" s="52" t="s">
         <v>79</v>
@@ -6641,12 +6634,12 @@
       <c r="B31" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="76" t="s">
+      <c r="C31" s="69" t="s">
         <v>152</v>
       </c>
-      <c r="D31" s="77"/>
-      <c r="E31" s="77"/>
-      <c r="F31" s="77"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
       <c r="G31" s="40" t="s">
         <v>139</v>
       </c>
@@ -6660,12 +6653,12 @@
       <c r="B32" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="74" t="s">
+      <c r="C32" s="71" t="s">
         <v>154</v>
       </c>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
+      <c r="D32" s="72"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="72"/>
       <c r="G32" s="46" t="s">
         <v>144</v>
       </c>
@@ -6764,12 +6757,12 @@
       <c r="B37" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="76" t="s">
+      <c r="C37" s="69" t="s">
         <v>153</v>
       </c>
-      <c r="D37" s="77"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="77"/>
+      <c r="D37" s="70"/>
+      <c r="E37" s="70"/>
+      <c r="F37" s="70"/>
       <c r="G37" s="40" t="s">
         <v>141</v>
       </c>
@@ -6783,12 +6776,12 @@
       <c r="B38" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="74" t="s">
+      <c r="C38" s="71" t="s">
         <v>158</v>
       </c>
-      <c r="D38" s="75"/>
-      <c r="E38" s="75"/>
-      <c r="F38" s="75"/>
+      <c r="D38" s="72"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="72"/>
       <c r="G38" s="46" t="s">
         <v>148</v>
       </c>
@@ -6800,10 +6793,10 @@
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
       <c r="B39" s="18"/>
-      <c r="C39" s="70"/>
-      <c r="D39" s="70"/>
-      <c r="E39" s="70"/>
-      <c r="F39" s="70"/>
+      <c r="C39" s="73"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="73"/>
       <c r="G39" s="18"/>
       <c r="H39" s="52" t="s">
         <v>79</v>
@@ -6901,11 +6894,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="C4:F4"/>
@@ -6919,6 +6907,11 @@
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7005,12 +6998,12 @@
       <c r="B4" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="69" t="s">
         <v>155</v>
       </c>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
       <c r="G4" s="40" t="s">
         <v>156</v>
       </c>
@@ -7023,12 +7016,12 @@
       <c r="B5" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="72" t="s">
+      <c r="C5" s="76" t="s">
         <v>157</v>
       </c>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
       <c r="G5" s="43" t="s">
         <v>146</v>
       </c>
@@ -7041,12 +7034,12 @@
       <c r="B6" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="71" t="s">
         <v>159</v>
       </c>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
       <c r="G6" s="46" t="s">
         <v>144</v>
       </c>
@@ -7140,12 +7133,12 @@
       <c r="B11" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="69" t="s">
         <v>160</v>
       </c>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
       <c r="G11" s="40" t="s">
         <v>141</v>
       </c>
@@ -7158,12 +7151,12 @@
       <c r="B12" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="72" t="s">
+      <c r="C12" s="76" t="s">
         <v>161</v>
       </c>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
       <c r="G12" s="43" t="s">
         <v>139</v>
       </c>
@@ -7176,12 +7169,12 @@
       <c r="B13" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="74" t="s">
+      <c r="C13" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
       <c r="G13" s="46" t="s">
         <v>144</v>
       </c>
@@ -7279,12 +7272,12 @@
       <c r="B19" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="C19" s="76" t="s">
+      <c r="C19" s="69" t="s">
         <v>163</v>
       </c>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
       <c r="G19" s="57" t="s">
         <v>148</v>
       </c>
@@ -7313,10 +7306,10 @@
     </row>
     <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="60"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="76"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
       <c r="G21" s="60"/>
       <c r="H21" s="54" t="s">
         <v>79</v>
@@ -7406,12 +7399,12 @@
       <c r="B26" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="C26" s="76" t="s">
+      <c r="C26" s="69" t="s">
         <v>165</v>
       </c>
-      <c r="D26" s="76"/>
-      <c r="E26" s="76"/>
-      <c r="F26" s="76"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
       <c r="G26" s="57" t="s">
         <v>156</v>
       </c>
@@ -7424,12 +7417,12 @@
       <c r="B27" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="C27" s="76" t="s">
+      <c r="C27" s="69" t="s">
         <v>167</v>
       </c>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="76"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
       <c r="G27" s="58" t="s">
         <v>144</v>
       </c>
@@ -7442,12 +7435,12 @@
       <c r="B28" s="45" t="s">
         <v>177</v>
       </c>
-      <c r="C28" s="74" t="s">
+      <c r="C28" s="71" t="s">
         <v>166</v>
       </c>
-      <c r="D28" s="74"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
       <c r="G28" s="59" t="s">
         <v>141</v>
       </c>
@@ -7460,12 +7453,12 @@
       <c r="B29" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="C29" s="74" t="s">
+      <c r="C29" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="71"/>
       <c r="G29" s="59" t="s">
         <v>169</v>
       </c>
@@ -7494,18 +7487,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8202,7 +8195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -8564,7 +8557,7 @@
   <dimension ref="A2:E23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8976,7 +8969,7 @@
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
     </row>
-    <row r="2" spans="1:16" ht="33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>13</v>
       </c>
@@ -9007,16 +9000,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>59</v>
+      </c>
+      <c r="C3" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>59</v>
       </c>
       <c r="D3" s="15">
         <f>Table38[[#This Row],[Target Burn Down]]</f>
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="3"/>
@@ -9036,12 +9029,12 @@
         <v>1</v>
       </c>
       <c r="B4" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C4" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>56.31818181818182</v>
+      </c>
+      <c r="C4" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>55.8</v>
       </c>
       <c r="D4" s="16">
         <v>59</v>
@@ -9064,12 +9057,12 @@
         <v>2</v>
       </c>
       <c r="B5" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>53.63636363636364</v>
+      </c>
+      <c r="C5" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>52.6</v>
       </c>
       <c r="D5" s="16">
         <v>59</v>
@@ -9092,12 +9085,12 @@
         <v>3</v>
       </c>
       <c r="B6" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>50.954545454545453</v>
+      </c>
+      <c r="C6" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>49.4</v>
       </c>
       <c r="D6" s="16">
         <v>59</v>
@@ -9120,12 +9113,12 @@
         <v>4</v>
       </c>
       <c r="B7" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>48.272727272727273</v>
+      </c>
+      <c r="C7" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>46.2</v>
       </c>
       <c r="D7" s="16">
         <v>59</v>
@@ -9148,12 +9141,12 @@
         <v>5</v>
       </c>
       <c r="B8" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>45.590909090909093</v>
+      </c>
+      <c r="C8" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>43</v>
       </c>
       <c r="D8" s="16">
         <v>59</v>
@@ -9176,12 +9169,12 @@
         <v>6</v>
       </c>
       <c r="B9" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>42.909090909090907</v>
+      </c>
+      <c r="C9" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>39.799999999999997</v>
       </c>
       <c r="D9" s="16">
         <v>59</v>
@@ -9204,12 +9197,12 @@
         <v>7</v>
       </c>
       <c r="B10" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>40.227272727272727</v>
+      </c>
+      <c r="C10" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>36.599999999999994</v>
       </c>
       <c r="D10" s="16">
         <v>59</v>
@@ -9232,12 +9225,12 @@
         <v>8</v>
       </c>
       <c r="B11" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>37.545454545454547</v>
+      </c>
+      <c r="C11" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>33.4</v>
       </c>
       <c r="D11" s="16">
         <v>59</v>
@@ -9260,12 +9253,12 @@
         <v>9</v>
       </c>
       <c r="B12" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C12" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>34.863636363636367</v>
+      </c>
+      <c r="C12" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>30.2</v>
       </c>
       <c r="D12" s="16">
         <v>59</v>
@@ -9288,12 +9281,12 @@
         <v>10</v>
       </c>
       <c r="B13" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C13" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>32.181818181818187</v>
+      </c>
+      <c r="C13" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>27</v>
       </c>
       <c r="D13" s="16">
         <v>59</v>
@@ -9316,12 +9309,12 @@
         <v>11</v>
       </c>
       <c r="B14" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>29.5</v>
+      </c>
+      <c r="C14" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>23.799999999999997</v>
       </c>
       <c r="D14" s="16">
         <v>59</v>
@@ -9344,12 +9337,12 @@
         <v>12</v>
       </c>
       <c r="B15" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>26.81818181818182</v>
+      </c>
+      <c r="C15" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>20.599999999999994</v>
       </c>
       <c r="D15" s="16">
         <v>59</v>
@@ -9372,12 +9365,12 @@
         <v>13</v>
       </c>
       <c r="B16" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>24.13636363636364</v>
+      </c>
+      <c r="C16" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>17.399999999999999</v>
       </c>
       <c r="D16" s="16">
         <v>59</v>
@@ -9388,12 +9381,12 @@
         <v>14</v>
       </c>
       <c r="B17" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C17" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>21.454545454545453</v>
+      </c>
+      <c r="C17" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>14.199999999999996</v>
       </c>
       <c r="D17" s="16">
         <v>59</v>
@@ -9404,12 +9397,12 @@
         <v>15</v>
       </c>
       <c r="B18" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C18" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>18.772727272727273</v>
+      </c>
+      <c r="C18" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>11</v>
       </c>
       <c r="D18" s="16">
         <v>59</v>
@@ -9420,12 +9413,12 @@
         <v>16</v>
       </c>
       <c r="B19" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C19" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>16.090909090909093</v>
+      </c>
+      <c r="C19" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>7.7999999999999972</v>
       </c>
       <c r="D19" s="16">
         <v>59</v>
@@ -9436,12 +9429,12 @@
         <v>17</v>
       </c>
       <c r="B20" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C20" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>13.409090909090914</v>
+      </c>
+      <c r="C20" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>4.5999999999999943</v>
       </c>
       <c r="D20" s="16">
         <v>59</v>
@@ -9452,12 +9445,12 @@
         <v>18</v>
       </c>
       <c r="B21" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C21" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>10.727272727272734</v>
+      </c>
+      <c r="C21" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>1.3999999999999986</v>
       </c>
       <c r="D21" s="16">
         <v>59</v>
@@ -9468,12 +9461,12 @@
         <v>19</v>
       </c>
       <c r="B22" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C22" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>8.0454545454545467</v>
+      </c>
+      <c r="C22" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>-1.8000000000000043</v>
       </c>
       <c r="D22" s="16">
         <v>59</v>
@@ -9484,12 +9477,12 @@
         <v>20</v>
       </c>
       <c r="B23" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C23" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>5.3636363636363669</v>
+      </c>
+      <c r="C23" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>-5</v>
       </c>
       <c r="D23" s="16">
         <v>59</v>
@@ -9500,12 +9493,12 @@
         <v>21</v>
       </c>
       <c r="B24" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
-        <v>0</v>
-      </c>
-      <c r="C24" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
+        <v>2.681818181818187</v>
+      </c>
+      <c r="C24" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>-8.2000000000000028</v>
       </c>
       <c r="D24" s="16">
         <v>59</v>
@@ -9516,12 +9509,12 @@
         <v>22</v>
       </c>
       <c r="B25" s="15">
-        <f>IFERROR(#REF!-(Table38[[#This Row],[Work Day]]*(#REF!/Sprint2Info!WorkingDays)),0)</f>
+        <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
         <v>0</v>
       </c>
-      <c r="C25" s="15" t="e">
-        <f>#REF!-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>#REF!</v>
+      <c r="C25" s="15">
+        <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
+        <v>-11.400000000000006</v>
       </c>
       <c r="D25" s="16">
         <v>59</v>

</xml_diff>

<commit_message>
Corregido documentacion especificacion requerimientos y organizado en carpetas
</commit_message>
<xml_diff>
--- a/Excel-Burndown-Chart-Template.xlsx
+++ b/Excel-Burndown-Chart-Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos de Micha\Tercer Semestre\Proyecto Metodologia\proyectometodologia7342\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emili\Desktop\ProyectoMetodologia\proyectometodologia7342\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4774B8-087C-4A07-AE6C-755C0BC4E6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="4" r:id="rId1"/>
@@ -33,7 +34,7 @@
     <definedName name="WorkingDays" localSheetId="4">Sprint2Info!$B$6</definedName>
     <definedName name="WorkingDays">Sprint1Info!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,9 +42,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -52,12 +51,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>PowerUps for Excel</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -86,12 +85,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>PowerUps for Excel</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
       <text>
         <r>
           <rPr>
@@ -120,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="193">
   <si>
     <t>Start Date</t>
   </si>
@@ -263,9 +262,6 @@
     <t>Alta</t>
   </si>
   <si>
-    <t>Terminado</t>
-  </si>
-  <si>
     <t>Agregar un proveedor</t>
   </si>
   <si>
@@ -353,9 +349,6 @@
     <t>HU11</t>
   </si>
   <si>
-    <t>No iniciado</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -653,17 +646,65 @@
     <t>HU10-2</t>
   </si>
   <si>
-    <t>HU11-3</t>
-  </si>
-  <si>
-    <t>HU11-4</t>
+    <t>Crear formulario de trabajadores</t>
+  </si>
+  <si>
+    <t>Creación, editar, y eliminar trabajadores</t>
+  </si>
+  <si>
+    <t>HU12</t>
+  </si>
+  <si>
+    <t>HU12-1</t>
+  </si>
+  <si>
+    <t>HU12-2</t>
+  </si>
+  <si>
+    <t>Implementar algoritmos de búsqueda</t>
+  </si>
+  <si>
+    <t>Revisión general del programa</t>
+  </si>
+  <si>
+    <t>HU13-1</t>
+  </si>
+  <si>
+    <t>HU13-2</t>
+  </si>
+  <si>
+    <t>HU133</t>
+  </si>
+  <si>
+    <t>HU13-4</t>
+  </si>
+  <si>
+    <t>Buscar ventas y artículos</t>
+  </si>
+  <si>
+    <t>Programa</t>
+  </si>
+  <si>
+    <t>un programa funcional</t>
+  </si>
+  <si>
+    <t>cumplir con las necesidades del negocio</t>
+  </si>
+  <si>
+    <t>Abierto</t>
+  </si>
+  <si>
+    <t>En Revisión</t>
+  </si>
+  <si>
+    <t>Por iniciar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -744,6 +785,12 @@
       <color theme="1"/>
       <name val="Segoe UI Light"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -789,7 +836,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -911,19 +958,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1143,7 +1177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1189,11 +1223,13 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1203,60 +1239,61 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1264,125 +1301,6 @@
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="41">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1548,6 +1466,23 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1578,6 +1513,23 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1617,6 +1569,23 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1647,6 +1616,23 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1686,6 +1672,23 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1719,6 +1722,23 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1734,6 +1754,23 @@
           <color indexed="64"/>
         </right>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1983,7 +2020,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2027,7 +2064,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2053,7 +2089,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-EC"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2264,7 +2300,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -2477,7 +2513,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -2698,7 +2734,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -2758,7 +2794,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="243407728"/>
@@ -2817,7 +2853,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="243407336"/>
@@ -2834,7 +2870,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2860,7 +2895,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-EC"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2890,7 +2925,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-EC"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2902,7 +2937,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2946,7 +2981,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2972,7 +3006,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-EC"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3183,7 +3217,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -3396,7 +3430,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -3617,7 +3651,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -3677,7 +3711,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="244669568"/>
@@ -3736,7 +3770,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="243408512"/>
@@ -3753,7 +3787,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3779,7 +3812,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-EC"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3809,7 +3842,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-EC"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4926,7 +4959,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4969,7 +5002,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4993,74 +5026,74 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <tableColumns count="2">
-    <tableColumn id="1" name="Column1" headerRowDxfId="38" dataDxfId="37"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="36" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" headerRowDxfId="38" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" headerRowDxfId="36" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table25" displayName="Table25" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <tableColumns count="2">
-    <tableColumn id="1" name="Column1" headerRowDxfId="32" dataDxfId="31"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="30" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" headerRowDxfId="32" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column2" headerRowDxfId="30" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SprintBacklog" displayName="SprintBacklog" ref="A2:G14" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
-  <autoFilter ref="A2:G13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="SprintBacklog" displayName="SprintBacklog" ref="A2:G14" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
+  <autoFilter ref="A2:G13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Sprint" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="6"/>
-    <tableColumn id="2" name="Item ID" dataDxfId="24" totalsRowDxfId="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Sprint" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Item ID" dataDxfId="23" totalsRowDxfId="22">
       <calculatedColumnFormula>IFERROR(B2+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="4"/>
-    <tableColumn id="4" name="Task Name" dataDxfId="22" totalsRowDxfId="3"/>
-    <tableColumn id="5" name="Assigned To" dataDxfId="21" totalsRowDxfId="2"/>
-    <tableColumn id="6" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="1">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Task Name" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Assigned To" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula>SprintBacklog[[#This Row],[Estimated Hours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Status" dataDxfId="19" totalsRowDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Status" dataDxfId="13" totalsRowDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:D26" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A2:D26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table3" displayName="Table3" ref="A2:D26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A2:D26" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Work Day" dataDxfId="16"/>
-    <tableColumn id="2" name="Target Burn Down" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Work Day" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Target Burn Down" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Forecast Burn Down" dataDxfId="7">
       <calculatedColumnFormula>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Actual Burn Down" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Actual Burn Down" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table38" displayName="Table38" ref="A2:D13" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A2:D13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table38" displayName="Table38" ref="A2:D13" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A2:D13" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Work Day" dataDxfId="10"/>
-    <tableColumn id="2" name="Target Burn Down" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Work Day" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Target Burn Down" dataDxfId="2">
       <calculatedColumnFormula>IFERROR(TotalHours-(Table38[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="8">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Forecast Burn Down" dataDxfId="1">
       <calculatedColumnFormula>TotalHours-(Table38[[#This Row],[Work Day]]*DevRate)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Actual Burn Down" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Actual Burn Down" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5328,11 +5361,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5343,367 +5376,367 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="35" t="s">
+      <c r="A1" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="31" t="s">
+      <c r="A2" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>103</v>
+      <c r="B3" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G3" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>103</v>
+      <c r="A4" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>103</v>
+      <c r="A5" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G5" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>103</v>
+      <c r="A6" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D6" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="E6" s="24" t="s">
-        <v>126</v>
-      </c>
       <c r="F6" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G6" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>103</v>
+      <c r="A7" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D7" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="E7" s="24" t="s">
-        <v>127</v>
-      </c>
       <c r="F7" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="G9" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="H9" s="28" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>103</v>
+      <c r="B10" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G10" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>103</v>
+      <c r="A11" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G11" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>77</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>103</v>
+      <c r="A12" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>77</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>103</v>
+      <c r="A13" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="F13" s="61" t="s">
-        <v>78</v>
+        <v>131</v>
+      </c>
+      <c r="F13" s="60" t="s">
+        <v>76</v>
       </c>
       <c r="G13" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>77</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" s="62" t="s">
-        <v>116</v>
-      </c>
-      <c r="D14" s="62" t="s">
-        <v>64</v>
+      <c r="A14" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="61" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="61" t="s">
+        <v>63</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="F14" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" s="63" t="s">
-        <v>174</v>
-      </c>
-      <c r="H14" s="29" t="s">
-        <v>77</v>
+        <v>138</v>
+      </c>
+      <c r="F14" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -5712,11 +5745,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5736,16 +5769,16 @@
         <v>36</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>10</v>
@@ -5773,76 +5806,76 @@
         <v>46</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="39" t="s">
+      <c r="H3" s="39"/>
+      <c r="I3" s="40" t="s">
         <v>71</v>
-      </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="71" t="s">
-        <v>141</v>
-      </c>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="43" t="s">
-        <v>149</v>
-      </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="44">
+      <c r="B4" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="76" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="42"/>
+      <c r="I4" s="43">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
-      <c r="B5" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="73" t="s">
-        <v>148</v>
-      </c>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="H5" s="46"/>
-      <c r="I5" s="47">
+      <c r="B5" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" s="45"/>
+      <c r="I5" s="46">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
       <c r="G6" s="18"/>
-      <c r="H6" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I6" s="56">
+      <c r="H6" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="55">
         <f>SUM(I4:I5)</f>
         <v>6</v>
       </c>
@@ -5859,16 +5892,16 @@
         <v>36</v>
       </c>
       <c r="E7" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>10</v>
@@ -5883,108 +5916,108 @@
         <v>42</v>
       </c>
       <c r="D8" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>73</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>74</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20" t="s">
         <v>46</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19"/>
       <c r="B9" s="18"/>
       <c r="C9" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
-      <c r="B10" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="75" t="s">
-        <v>143</v>
-      </c>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="40" t="s">
-        <v>144</v>
-      </c>
-      <c r="H10" s="40"/>
-      <c r="I10" s="48">
+      <c r="B10" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="72" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" s="39"/>
+      <c r="I10" s="47">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
-      <c r="B11" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="71" t="s">
-        <v>145</v>
-      </c>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="43" t="s">
-        <v>142</v>
-      </c>
-      <c r="H11" s="43"/>
-      <c r="I11" s="44">
+      <c r="B11" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="76" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="H11" s="42"/>
+      <c r="I11" s="43">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
-      <c r="B12" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="73" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="H12" s="46"/>
-      <c r="I12" s="49">
+      <c r="B12" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" s="45"/>
+      <c r="I12" s="48">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
       <c r="G13" s="18"/>
-      <c r="H13" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I13" s="56">
+      <c r="H13" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="55">
         <f>SUM(I10:I12)</f>
         <v>8</v>
       </c>
@@ -6001,16 +6034,16 @@
         <v>36</v>
       </c>
       <c r="E14" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>10</v>
@@ -6028,90 +6061,90 @@
         <v>43</v>
       </c>
       <c r="E15" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>49</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>50</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="20" t="s">
         <v>46</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19"/>
       <c r="B16" s="18"/>
       <c r="C16" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
-      <c r="B17" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="75" t="s">
-        <v>150</v>
-      </c>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="40" t="s">
-        <v>151</v>
-      </c>
-      <c r="H17" s="40"/>
-      <c r="I17" s="48">
+      <c r="B17" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="72" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="H17" s="39"/>
+      <c r="I17" s="47">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
-      <c r="B18" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="71" t="s">
-        <v>152</v>
-      </c>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="43" t="s">
-        <v>144</v>
-      </c>
-      <c r="H18" s="43"/>
-      <c r="I18" s="44">
+      <c r="B18" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="76" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="42"/>
+      <c r="I18" s="43">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
-      <c r="B19" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" s="73" t="s">
-        <v>153</v>
-      </c>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="H19" s="46"/>
-      <c r="I19" s="47">
+      <c r="B19" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="74" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19" s="75"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="H19" s="45"/>
+      <c r="I19" s="46">
         <v>6</v>
       </c>
     </row>
@@ -6123,10 +6156,10 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
-      <c r="H20" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I20" s="56">
+      <c r="H20" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I20" s="55">
         <f>SUM(I17:I19)</f>
         <v>11</v>
       </c>
@@ -6143,16 +6176,16 @@
         <v>36</v>
       </c>
       <c r="E21" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I21" s="17" t="s">
         <v>10</v>
@@ -6170,86 +6203,86 @@
         <v>43</v>
       </c>
       <c r="E22" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="20" t="s">
         <v>51</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>52</v>
       </c>
       <c r="G22" s="21"/>
       <c r="H22" s="20" t="s">
         <v>46</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="18"/>
       <c r="C23" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
-      <c r="B24" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="75" t="s">
-        <v>154</v>
-      </c>
-      <c r="D24" s="76"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="H24" s="40"/>
-      <c r="I24" s="48">
+      <c r="B24" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="H24" s="39"/>
+      <c r="I24" s="47">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
-      <c r="B25" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="70" t="s">
-        <v>173</v>
-      </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="46" t="s">
-        <v>149</v>
-      </c>
-      <c r="H25" s="46"/>
-      <c r="I25" s="47">
+      <c r="B25" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="79" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="H25" s="45"/>
+      <c r="I25" s="46">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
       <c r="G26" s="18"/>
-      <c r="H26" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I26" s="56">
+      <c r="H26" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I26" s="55">
         <f>SUM(I24:I25)</f>
         <v>10</v>
       </c>
@@ -6266,16 +6299,16 @@
         <v>36</v>
       </c>
       <c r="E27" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I27" s="17" t="s">
         <v>10</v>
@@ -6293,17 +6326,17 @@
         <v>43</v>
       </c>
       <c r="E28" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="20" t="s">
         <v>53</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>54</v>
       </c>
       <c r="G28" s="21"/>
       <c r="H28" s="20" t="s">
         <v>46</v>
       </c>
       <c r="I28" s="20" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -6321,54 +6354,54 @@
       <c r="A30" s="19"/>
       <c r="B30" s="18"/>
       <c r="C30" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H30" s="18"/>
       <c r="I30" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
-      <c r="B31" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="75" t="s">
-        <v>155</v>
-      </c>
-      <c r="D31" s="76"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="40" t="s">
-        <v>142</v>
-      </c>
-      <c r="H31" s="40"/>
-      <c r="I31" s="48">
+      <c r="B31" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="72" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="H31" s="39"/>
+      <c r="I31" s="47">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
-      <c r="B32" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" s="73" t="s">
-        <v>157</v>
-      </c>
-      <c r="D32" s="74"/>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="H32" s="46"/>
-      <c r="I32" s="47">
+      <c r="B32" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="74" t="s">
+        <v>155</v>
+      </c>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="H32" s="45"/>
+      <c r="I32" s="46">
         <v>6</v>
       </c>
     </row>
@@ -6380,10 +6413,10 @@
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
       <c r="G33" s="18"/>
-      <c r="H33" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I33" s="56">
+      <c r="H33" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I33" s="55">
         <f>SUM(I31:I32)</f>
         <v>10</v>
       </c>
@@ -6400,16 +6433,16 @@
         <v>36</v>
       </c>
       <c r="E34" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I34" s="17" t="s">
         <v>10</v>
@@ -6427,120 +6460,241 @@
         <v>43</v>
       </c>
       <c r="E35" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="20" t="s">
         <v>55</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>56</v>
       </c>
       <c r="G35" s="21"/>
       <c r="H35" s="20" t="s">
         <v>46</v>
       </c>
       <c r="I35" s="20" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19"/>
       <c r="B36" s="18"/>
       <c r="C36" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H36" s="18"/>
       <c r="I36" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
-      <c r="B37" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="75" t="s">
-        <v>156</v>
-      </c>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="76"/>
-      <c r="G37" s="40" t="s">
-        <v>144</v>
-      </c>
-      <c r="H37" s="40"/>
-      <c r="I37" s="48">
+      <c r="B37" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
+      <c r="G37" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="H37" s="39"/>
+      <c r="I37" s="47">
         <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19"/>
-      <c r="B38" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" s="73" t="s">
-        <v>161</v>
-      </c>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="74"/>
-      <c r="G38" s="46" t="s">
-        <v>151</v>
-      </c>
-      <c r="H38" s="46"/>
-      <c r="I38" s="47">
+      <c r="B38" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="74" t="s">
+        <v>159</v>
+      </c>
+      <c r="D38" s="75"/>
+      <c r="E38" s="75"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="H38" s="45"/>
+      <c r="I38" s="46">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
       <c r="B39" s="18"/>
-      <c r="C39" s="69"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="69"/>
+      <c r="C39" s="78"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
       <c r="G39" s="18"/>
-      <c r="H39" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I39" s="56">
+      <c r="H39" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I39" s="55">
         <f>SUM(I37:I38)</f>
         <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
-    </row>
-    <row r="41" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B40" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H40" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I40" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="19"/>
-      <c r="H41" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="I41" s="51">
-        <f>I6+I13+I20+I26+I33+I39</f>
+      <c r="B41" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="20" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G41" s="21"/>
+      <c r="H41" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I41" s="20" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="19"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H42" s="18"/>
+      <c r="I42" s="22" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
+      <c r="B43" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="72" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="H43" s="39"/>
+      <c r="I43" s="47">
+        <v>7</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="76" t="s">
+        <v>158</v>
+      </c>
+      <c r="D44" s="77"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="77"/>
+      <c r="G44" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="H44" s="42"/>
+      <c r="I44" s="43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="74" t="s">
+        <v>160</v>
+      </c>
+      <c r="D45" s="75"/>
+      <c r="E45" s="75"/>
+      <c r="F45" s="75"/>
+      <c r="G45" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="H45" s="45"/>
+      <c r="I45" s="46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="19"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I46" s="55">
+        <f>SUM(I43:I45)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A47" s="19"/>
+      <c r="H47" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="I47" s="50">
+        <f>SUM(I6,I13,I20,I26,I33,I39,I46,)</f>
+        <v>71</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
@@ -6564,8 +6718,6 @@
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B55" s="18"/>
@@ -6598,10 +6750,8 @@
       <c r="I57" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
+  <mergeCells count="21">
+    <mergeCell ref="C26:F26"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C5:F5"/>
@@ -6614,9 +6764,14 @@
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C26:F26"/>
     <mergeCell ref="C31:F31"/>
     <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6624,14 +6779,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="6" max="6" width="61.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="17" t="s">
@@ -6644,16 +6803,16 @@
         <v>36</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>10</v>
@@ -6661,111 +6820,105 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>42</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="20" t="s">
         <v>46</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="18"/>
       <c r="C3" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="75" t="s">
-        <v>158</v>
-      </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="40" t="s">
-        <v>159</v>
-      </c>
-      <c r="H4" s="40"/>
-      <c r="I4" s="48">
+      <c r="B4" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="72" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="39"/>
+      <c r="I4" s="47">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="71" t="s">
-        <v>160</v>
-      </c>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="43" t="s">
-        <v>149</v>
-      </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="44">
-        <v>3</v>
+      <c r="B5" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="76" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" s="42"/>
+      <c r="I5" s="43">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>162</v>
-      </c>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="H6" s="46"/>
-      <c r="I6" s="47">
-        <v>4</v>
+      <c r="B6" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="74" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="H6" s="45"/>
+      <c r="I6" s="46">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I7" s="56">
+      <c r="H7" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="55">
         <f>SUM(I4:I6)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6779,16 +6932,16 @@
         <v>36</v>
       </c>
       <c r="E8" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I8" s="17" t="s">
         <v>10</v>
@@ -6796,7 +6949,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>42</v>
@@ -6805,416 +6958,504 @@
         <v>43</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="20" t="s">
         <v>46</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="18"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="22" t="s">
+      <c r="H10" s="59"/>
+      <c r="I10" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="22" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="75" t="s">
-        <v>163</v>
-      </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="40" t="s">
-        <v>144</v>
-      </c>
-      <c r="H11" s="40"/>
-      <c r="I11" s="48">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" s="71" t="s">
+      <c r="B11" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="72" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="43" t="s">
-        <v>142</v>
-      </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="44">
-        <v>2</v>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="H11" s="56"/>
+      <c r="I11" s="47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58" t="s">
+        <v>147</v>
+      </c>
+      <c r="H12" s="58"/>
+      <c r="I12" s="46">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="C13" s="73" t="s">
-        <v>165</v>
-      </c>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="H13" s="46"/>
-      <c r="I13" s="47">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H14" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I14" s="56">
-        <f>SUM(I11:I13)</f>
-        <v>15</v>
+      <c r="B13" s="59"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="54">
+        <f>SUM(I11:I12)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="17" t="s">
+      <c r="B15" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="21"/>
+      <c r="H15" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="70"/>
+      <c r="C16" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="70"/>
+      <c r="I16" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="72" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="69" t="s">
+        <v>149</v>
+      </c>
+      <c r="H17" s="69"/>
+      <c r="I17" s="47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="68" t="s">
+        <v>176</v>
+      </c>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="68" t="s">
+        <v>147</v>
+      </c>
+      <c r="H18" s="68"/>
+      <c r="I18" s="46">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="70"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" s="54">
+        <f>SUM(I17:I18)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C20" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D20" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E20" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="G20" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="I20" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="70"/>
+      <c r="C22" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" s="70"/>
+      <c r="I22" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="C23" s="72" t="s">
+        <v>180</v>
+      </c>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="69" t="s">
+        <v>149</v>
+      </c>
+      <c r="H23" s="69"/>
+      <c r="I23" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="C24" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68" t="s">
+        <v>147</v>
+      </c>
+      <c r="H24" s="68"/>
+      <c r="I24" s="46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="70"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="I25" s="54">
+        <f>SUM(I23:I24)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="H26" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="G27" s="21"/>
+      <c r="H27" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I27" s="71" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="59"/>
+      <c r="C28" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28" s="59"/>
+      <c r="I28" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="C29" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="56" t="s">
+        <v>157</v>
+      </c>
+      <c r="H29" s="56"/>
+      <c r="I29" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="C30" s="72" t="s">
+        <v>168</v>
+      </c>
+      <c r="D30" s="72"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="72"/>
+      <c r="G30" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="H30" s="57"/>
+      <c r="I30" s="43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="C31" s="74" t="s">
+        <v>167</v>
+      </c>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="H31" s="58"/>
+      <c r="I31" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="C32" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="74"/>
+      <c r="G32" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="H32" s="58"/>
+      <c r="I32" s="46">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" s="21"/>
-      <c r="H17" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="60"/>
-      <c r="C18" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="H18" s="60"/>
-      <c r="I18" s="22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="38" t="s">
-        <v>175</v>
-      </c>
-      <c r="C19" s="75" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="57" t="s">
-        <v>151</v>
-      </c>
-      <c r="H19" s="57"/>
-      <c r="I19" s="48">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="45" t="s">
-        <v>176</v>
-      </c>
-      <c r="C20" s="59" t="s">
-        <v>167</v>
-      </c>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59" t="s">
-        <v>149</v>
-      </c>
-      <c r="H20" s="59"/>
-      <c r="I20" s="47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="60"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="I21" s="55">
-        <f>SUM(I19:I20)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="H23" s="17" t="s">
+    <row r="33" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H33" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I33" s="52">
+        <f>SUM(I29:I32)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="I34" s="49">
+        <f>SUM(I7,I13,I19,I25,I33)</f>
         <v>69</v>
       </c>
-      <c r="I23" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" s="21"/>
-      <c r="H24" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" s="20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="60"/>
-      <c r="C25" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="H25" s="60"/>
-      <c r="I25" s="22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="75" t="s">
-        <v>168</v>
-      </c>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="57" t="s">
-        <v>159</v>
-      </c>
-      <c r="H26" s="57"/>
-      <c r="I26" s="48">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="C27" s="75" t="s">
-        <v>170</v>
-      </c>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="58" t="s">
-        <v>147</v>
-      </c>
-      <c r="H27" s="58"/>
-      <c r="I27" s="44">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="45" t="s">
-        <v>177</v>
-      </c>
-      <c r="C28" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="59" t="s">
-        <v>144</v>
-      </c>
-      <c r="H28" s="59"/>
-      <c r="I28" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="45" t="s">
-        <v>178</v>
-      </c>
-      <c r="C29" s="73" t="s">
-        <v>171</v>
-      </c>
-      <c r="D29" s="73"/>
-      <c r="E29" s="73"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="H29" s="59"/>
-      <c r="I29" s="47">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H30" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I30" s="53">
-        <f>SUM(I26:I29)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H31" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="I31" s="50">
-        <f>I14+I7+I21+I30</f>
-        <v>59</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="C12:F12"/>
+  <mergeCells count="13">
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C11:F11"/>
     <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C5:F5"/>
     <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C17:F17"/>
     <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C26:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7348,7 +7589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
@@ -7486,7 +7727,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:G14"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -7732,46 +7973,46 @@
       <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="64">
+      <c r="A13" s="63">
         <v>2</v>
       </c>
-      <c r="B13" s="65">
+      <c r="B13" s="64">
         <f>IFERROR(B12+1,1)</f>
         <v>11</v>
       </c>
-      <c r="C13" s="66">
+      <c r="C13" s="65">
         <v>10</v>
       </c>
-      <c r="D13" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="67"/>
-      <c r="F13" s="64">
+      <c r="D13" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="66"/>
+      <c r="F13" s="63">
         <f>SprintBacklog[[#This Row],[Estimated Hours]]</f>
         <v>10</v>
       </c>
-      <c r="G13" s="67"/>
+      <c r="G13" s="66"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68">
+      <c r="B14" s="67"/>
+      <c r="C14" s="67">
         <f>SUBTOTAL(109,SprintBacklog[Estimated Hours])</f>
         <v>124</v>
       </c>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68">
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67">
         <f>SUBTOTAL(109,SprintBacklog[Remaining Hours])</f>
         <v>124</v>
       </c>
-      <c r="G14" s="68"/>
+      <c r="G14" s="67"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G13" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"In Progress, Completed, Blocked"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7783,7 +8024,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:E26"/>
   <sheetViews>
     <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
@@ -8220,10 +8461,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Agregado archivos del proyecto
</commit_message>
<xml_diff>
--- a/Excel-Burndown-Chart-Template.xlsx
+++ b/Excel-Burndown-Chart-Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos de Micha\Tercer Semestre\Proyecto Metodologia\proyectometodologia7342\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emili\Desktop\ProyectoMetodologia\proyectometodologia7342\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4774B8-087C-4A07-AE6C-755C0BC4E6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="4" r:id="rId1"/>
@@ -33,7 +34,7 @@
     <definedName name="WorkingDays" localSheetId="4">Sprint2Info!$B$6</definedName>
     <definedName name="WorkingDays">Sprint1Info!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,9 +42,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -52,12 +51,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>PowerUps for Excel</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -86,12 +85,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>PowerUps for Excel</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
       <text>
         <r>
           <rPr>
@@ -120,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="193">
   <si>
     <t>Start Date</t>
   </si>
@@ -263,9 +262,6 @@
     <t>Alta</t>
   </si>
   <si>
-    <t>Terminado</t>
-  </si>
-  <si>
     <t>Agregar un proveedor</t>
   </si>
   <si>
@@ -353,9 +349,6 @@
     <t>HU11</t>
   </si>
   <si>
-    <t>No iniciado</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -653,17 +646,65 @@
     <t>HU10-2</t>
   </si>
   <si>
-    <t>HU11-3</t>
-  </si>
-  <si>
-    <t>HU11-4</t>
+    <t>Crear formulario de trabajadores</t>
+  </si>
+  <si>
+    <t>Creación, editar, y eliminar trabajadores</t>
+  </si>
+  <si>
+    <t>HU12</t>
+  </si>
+  <si>
+    <t>HU12-1</t>
+  </si>
+  <si>
+    <t>HU12-2</t>
+  </si>
+  <si>
+    <t>Implementar algoritmos de búsqueda</t>
+  </si>
+  <si>
+    <t>Revisión general del programa</t>
+  </si>
+  <si>
+    <t>HU13-1</t>
+  </si>
+  <si>
+    <t>HU13-2</t>
+  </si>
+  <si>
+    <t>HU133</t>
+  </si>
+  <si>
+    <t>HU13-4</t>
+  </si>
+  <si>
+    <t>Buscar ventas y artículos</t>
+  </si>
+  <si>
+    <t>Programa</t>
+  </si>
+  <si>
+    <t>un programa funcional</t>
+  </si>
+  <si>
+    <t>cumplir con las necesidades del negocio</t>
+  </si>
+  <si>
+    <t>Abierto</t>
+  </si>
+  <si>
+    <t>En Revisión</t>
+  </si>
+  <si>
+    <t>Por iniciar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -744,6 +785,12 @@
       <color theme="1"/>
       <name val="Segoe UI Light"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -789,7 +836,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -911,19 +958,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1143,7 +1177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1189,11 +1223,13 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1203,60 +1239,61 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1264,125 +1301,6 @@
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="41">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Light"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1548,6 +1466,23 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1578,6 +1513,23 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1617,6 +1569,23 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1647,6 +1616,23 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1686,6 +1672,23 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1719,6 +1722,23 @@
     <dxf>
       <font>
         <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1734,6 +1754,23 @@
           <color indexed="64"/>
         </right>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Segoe UI Light"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1983,7 +2020,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2027,7 +2064,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2053,7 +2089,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-EC"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2264,7 +2300,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -2477,7 +2513,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -2698,7 +2734,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -2758,7 +2794,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="243407728"/>
@@ -2817,7 +2853,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="243407336"/>
@@ -2834,7 +2870,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2860,7 +2895,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-EC"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2890,7 +2925,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-EC"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2902,7 +2937,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2946,7 +2981,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2972,7 +3006,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-EC"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3183,7 +3217,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -3396,7 +3430,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -3617,7 +3651,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-57AD-4103-AA38-D12E8EA744C5}"/>
             </c:ext>
@@ -3677,7 +3711,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="244669568"/>
@@ -3736,7 +3770,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-EC"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="243408512"/>
@@ -3753,7 +3787,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3779,7 +3812,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-EC"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3809,7 +3842,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-EC"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4926,7 +4959,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4969,7 +5002,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4993,74 +5026,74 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <tableColumns count="2">
-    <tableColumn id="1" name="Column1" headerRowDxfId="38" dataDxfId="37"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="36" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" headerRowDxfId="38" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" headerRowDxfId="36" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table25" displayName="Table25" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table25" displayName="Table25" ref="A2:B10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <tableColumns count="2">
-    <tableColumn id="1" name="Column1" headerRowDxfId="32" dataDxfId="31"/>
-    <tableColumn id="2" name="Column2" headerRowDxfId="30" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" headerRowDxfId="32" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column2" headerRowDxfId="30" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="SprintBacklog" displayName="SprintBacklog" ref="A2:G14" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
-  <autoFilter ref="A2:G13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="SprintBacklog" displayName="SprintBacklog" ref="A2:G14" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27" totalsRowDxfId="26">
+  <autoFilter ref="A2:G13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Sprint" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="6"/>
-    <tableColumn id="2" name="Item ID" dataDxfId="24" totalsRowDxfId="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Sprint" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Item ID" dataDxfId="23" totalsRowDxfId="22">
       <calculatedColumnFormula>IFERROR(B2+1,1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="4"/>
-    <tableColumn id="4" name="Task Name" dataDxfId="22" totalsRowDxfId="3"/>
-    <tableColumn id="5" name="Assigned To" dataDxfId="21" totalsRowDxfId="2"/>
-    <tableColumn id="6" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="1">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Estimated Hours" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Task Name" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Assigned To" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Remaining Hours" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula>SprintBacklog[[#This Row],[Estimated Hours]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Status" dataDxfId="19" totalsRowDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Status" dataDxfId="13" totalsRowDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:D26" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A2:D26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table3" displayName="Table3" ref="A2:D26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A2:D26" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Work Day" dataDxfId="16"/>
-    <tableColumn id="2" name="Target Burn Down" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Work Day" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Target Burn Down" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Forecast Burn Down" dataDxfId="7">
       <calculatedColumnFormula>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Actual Burn Down" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Actual Burn Down" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table38" displayName="Table38" ref="A2:D13" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A2:D13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table38" displayName="Table38" ref="A2:D13" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A2:D13" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Work Day" dataDxfId="10"/>
-    <tableColumn id="2" name="Target Burn Down" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Work Day" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Target Burn Down" dataDxfId="2">
       <calculatedColumnFormula>IFERROR(TotalHours-(Table38[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Forecast Burn Down" dataDxfId="8">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Forecast Burn Down" dataDxfId="1">
       <calculatedColumnFormula>TotalHours-(Table38[[#This Row],[Work Day]]*DevRate)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Actual Burn Down" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Actual Burn Down" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium26" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5328,11 +5361,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5343,367 +5376,367 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="35" t="s">
+      <c r="A1" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="35" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="31" t="s">
+      <c r="A2" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>103</v>
+      <c r="B3" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G3" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>103</v>
+      <c r="A4" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H4" s="28" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>103</v>
+      <c r="A5" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G5" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>103</v>
+      <c r="A6" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D6" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="E6" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="E6" s="24" t="s">
-        <v>126</v>
-      </c>
       <c r="F6" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G6" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>103</v>
+      <c r="A7" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C7" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D7" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="E7" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="E7" s="24" t="s">
-        <v>127</v>
-      </c>
       <c r="F7" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="G8" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="G9" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="H9" s="28" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>103</v>
+      <c r="B10" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G10" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>77</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>103</v>
+      <c r="A11" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F11" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G11" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>77</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>103</v>
+      <c r="A12" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>77</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
-        <v>115</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>103</v>
+      <c r="A13" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="F13" s="61" t="s">
-        <v>78</v>
+        <v>131</v>
+      </c>
+      <c r="F13" s="60" t="s">
+        <v>76</v>
       </c>
       <c r="G13" s="26" t="s">
         <v>46</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>77</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" s="62" t="s">
-        <v>116</v>
-      </c>
-      <c r="D14" s="62" t="s">
-        <v>64</v>
+      <c r="A14" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="61" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="61" t="s">
+        <v>63</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="F14" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" s="63" t="s">
-        <v>174</v>
-      </c>
-      <c r="H14" s="29" t="s">
-        <v>77</v>
+        <v>138</v>
+      </c>
+      <c r="F14" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="62" t="s">
+        <v>172</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -5712,11 +5745,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5736,16 +5769,16 @@
         <v>36</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>10</v>
@@ -5773,76 +5806,76 @@
         <v>46</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="19"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="39" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="39" t="s">
+      <c r="H3" s="39"/>
+      <c r="I3" s="40" t="s">
         <v>71</v>
-      </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="19"/>
-      <c r="B4" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="71" t="s">
-        <v>141</v>
-      </c>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="43" t="s">
-        <v>149</v>
-      </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="44">
+      <c r="B4" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="76" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="42"/>
+      <c r="I4" s="43">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
-      <c r="B5" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="73" t="s">
-        <v>148</v>
-      </c>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="H5" s="46"/>
-      <c r="I5" s="47">
+      <c r="B5" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="74" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" s="45"/>
+      <c r="I5" s="46">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
       <c r="G6" s="18"/>
-      <c r="H6" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I6" s="56">
+      <c r="H6" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I6" s="55">
         <f>SUM(I4:I5)</f>
         <v>6</v>
       </c>
@@ -5859,16 +5892,16 @@
         <v>36</v>
       </c>
       <c r="E7" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>10</v>
@@ -5883,108 +5916,108 @@
         <v>42</v>
       </c>
       <c r="D8" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>73</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>74</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20" t="s">
         <v>46</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19"/>
       <c r="B9" s="18"/>
       <c r="C9" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
-      <c r="B10" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="75" t="s">
-        <v>143</v>
-      </c>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="40" t="s">
-        <v>144</v>
-      </c>
-      <c r="H10" s="40"/>
-      <c r="I10" s="48">
+      <c r="B10" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="72" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" s="39"/>
+      <c r="I10" s="47">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
-      <c r="B11" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="71" t="s">
-        <v>145</v>
-      </c>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="43" t="s">
-        <v>142</v>
-      </c>
-      <c r="H11" s="43"/>
-      <c r="I11" s="44">
+      <c r="B11" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="76" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="H11" s="42"/>
+      <c r="I11" s="43">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19"/>
-      <c r="B12" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="73" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="H12" s="46"/>
-      <c r="I12" s="49">
+      <c r="B12" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="74" t="s">
+        <v>144</v>
+      </c>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" s="45"/>
+      <c r="I12" s="48">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
       <c r="G13" s="18"/>
-      <c r="H13" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I13" s="56">
+      <c r="H13" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="55">
         <f>SUM(I10:I12)</f>
         <v>8</v>
       </c>
@@ -6001,16 +6034,16 @@
         <v>36</v>
       </c>
       <c r="E14" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I14" s="17" t="s">
         <v>10</v>
@@ -6028,90 +6061,90 @@
         <v>43</v>
       </c>
       <c r="E15" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>49</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>50</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="20" t="s">
         <v>46</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19"/>
       <c r="B16" s="18"/>
       <c r="C16" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
-      <c r="B17" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="75" t="s">
-        <v>150</v>
-      </c>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="40" t="s">
-        <v>151</v>
-      </c>
-      <c r="H17" s="40"/>
-      <c r="I17" s="48">
+      <c r="B17" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="72" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="H17" s="39"/>
+      <c r="I17" s="47">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
-      <c r="B18" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="71" t="s">
-        <v>152</v>
-      </c>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="43" t="s">
-        <v>144</v>
-      </c>
-      <c r="H18" s="43"/>
-      <c r="I18" s="44">
+      <c r="B18" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="76" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="42"/>
+      <c r="I18" s="43">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
-      <c r="B19" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="C19" s="73" t="s">
-        <v>153</v>
-      </c>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="H19" s="46"/>
-      <c r="I19" s="47">
+      <c r="B19" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="74" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19" s="75"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="H19" s="45"/>
+      <c r="I19" s="46">
         <v>6</v>
       </c>
     </row>
@@ -6123,10 +6156,10 @@
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
-      <c r="H20" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I20" s="56">
+      <c r="H20" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I20" s="55">
         <f>SUM(I17:I19)</f>
         <v>11</v>
       </c>
@@ -6143,16 +6176,16 @@
         <v>36</v>
       </c>
       <c r="E21" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I21" s="17" t="s">
         <v>10</v>
@@ -6170,86 +6203,86 @@
         <v>43</v>
       </c>
       <c r="E22" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="20" t="s">
         <v>51</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>52</v>
       </c>
       <c r="G22" s="21"/>
       <c r="H22" s="20" t="s">
         <v>46</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="18"/>
       <c r="C23" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
-      <c r="B24" s="38" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="75" t="s">
-        <v>154</v>
-      </c>
-      <c r="D24" s="76"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="H24" s="40"/>
-      <c r="I24" s="48">
+      <c r="B24" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="72" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="H24" s="39"/>
+      <c r="I24" s="47">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
-      <c r="B25" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="70" t="s">
-        <v>173</v>
-      </c>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="46" t="s">
-        <v>149</v>
-      </c>
-      <c r="H25" s="46"/>
-      <c r="I25" s="47">
+      <c r="B25" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="79" t="s">
+        <v>171</v>
+      </c>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="H25" s="45"/>
+      <c r="I25" s="46">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
       <c r="G26" s="18"/>
-      <c r="H26" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I26" s="56">
+      <c r="H26" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I26" s="55">
         <f>SUM(I24:I25)</f>
         <v>10</v>
       </c>
@@ -6266,16 +6299,16 @@
         <v>36</v>
       </c>
       <c r="E27" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I27" s="17" t="s">
         <v>10</v>
@@ -6293,17 +6326,17 @@
         <v>43</v>
       </c>
       <c r="E28" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="20" t="s">
         <v>53</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>54</v>
       </c>
       <c r="G28" s="21"/>
       <c r="H28" s="20" t="s">
         <v>46</v>
       </c>
       <c r="I28" s="20" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -6321,54 +6354,54 @@
       <c r="A30" s="19"/>
       <c r="B30" s="18"/>
       <c r="C30" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
       <c r="G30" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H30" s="18"/>
       <c r="I30" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
-      <c r="B31" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="75" t="s">
-        <v>155</v>
-      </c>
-      <c r="D31" s="76"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="40" t="s">
-        <v>142</v>
-      </c>
-      <c r="H31" s="40"/>
-      <c r="I31" s="48">
+      <c r="B31" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="72" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="73"/>
+      <c r="E31" s="73"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="H31" s="39"/>
+      <c r="I31" s="47">
         <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
-      <c r="B32" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" s="73" t="s">
-        <v>157</v>
-      </c>
-      <c r="D32" s="74"/>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="H32" s="46"/>
-      <c r="I32" s="47">
+      <c r="B32" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="74" t="s">
+        <v>155</v>
+      </c>
+      <c r="D32" s="75"/>
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="H32" s="45"/>
+      <c r="I32" s="46">
         <v>6</v>
       </c>
     </row>
@@ -6380,10 +6413,10 @@
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
       <c r="G33" s="18"/>
-      <c r="H33" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I33" s="56">
+      <c r="H33" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I33" s="55">
         <f>SUM(I31:I32)</f>
         <v>10</v>
       </c>
@@ -6400,16 +6433,16 @@
         <v>36</v>
       </c>
       <c r="E34" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I34" s="17" t="s">
         <v>10</v>
@@ -6427,120 +6460,241 @@
         <v>43</v>
       </c>
       <c r="E35" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F35" s="20" t="s">
         <v>55</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>56</v>
       </c>
       <c r="G35" s="21"/>
       <c r="H35" s="20" t="s">
         <v>46</v>
       </c>
       <c r="I35" s="20" t="s">
-        <v>47</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19"/>
       <c r="B36" s="18"/>
       <c r="C36" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
       <c r="F36" s="18"/>
       <c r="G36" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H36" s="18"/>
       <c r="I36" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
-      <c r="B37" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="75" t="s">
-        <v>156</v>
-      </c>
-      <c r="D37" s="76"/>
-      <c r="E37" s="76"/>
-      <c r="F37" s="76"/>
-      <c r="G37" s="40" t="s">
-        <v>144</v>
-      </c>
-      <c r="H37" s="40"/>
-      <c r="I37" s="48">
+      <c r="B37" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="72" t="s">
+        <v>154</v>
+      </c>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
+      <c r="G37" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="H37" s="39"/>
+      <c r="I37" s="47">
         <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19"/>
-      <c r="B38" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" s="73" t="s">
-        <v>161</v>
-      </c>
-      <c r="D38" s="74"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="74"/>
-      <c r="G38" s="46" t="s">
-        <v>151</v>
-      </c>
-      <c r="H38" s="46"/>
-      <c r="I38" s="47">
+      <c r="B38" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="74" t="s">
+        <v>159</v>
+      </c>
+      <c r="D38" s="75"/>
+      <c r="E38" s="75"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="H38" s="45"/>
+      <c r="I38" s="46">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="19"/>
       <c r="B39" s="18"/>
-      <c r="C39" s="69"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="69"/>
+      <c r="C39" s="78"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="78"/>
       <c r="G39" s="18"/>
-      <c r="H39" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I39" s="56">
+      <c r="H39" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I39" s="55">
         <f>SUM(I37:I38)</f>
         <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
-    </row>
-    <row r="41" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B40" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H40" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I40" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="19"/>
-      <c r="H41" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="I41" s="51">
-        <f>I6+I13+I20+I26+I33+I39</f>
+      <c r="B41" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="20" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G41" s="21"/>
+      <c r="H41" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I41" s="20" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="19"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H42" s="18"/>
+      <c r="I42" s="22" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
+      <c r="B43" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="72" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="H43" s="39"/>
+      <c r="I43" s="47">
+        <v>7</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="76" t="s">
+        <v>158</v>
+      </c>
+      <c r="D44" s="77"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="77"/>
+      <c r="G44" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="H44" s="42"/>
+      <c r="I44" s="43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="74" t="s">
+        <v>160</v>
+      </c>
+      <c r="D45" s="75"/>
+      <c r="E45" s="75"/>
+      <c r="F45" s="75"/>
+      <c r="G45" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="H45" s="45"/>
+      <c r="I45" s="46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="19"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I46" s="55">
+        <f>SUM(I43:I45)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A47" s="19"/>
+      <c r="H47" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="I47" s="50">
+        <f>SUM(I6,I13,I20,I26,I33,I39,I46,)</f>
+        <v>71</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
@@ -6564,8 +6718,6 @@
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
       <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B55" s="18"/>
@@ -6598,10 +6750,8 @@
       <c r="I57" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
+  <mergeCells count="21">
+    <mergeCell ref="C26:F26"/>
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C5:F5"/>
@@ -6614,9 +6764,14 @@
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C26:F26"/>
     <mergeCell ref="C31:F31"/>
     <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6624,14 +6779,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="6" max="6" width="61.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="17" t="s">
@@ -6644,16 +6803,16 @@
         <v>36</v>
       </c>
       <c r="E1" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>10</v>
@@ -6661,111 +6820,105 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>42</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G2" s="21"/>
       <c r="H2" s="20" t="s">
         <v>46</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="18"/>
       <c r="C3" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="75" t="s">
-        <v>158</v>
-      </c>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="40" t="s">
-        <v>159</v>
-      </c>
-      <c r="H4" s="40"/>
-      <c r="I4" s="48">
+      <c r="B4" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="72" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="39"/>
+      <c r="I4" s="47">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="71" t="s">
-        <v>160</v>
-      </c>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="43" t="s">
-        <v>149</v>
-      </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="44">
-        <v>3</v>
+      <c r="B5" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="76" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" s="42"/>
+      <c r="I5" s="43">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>162</v>
-      </c>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="H6" s="46"/>
-      <c r="I6" s="47">
-        <v>4</v>
+      <c r="B6" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="74" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="H6" s="45"/>
+      <c r="I6" s="46">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I7" s="56">
+      <c r="H7" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="55">
         <f>SUM(I4:I6)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -6779,16 +6932,16 @@
         <v>36</v>
       </c>
       <c r="E8" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I8" s="17" t="s">
         <v>10</v>
@@ -6796,7 +6949,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>42</v>
@@ -6805,416 +6958,504 @@
         <v>43</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="20" t="s">
         <v>46</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>47</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="18"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="22" t="s">
+      <c r="H10" s="59"/>
+      <c r="I10" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="22" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="75" t="s">
-        <v>163</v>
-      </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="40" t="s">
-        <v>144</v>
-      </c>
-      <c r="H11" s="40"/>
-      <c r="I11" s="48">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" s="71" t="s">
+      <c r="B11" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="72" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="43" t="s">
-        <v>142</v>
-      </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="44">
-        <v>2</v>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="H11" s="56"/>
+      <c r="I11" s="47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58" t="s">
+        <v>147</v>
+      </c>
+      <c r="H12" s="58"/>
+      <c r="I12" s="46">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="C13" s="73" t="s">
-        <v>165</v>
-      </c>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="H13" s="46"/>
-      <c r="I13" s="47">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H14" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I14" s="56">
-        <f>SUM(I11:I13)</f>
-        <v>15</v>
+      <c r="B13" s="59"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="I13" s="54">
+        <f>SUM(I11:I12)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="19"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="17" t="s">
+      <c r="B15" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="21"/>
+      <c r="H15" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="70"/>
+      <c r="C16" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="70"/>
+      <c r="I16" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="72" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="69" t="s">
+        <v>149</v>
+      </c>
+      <c r="H17" s="69"/>
+      <c r="I17" s="47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="68" t="s">
+        <v>176</v>
+      </c>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="68" t="s">
+        <v>147</v>
+      </c>
+      <c r="H18" s="68"/>
+      <c r="I18" s="46">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="70"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" s="54">
+        <f>SUM(I17:I18)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C20" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D20" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E20" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="G20" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="I20" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="70"/>
+      <c r="C22" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" s="70"/>
+      <c r="I22" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="C23" s="72" t="s">
+        <v>180</v>
+      </c>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="69" t="s">
+        <v>149</v>
+      </c>
+      <c r="H23" s="69"/>
+      <c r="I23" s="47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="C24" s="68" t="s">
+        <v>181</v>
+      </c>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68" t="s">
+        <v>147</v>
+      </c>
+      <c r="H24" s="68"/>
+      <c r="I24" s="46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="70"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="I25" s="54">
+        <f>SUM(I23:I24)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="H26" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="G27" s="21"/>
+      <c r="H27" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I27" s="71" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="59"/>
+      <c r="C28" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28" s="59"/>
+      <c r="I28" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="C29" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="56" t="s">
+        <v>157</v>
+      </c>
+      <c r="H29" s="56"/>
+      <c r="I29" s="47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="C30" s="72" t="s">
+        <v>168</v>
+      </c>
+      <c r="D30" s="72"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="72"/>
+      <c r="G30" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="H30" s="57"/>
+      <c r="I30" s="43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="C31" s="74" t="s">
+        <v>167</v>
+      </c>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="58" t="s">
+        <v>142</v>
+      </c>
+      <c r="H31" s="58"/>
+      <c r="I31" s="46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="C32" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="74"/>
+      <c r="G32" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="H32" s="58"/>
+      <c r="I32" s="46">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" s="21"/>
-      <c r="H17" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="60"/>
-      <c r="C18" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="H18" s="60"/>
-      <c r="I18" s="22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="38" t="s">
-        <v>175</v>
-      </c>
-      <c r="C19" s="75" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="57" t="s">
-        <v>151</v>
-      </c>
-      <c r="H19" s="57"/>
-      <c r="I19" s="48">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="45" t="s">
-        <v>176</v>
-      </c>
-      <c r="C20" s="59" t="s">
-        <v>167</v>
-      </c>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59" t="s">
-        <v>149</v>
-      </c>
-      <c r="H20" s="59"/>
-      <c r="I20" s="47">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="60"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="I21" s="55">
-        <f>SUM(I19:I20)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="H23" s="17" t="s">
+    <row r="33" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H33" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I33" s="52">
+        <f>SUM(I29:I32)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H34" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="I34" s="49">
+        <f>SUM(I7,I13,I19,I25,I33)</f>
         <v>69</v>
       </c>
-      <c r="I23" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="G24" s="21"/>
-      <c r="H24" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" s="20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="60"/>
-      <c r="C25" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="H25" s="60"/>
-      <c r="I25" s="22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="75" t="s">
-        <v>168</v>
-      </c>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="57" t="s">
-        <v>159</v>
-      </c>
-      <c r="H26" s="57"/>
-      <c r="I26" s="48">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="C27" s="75" t="s">
-        <v>170</v>
-      </c>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="58" t="s">
-        <v>147</v>
-      </c>
-      <c r="H27" s="58"/>
-      <c r="I27" s="44">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="45" t="s">
-        <v>177</v>
-      </c>
-      <c r="C28" s="73" t="s">
-        <v>169</v>
-      </c>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="59" t="s">
-        <v>144</v>
-      </c>
-      <c r="H28" s="59"/>
-      <c r="I28" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="45" t="s">
-        <v>178</v>
-      </c>
-      <c r="C29" s="73" t="s">
-        <v>171</v>
-      </c>
-      <c r="D29" s="73"/>
-      <c r="E29" s="73"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="59" t="s">
-        <v>172</v>
-      </c>
-      <c r="H29" s="59"/>
-      <c r="I29" s="47">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H30" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="I30" s="53">
-        <f>SUM(I26:I29)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H31" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="I31" s="50">
-        <f>I14+I7+I21+I30</f>
-        <v>59</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="C12:F12"/>
+  <mergeCells count="13">
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C11:F11"/>
     <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C5:F5"/>
     <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C17:F17"/>
     <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C26:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7348,7 +7589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
@@ -7486,7 +7727,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:G14"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -7732,46 +7973,46 @@
       <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="64">
+      <c r="A13" s="63">
         <v>2</v>
       </c>
-      <c r="B13" s="65">
+      <c r="B13" s="64">
         <f>IFERROR(B12+1,1)</f>
         <v>11</v>
       </c>
-      <c r="C13" s="66">
+      <c r="C13" s="65">
         <v>10</v>
       </c>
-      <c r="D13" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="E13" s="67"/>
-      <c r="F13" s="64">
+      <c r="D13" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="66"/>
+      <c r="F13" s="63">
         <f>SprintBacklog[[#This Row],[Estimated Hours]]</f>
         <v>10</v>
       </c>
-      <c r="G13" s="67"/>
+      <c r="G13" s="66"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68">
+      <c r="B14" s="67"/>
+      <c r="C14" s="67">
         <f>SUBTOTAL(109,SprintBacklog[Estimated Hours])</f>
         <v>124</v>
       </c>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68">
+      <c r="D14" s="67"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67">
         <f>SUBTOTAL(109,SprintBacklog[Remaining Hours])</f>
         <v>124</v>
       </c>
-      <c r="G14" s="68"/>
+      <c r="G14" s="67"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G13" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"In Progress, Completed, Blocked"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7783,7 +8024,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:E26"/>
   <sheetViews>
     <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
@@ -8220,10 +8461,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
se modificaron los valores aproximados de trabajo, revisar para dar por terminado
</commit_message>
<xml_diff>
--- a/Excel-Burndown-Chart-Template.xlsx
+++ b/Excel-Burndown-Chart-Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BackLog" sheetId="4" r:id="rId1"/>
@@ -2417,7 +2417,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2570,64 +2569,64 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>57</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54.15</c:v>
+                  <c:v>79.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51.3</c:v>
+                  <c:v>75.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48.45</c:v>
+                  <c:v>71.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45.6</c:v>
+                  <c:v>67.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42.75</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39.9</c:v>
+                  <c:v>58.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37.049999999999997</c:v>
+                  <c:v>54.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34.200000000000003</c:v>
+                  <c:v>50.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>31.349999999999998</c:v>
+                  <c:v>46.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>28.5</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25.65</c:v>
+                  <c:v>37.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>22.799999999999997</c:v>
+                  <c:v>33.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19.949999999999996</c:v>
+                  <c:v>29.4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17.100000000000001</c:v>
+                  <c:v>25.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14.25</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.399999999999999</c:v>
+                  <c:v>16.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.5499999999999972</c:v>
+                  <c:v>12.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.6999999999999957</c:v>
+                  <c:v>8.3999999999999915</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.8500000000000014</c:v>
+                  <c:v>4.2000000000000028</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -2765,67 +2764,67 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>57</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.043478260869563</c:v>
+                  <c:v>79.826086956521735</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43.086956521739133</c:v>
+                  <c:v>75.652173913043484</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.130434782608695</c:v>
+                  <c:v>71.478260869565219</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.173913043478262</c:v>
+                  <c:v>67.304347826086953</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.217391304347828</c:v>
+                  <c:v>63.130434782608695</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.260869565217391</c:v>
+                  <c:v>58.956521739130437</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.3043478260869605</c:v>
+                  <c:v>54.782608695652172</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3478260869565233</c:v>
+                  <c:v>50.608695652173914</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-5.608695652173914</c:v>
+                  <c:v>46.434782608695656</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-12.565217391304344</c:v>
+                  <c:v>42.260869565217391</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-19.521739130434781</c:v>
+                  <c:v>38.086956521739133</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-26.478260869565219</c:v>
+                  <c:v>33.913043478260875</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-33.434782608695656</c:v>
+                  <c:v>29.739130434782609</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-40.391304347826079</c:v>
+                  <c:v>25.565217391304351</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-47.347826086956516</c:v>
+                  <c:v>21.391304347826086</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-54.304347826086953</c:v>
+                  <c:v>17.217391304347828</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-61.260869565217391</c:v>
+                  <c:v>13.043478260869563</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-68.217391304347828</c:v>
+                  <c:v>8.8695652173913118</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-75.173913043478251</c:v>
+                  <c:v>4.6956521739130466</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-82.130434782608688</c:v>
+                  <c:v>0.52173913043478137</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2968,7 +2967,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>57</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>57</c:v>
@@ -3050,11 +3049,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="237257144"/>
-        <c:axId val="237257536"/>
+        <c:axId val="239343728"/>
+        <c:axId val="239344120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="237257144"/>
+        <c:axId val="239343728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3097,7 +3096,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237257536"/>
+        <c:crossAx val="239344120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3105,7 +3104,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="237257536"/>
+        <c:axId val="239344120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3156,7 +3155,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237257144"/>
+        <c:crossAx val="239343728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3170,7 +3169,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3441,70 +3439,70 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>59</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56.31818181818182</c:v>
+                  <c:v>91.63636363636364</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>53.63636363636364</c:v>
+                  <c:v>87.27272727272728</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50.954545454545453</c:v>
+                  <c:v>82.909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48.272727272727273</c:v>
+                  <c:v>78.545454545454547</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45.590909090909093</c:v>
+                  <c:v>74.181818181818187</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42.909090909090907</c:v>
+                  <c:v>69.818181818181813</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40.227272727272727</c:v>
+                  <c:v>65.454545454545453</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37.545454545454547</c:v>
+                  <c:v>61.090909090909093</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.863636363636367</c:v>
+                  <c:v>56.727272727272734</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32.181818181818187</c:v>
+                  <c:v>52.363636363636367</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29.5</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26.81818181818182</c:v>
+                  <c:v>43.63636363636364</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>24.13636363636364</c:v>
+                  <c:v>39.27272727272728</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21.454545454545453</c:v>
+                  <c:v>34.909090909090914</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18.772727272727273</c:v>
+                  <c:v>30.545454545454547</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.090909090909093</c:v>
+                  <c:v>26.181818181818187</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13.409090909090914</c:v>
+                  <c:v>21.818181818181827</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.727272727272734</c:v>
+                  <c:v>17.454545454545467</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.0454545454545467</c:v>
+                  <c:v>13.090909090909093</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.3636363636363669</c:v>
+                  <c:v>8.7272727272727337</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.681818181818187</c:v>
+                  <c:v>4.363636363636374</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>0</c:v>
@@ -3637,73 +3635,73 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>59</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55.8</c:v>
+                  <c:v>91.84</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.6</c:v>
+                  <c:v>87.68</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>49.4</c:v>
+                  <c:v>83.52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46.2</c:v>
+                  <c:v>79.36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43</c:v>
+                  <c:v>75.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39.799999999999997</c:v>
+                  <c:v>71.039999999999992</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36.599999999999994</c:v>
+                  <c:v>66.88</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33.4</c:v>
+                  <c:v>62.72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.2</c:v>
+                  <c:v>58.56</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27</c:v>
+                  <c:v>54.4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23.799999999999997</c:v>
+                  <c:v>50.239999999999995</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20.599999999999994</c:v>
+                  <c:v>46.08</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17.399999999999999</c:v>
+                  <c:v>41.92</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.199999999999996</c:v>
+                  <c:v>37.76</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11</c:v>
+                  <c:v>33.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.7999999999999972</c:v>
+                  <c:v>29.439999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.5999999999999943</c:v>
+                  <c:v>25.28</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.3999999999999986</c:v>
+                  <c:v>21.120000000000005</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-1.8000000000000043</c:v>
+                  <c:v>16.959999999999994</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-5</c:v>
+                  <c:v>12.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-8.2000000000000028</c:v>
+                  <c:v>8.64</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-11.400000000000006</c:v>
+                  <c:v>4.4799999999999898</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3833,7 +3831,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>59</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>59</c:v>
@@ -3916,11 +3914,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="390160960"/>
-        <c:axId val="390160568"/>
+        <c:axId val="239344904"/>
+        <c:axId val="239345296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="390160960"/>
+        <c:axId val="239344904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3963,7 +3961,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="390160568"/>
+        <c:crossAx val="239345296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3971,7 +3969,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="390160568"/>
+        <c:axId val="239345296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4022,7 +4020,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="390160960"/>
+        <c:crossAx val="239344904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5626,7 +5624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
@@ -6010,8 +6008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6104,7 +6102,7 @@
       </c>
       <c r="H4" s="43"/>
       <c r="I4" s="44">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6123,7 +6121,7 @@
       </c>
       <c r="H5" s="46"/>
       <c r="I5" s="47">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6139,7 +6137,7 @@
       </c>
       <c r="I6" s="56">
         <f>SUM(I4:I5)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -6227,7 +6225,7 @@
       </c>
       <c r="H10" s="40"/>
       <c r="I10" s="48">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -6246,7 +6244,7 @@
       </c>
       <c r="H11" s="43"/>
       <c r="I11" s="44">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6265,7 +6263,7 @@
       </c>
       <c r="H12" s="46"/>
       <c r="I12" s="49">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6281,7 +6279,7 @@
       </c>
       <c r="I13" s="56">
         <f>SUM(I10:I12)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -6369,7 +6367,7 @@
       </c>
       <c r="H17" s="40"/>
       <c r="I17" s="48">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -6388,7 +6386,7 @@
       </c>
       <c r="H18" s="43"/>
       <c r="I18" s="44">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6407,7 +6405,7 @@
       </c>
       <c r="H19" s="46"/>
       <c r="I19" s="47">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6423,7 +6421,7 @@
       </c>
       <c r="I20" s="56">
         <f>SUM(I17:I19)</f>
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -6511,7 +6509,7 @@
       </c>
       <c r="H24" s="40"/>
       <c r="I24" s="48">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6546,7 +6544,7 @@
       </c>
       <c r="I26" s="56">
         <f>SUM(I24:I25)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -6645,7 +6643,7 @@
       </c>
       <c r="H31" s="40"/>
       <c r="I31" s="48">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6664,7 +6662,7 @@
       </c>
       <c r="H32" s="46"/>
       <c r="I32" s="47">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6680,7 +6678,7 @@
       </c>
       <c r="I33" s="56">
         <f>SUM(I31:I32)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -6768,7 +6766,7 @@
       </c>
       <c r="H37" s="40"/>
       <c r="I37" s="48">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6803,7 +6801,7 @@
       </c>
       <c r="I39" s="56">
         <f>SUM(I37:I38)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -6816,7 +6814,7 @@
       </c>
       <c r="I41" s="51">
         <f>I6+I13+I20+I26+I33+I39</f>
-        <v>57</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -6922,8 +6920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7009,7 +7007,7 @@
       </c>
       <c r="H4" s="40"/>
       <c r="I4" s="48">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -7027,7 +7025,7 @@
       </c>
       <c r="H5" s="43"/>
       <c r="I5" s="44">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7045,7 +7043,7 @@
       </c>
       <c r="H6" s="46"/>
       <c r="I6" s="47">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7060,7 +7058,7 @@
       </c>
       <c r="I7" s="56">
         <f>SUM(I4:I6)</f>
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -7144,7 +7142,7 @@
       </c>
       <c r="H11" s="40"/>
       <c r="I11" s="48">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -7162,7 +7160,7 @@
       </c>
       <c r="H12" s="43"/>
       <c r="I12" s="44">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7180,7 +7178,7 @@
       </c>
       <c r="H13" s="46"/>
       <c r="I13" s="47">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7189,7 +7187,7 @@
       </c>
       <c r="I14" s="56">
         <f>SUM(I11:I13)</f>
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -7283,7 +7281,7 @@
       </c>
       <c r="H19" s="57"/>
       <c r="I19" s="48">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7301,7 +7299,7 @@
       </c>
       <c r="H20" s="59"/>
       <c r="I20" s="47">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7316,7 +7314,7 @@
       </c>
       <c r="I21" s="55">
         <f>SUM(I19:I20)</f>
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -7428,7 +7426,7 @@
       </c>
       <c r="H27" s="58"/>
       <c r="I27" s="44">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7446,7 +7444,7 @@
       </c>
       <c r="H28" s="59"/>
       <c r="I28" s="47">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7473,7 +7471,7 @@
       </c>
       <c r="I30" s="53">
         <f>SUM(I26:I29)</f>
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
@@ -7482,7 +7480,7 @@
       </c>
       <c r="I31" s="50">
         <f>I14+I7+I21+I30</f>
-        <v>59</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -7509,7 +7507,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7586,7 +7584,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="8">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -7598,7 +7596,7 @@
       </c>
       <c r="B9" s="3">
         <f>(B4-B5)*B8*B7*8</f>
-        <v>160</v>
+        <v>96</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -7608,7 +7606,7 @@
       </c>
       <c r="B10" s="3">
         <f>IFERROR(B9/B4,0)</f>
-        <v>6.9565217391304346</v>
+        <v>4.1739130434782608</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -7647,7 +7645,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7724,7 +7722,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="8">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>23</v>
@@ -7736,7 +7734,7 @@
       </c>
       <c r="B9" s="3">
         <f>(B4-B5)*B8*B7*8</f>
-        <v>70.400000000000006</v>
+        <v>91.52000000000001</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -7746,7 +7744,7 @@
       </c>
       <c r="B10" s="3">
         <f>IFERROR(B9/B4,0)</f>
-        <v>3.2</v>
+        <v>4.16</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -7784,8 +7782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G17"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7832,7 +7830,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>80</v>
@@ -7856,7 +7854,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>99</v>
@@ -7880,7 +7878,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>81</v>
@@ -7904,7 +7902,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>82</v>
@@ -7928,7 +7926,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>98</v>
@@ -7952,7 +7950,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>84</v>
@@ -7976,7 +7974,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>85</v>
@@ -8000,7 +7998,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>83</v>
@@ -8024,7 +8022,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>86</v>
@@ -8072,7 +8070,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="66">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D13" s="64" t="s">
         <v>88</v>
@@ -8096,7 +8094,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="66">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" s="64" t="s">
         <v>89</v>
@@ -8120,7 +8118,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="66">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D15" s="64" t="s">
         <v>90</v>
@@ -8130,7 +8128,7 @@
       </c>
       <c r="F15" s="64">
         <f>SprintBacklog[[#This Row],[Estimated Hours]]</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>174</v>
@@ -8168,13 +8166,13 @@
       <c r="B17" s="68"/>
       <c r="C17" s="68">
         <f>SUBTOTAL(109,SprintBacklog[Estimated Hours])</f>
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="D17" s="68"/>
       <c r="E17" s="68"/>
       <c r="F17" s="68">
         <f>SUBTOTAL(109,SprintBacklog[Remaining Hours])</f>
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G17" s="68"/>
     </row>
@@ -8195,8 +8193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G15"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8243,7 +8241,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>92</v>
@@ -8267,7 +8265,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="11">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>93</v>
@@ -8291,7 +8289,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="11">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>94</v>
@@ -8315,7 +8313,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>95</v>
@@ -8339,7 +8337,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="11">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>96</v>
@@ -8363,7 +8361,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>97</v>
@@ -8387,7 +8385,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>175</v>
@@ -8411,7 +8409,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="11">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>176</v>
@@ -8459,7 +8457,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="11">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>173</v>
@@ -8483,7 +8481,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="66">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D13" s="64" t="s">
         <v>177</v>
@@ -8529,7 +8527,7 @@
       <c r="B15" s="68"/>
       <c r="C15" s="68">
         <f>SUBTOTAL(109,SprintBacklog6[Estimated Hours])</f>
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="D15" s="68"/>
       <c r="E15" s="68"/>
@@ -8556,8 +8554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.85546875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8588,15 +8586,15 @@
       </c>
       <c r="B3" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="C3" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="D3" s="15">
         <f>Table3[[#This Row],[Target Burn Down]]</f>
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="E3" s="15"/>
     </row>
@@ -8606,11 +8604,11 @@
       </c>
       <c r="B4" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>54.15</v>
+        <v>79.8</v>
       </c>
       <c r="C4" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>50.043478260869563</v>
+        <v>79.826086956521735</v>
       </c>
       <c r="D4" s="16">
         <v>57</v>
@@ -8623,11 +8621,11 @@
       </c>
       <c r="B5" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>51.3</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="C5" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>43.086956521739133</v>
+        <v>75.652173913043484</v>
       </c>
       <c r="D5" s="16">
         <v>57</v>
@@ -8640,11 +8638,11 @@
       </c>
       <c r="B6" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>48.45</v>
+        <v>71.400000000000006</v>
       </c>
       <c r="C6" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>36.130434782608695</v>
+        <v>71.478260869565219</v>
       </c>
       <c r="D6" s="16">
         <v>57</v>
@@ -8657,11 +8655,11 @@
       </c>
       <c r="B7" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>45.6</v>
+        <v>67.2</v>
       </c>
       <c r="C7" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>29.173913043478262</v>
+        <v>67.304347826086953</v>
       </c>
       <c r="D7" s="16">
         <v>57</v>
@@ -8674,11 +8672,11 @@
       </c>
       <c r="B8" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>42.75</v>
+        <v>63</v>
       </c>
       <c r="C8" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>22.217391304347828</v>
+        <v>63.130434782608695</v>
       </c>
       <c r="D8" s="16">
         <v>57</v>
@@ -8691,11 +8689,11 @@
       </c>
       <c r="B9" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>39.9</v>
+        <v>58.8</v>
       </c>
       <c r="C9" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>15.260869565217391</v>
+        <v>58.956521739130437</v>
       </c>
       <c r="D9" s="16">
         <v>57</v>
@@ -8708,11 +8706,11 @@
       </c>
       <c r="B10" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>37.049999999999997</v>
+        <v>54.599999999999994</v>
       </c>
       <c r="C10" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>8.3043478260869605</v>
+        <v>54.782608695652172</v>
       </c>
       <c r="D10" s="16">
         <v>57</v>
@@ -8725,11 +8723,11 @@
       </c>
       <c r="B11" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>34.200000000000003</v>
+        <v>50.4</v>
       </c>
       <c r="C11" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>1.3478260869565233</v>
+        <v>50.608695652173914</v>
       </c>
       <c r="D11" s="16">
         <v>57</v>
@@ -8742,11 +8740,11 @@
       </c>
       <c r="B12" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>31.349999999999998</v>
+        <v>46.199999999999996</v>
       </c>
       <c r="C12" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-5.608695652173914</v>
+        <v>46.434782608695656</v>
       </c>
       <c r="D12" s="16">
         <v>57</v>
@@ -8759,11 +8757,11 @@
       </c>
       <c r="B13" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>28.5</v>
+        <v>42</v>
       </c>
       <c r="C13" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-12.565217391304344</v>
+        <v>42.260869565217391</v>
       </c>
       <c r="D13" s="16">
         <v>57</v>
@@ -8776,11 +8774,11 @@
       </c>
       <c r="B14" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>25.65</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="C14" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-19.521739130434781</v>
+        <v>38.086956521739133</v>
       </c>
       <c r="D14" s="16">
         <v>57</v>
@@ -8792,11 +8790,11 @@
       </c>
       <c r="B15" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>22.799999999999997</v>
+        <v>33.599999999999994</v>
       </c>
       <c r="C15" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-26.478260869565219</v>
+        <v>33.913043478260875</v>
       </c>
       <c r="D15" s="16">
         <v>57</v>
@@ -8808,11 +8806,11 @@
       </c>
       <c r="B16" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>19.949999999999996</v>
+        <v>29.4</v>
       </c>
       <c r="C16" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-33.434782608695656</v>
+        <v>29.739130434782609</v>
       </c>
       <c r="D16" s="16">
         <v>57</v>
@@ -8824,11 +8822,11 @@
       </c>
       <c r="B17" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>17.100000000000001</v>
+        <v>25.199999999999996</v>
       </c>
       <c r="C17" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-40.391304347826079</v>
+        <v>25.565217391304351</v>
       </c>
       <c r="D17" s="16">
         <v>57</v>
@@ -8840,11 +8838,11 @@
       </c>
       <c r="B18" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>14.25</v>
+        <v>21</v>
       </c>
       <c r="C18" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-47.347826086956516</v>
+        <v>21.391304347826086</v>
       </c>
       <c r="D18" s="16">
         <v>57</v>
@@ -8856,11 +8854,11 @@
       </c>
       <c r="B19" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>11.399999999999999</v>
+        <v>16.799999999999997</v>
       </c>
       <c r="C19" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-54.304347826086953</v>
+        <v>17.217391304347828</v>
       </c>
       <c r="D19" s="16">
         <v>57</v>
@@ -8872,11 +8870,11 @@
       </c>
       <c r="B20" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>8.5499999999999972</v>
+        <v>12.599999999999994</v>
       </c>
       <c r="C20" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-61.260869565217391</v>
+        <v>13.043478260869563</v>
       </c>
       <c r="D20" s="16">
         <v>57</v>
@@ -8888,11 +8886,11 @@
       </c>
       <c r="B21" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>5.6999999999999957</v>
+        <v>8.3999999999999915</v>
       </c>
       <c r="C21" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-68.217391304347828</v>
+        <v>8.8695652173913118</v>
       </c>
       <c r="D21" s="16">
         <v>57</v>
@@ -8904,11 +8902,11 @@
       </c>
       <c r="B22" s="15">
         <f>IFERROR(TotalHours-(Table3[[#This Row],[Work Day]]*(TotalHours/WorkingDays)),0)</f>
-        <v>2.8500000000000014</v>
+        <v>4.2000000000000028</v>
       </c>
       <c r="C22" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-75.173913043478251</v>
+        <v>4.6956521739130466</v>
       </c>
       <c r="D22" s="16">
         <v>57</v>
@@ -8924,7 +8922,7 @@
       </c>
       <c r="C23" s="15">
         <f>TotalHours-(Table3[[#This Row],[Work Day]]*DevRate)</f>
-        <v>-82.130434782608688</v>
+        <v>0.52173913043478137</v>
       </c>
       <c r="D23" s="16">
         <v>57</v>
@@ -9001,15 +8999,15 @@
       </c>
       <c r="B3" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="C3" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="D3" s="15">
         <f>Table38[[#This Row],[Target Burn Down]]</f>
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="E3" s="15"/>
       <c r="F3" s="3"/>
@@ -9030,11 +9028,11 @@
       </c>
       <c r="B4" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>56.31818181818182</v>
+        <v>91.63636363636364</v>
       </c>
       <c r="C4" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>55.8</v>
+        <v>91.84</v>
       </c>
       <c r="D4" s="16">
         <v>59</v>
@@ -9058,11 +9056,11 @@
       </c>
       <c r="B5" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>53.63636363636364</v>
+        <v>87.27272727272728</v>
       </c>
       <c r="C5" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>52.6</v>
+        <v>87.68</v>
       </c>
       <c r="D5" s="16">
         <v>59</v>
@@ -9086,11 +9084,11 @@
       </c>
       <c r="B6" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>50.954545454545453</v>
+        <v>82.909090909090907</v>
       </c>
       <c r="C6" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>49.4</v>
+        <v>83.52</v>
       </c>
       <c r="D6" s="16">
         <v>59</v>
@@ -9114,11 +9112,11 @@
       </c>
       <c r="B7" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>48.272727272727273</v>
+        <v>78.545454545454547</v>
       </c>
       <c r="C7" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>46.2</v>
+        <v>79.36</v>
       </c>
       <c r="D7" s="16">
         <v>59</v>
@@ -9142,11 +9140,11 @@
       </c>
       <c r="B8" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>45.590909090909093</v>
+        <v>74.181818181818187</v>
       </c>
       <c r="C8" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>43</v>
+        <v>75.2</v>
       </c>
       <c r="D8" s="16">
         <v>59</v>
@@ -9170,11 +9168,11 @@
       </c>
       <c r="B9" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>42.909090909090907</v>
+        <v>69.818181818181813</v>
       </c>
       <c r="C9" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>39.799999999999997</v>
+        <v>71.039999999999992</v>
       </c>
       <c r="D9" s="16">
         <v>59</v>
@@ -9198,11 +9196,11 @@
       </c>
       <c r="B10" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>40.227272727272727</v>
+        <v>65.454545454545453</v>
       </c>
       <c r="C10" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>36.599999999999994</v>
+        <v>66.88</v>
       </c>
       <c r="D10" s="16">
         <v>59</v>
@@ -9226,11 +9224,11 @@
       </c>
       <c r="B11" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>37.545454545454547</v>
+        <v>61.090909090909093</v>
       </c>
       <c r="C11" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>33.4</v>
+        <v>62.72</v>
       </c>
       <c r="D11" s="16">
         <v>59</v>
@@ -9254,11 +9252,11 @@
       </c>
       <c r="B12" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>34.863636363636367</v>
+        <v>56.727272727272734</v>
       </c>
       <c r="C12" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>30.2</v>
+        <v>58.56</v>
       </c>
       <c r="D12" s="16">
         <v>59</v>
@@ -9282,11 +9280,11 @@
       </c>
       <c r="B13" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>32.181818181818187</v>
+        <v>52.363636363636367</v>
       </c>
       <c r="C13" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>27</v>
+        <v>54.4</v>
       </c>
       <c r="D13" s="16">
         <v>59</v>
@@ -9310,11 +9308,11 @@
       </c>
       <c r="B14" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>29.5</v>
+        <v>48</v>
       </c>
       <c r="C14" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>23.799999999999997</v>
+        <v>50.239999999999995</v>
       </c>
       <c r="D14" s="16">
         <v>59</v>
@@ -9338,11 +9336,11 @@
       </c>
       <c r="B15" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>26.81818181818182</v>
+        <v>43.63636363636364</v>
       </c>
       <c r="C15" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>20.599999999999994</v>
+        <v>46.08</v>
       </c>
       <c r="D15" s="16">
         <v>59</v>
@@ -9366,11 +9364,11 @@
       </c>
       <c r="B16" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>24.13636363636364</v>
+        <v>39.27272727272728</v>
       </c>
       <c r="C16" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>17.399999999999999</v>
+        <v>41.92</v>
       </c>
       <c r="D16" s="16">
         <v>59</v>
@@ -9382,11 +9380,11 @@
       </c>
       <c r="B17" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>21.454545454545453</v>
+        <v>34.909090909090914</v>
       </c>
       <c r="C17" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>14.199999999999996</v>
+        <v>37.76</v>
       </c>
       <c r="D17" s="16">
         <v>59</v>
@@ -9398,11 +9396,11 @@
       </c>
       <c r="B18" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>18.772727272727273</v>
+        <v>30.545454545454547</v>
       </c>
       <c r="C18" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>11</v>
+        <v>33.599999999999994</v>
       </c>
       <c r="D18" s="16">
         <v>59</v>
@@ -9414,11 +9412,11 @@
       </c>
       <c r="B19" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>16.090909090909093</v>
+        <v>26.181818181818187</v>
       </c>
       <c r="C19" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>7.7999999999999972</v>
+        <v>29.439999999999998</v>
       </c>
       <c r="D19" s="16">
         <v>59</v>
@@ -9430,11 +9428,11 @@
       </c>
       <c r="B20" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>13.409090909090914</v>
+        <v>21.818181818181827</v>
       </c>
       <c r="C20" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>4.5999999999999943</v>
+        <v>25.28</v>
       </c>
       <c r="D20" s="16">
         <v>59</v>
@@ -9446,11 +9444,11 @@
       </c>
       <c r="B21" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>10.727272727272734</v>
+        <v>17.454545454545467</v>
       </c>
       <c r="C21" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>1.3999999999999986</v>
+        <v>21.120000000000005</v>
       </c>
       <c r="D21" s="16">
         <v>59</v>
@@ -9462,11 +9460,11 @@
       </c>
       <c r="B22" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>8.0454545454545467</v>
+        <v>13.090909090909093</v>
       </c>
       <c r="C22" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>-1.8000000000000043</v>
+        <v>16.959999999999994</v>
       </c>
       <c r="D22" s="16">
         <v>59</v>
@@ -9478,11 +9476,11 @@
       </c>
       <c r="B23" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>5.3636363636363669</v>
+        <v>8.7272727272727337</v>
       </c>
       <c r="C23" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>-5</v>
+        <v>12.799999999999997</v>
       </c>
       <c r="D23" s="16">
         <v>59</v>
@@ -9494,11 +9492,11 @@
       </c>
       <c r="B24" s="15">
         <f>IFERROR(SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*(SprintBacklog6[[#Totals],[Estimated Hours]]/Sprint2Info!WorkingDays)),0)</f>
-        <v>2.681818181818187</v>
+        <v>4.363636363636374</v>
       </c>
       <c r="C24" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>-8.2000000000000028</v>
+        <v>8.64</v>
       </c>
       <c r="D24" s="16">
         <v>59</v>
@@ -9514,7 +9512,7 @@
       </c>
       <c r="C25" s="15">
         <f>SprintBacklog6[[#Totals],[Estimated Hours]]-(Table38[[#This Row],[Work Day]]*Sprint2Info!DevRate)</f>
-        <v>-11.400000000000006</v>
+        <v>4.4799999999999898</v>
       </c>
       <c r="D25" s="16">
         <v>59</v>

</xml_diff>